<commit_message>
Actualización de quincenal resumen
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ResumenBalanceEnergLIV.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ResumenBalanceEnergLIV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\quincenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62A4275F-23CA-49A6-8A13-0D004FC3E798}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ADFBC3-1FEB-4795-BF66-43DC224C210B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="642" uniqueCount="467">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="471">
   <si>
     <t>LOTE IV</t>
   </si>
@@ -1483,15 +1483,28 @@
   </si>
   <si>
     <t>{{dataResultResumen.FactorConversionSCFDGalQ2}}</t>
+  </si>
+  <si>
+    <t>{{dataResultResumen.EnergiaMMBTUQ1GLP}}</t>
+  </si>
+  <si>
+    <t>{{dataResultResumen.EnergiaMMBTUQ1CGN}}</t>
+  </si>
+  <si>
+    <t>{{dataResultResumen.EnergiaMMBTUQ2GLP}}</t>
+  </si>
+  <si>
+    <t>{{dataResultResumen.EnergiaMMBTUQ2CGN}}</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="[$-280A]dddd\ d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
+    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
   </numFmts>
   <fonts count="18" x14ac:knownFonts="1">
     <font>
@@ -2013,7 +2026,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="96">
+  <cellXfs count="97">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2031,7 +2044,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2076,40 +2088,105 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="20" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="20" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2122,9 +2199,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2139,96 +2213,6 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2265,13 +2249,43 @@
     <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="164" fontId="9" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="2" fontId="9" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="167" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="3" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="1" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="13" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="167" fontId="9" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="167" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2569,7 +2583,7 @@
   <dimension ref="B1:AB42"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D38" sqref="D38"/>
+      <selection activeCell="B2" sqref="B2:E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2582,1696 +2596,1743 @@
   <sheetData>
     <row r="1" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="50" t="s">
+      <c r="B2" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="50"/>
-      <c r="D2" s="50"/>
-      <c r="E2" s="50"/>
+      <c r="C2" s="37"/>
+      <c r="D2" s="37"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="26" t="s">
+      <c r="G2" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="27" t="s">
+      <c r="H2" s="26" t="s">
         <v>54</v>
       </c>
     </row>
     <row r="4" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="36" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
-      <c r="M4" s="55"/>
-      <c r="N4" s="55"/>
-      <c r="O4" s="55"/>
-      <c r="P4" s="55"/>
-      <c r="Q4" s="55"/>
-      <c r="R4" s="55"/>
-      <c r="S4" s="55"/>
-      <c r="T4" s="55"/>
-      <c r="U4" s="55"/>
-      <c r="V4" s="55"/>
-      <c r="W4" s="55"/>
-      <c r="X4" s="55"/>
-      <c r="Y4" s="55"/>
-      <c r="Z4" s="55"/>
-      <c r="AA4" s="55"/>
-      <c r="AB4" s="55"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
+      <c r="M4" s="36"/>
+      <c r="N4" s="36"/>
+      <c r="O4" s="36"/>
+      <c r="P4" s="36"/>
+      <c r="Q4" s="36"/>
+      <c r="R4" s="36"/>
+      <c r="S4" s="36"/>
+      <c r="T4" s="36"/>
+      <c r="U4" s="36"/>
+      <c r="V4" s="36"/>
+      <c r="W4" s="36"/>
+      <c r="X4" s="36"/>
+      <c r="Y4" s="36"/>
+      <c r="Z4" s="36"/>
+      <c r="AA4" s="36"/>
+      <c r="AB4" s="36"/>
     </row>
     <row r="6" spans="2:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="57"/>
-      <c r="D6" s="58"/>
-      <c r="E6" s="51" t="s">
+      <c r="C6" s="43"/>
+      <c r="D6" s="44"/>
+      <c r="E6" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="51"/>
-      <c r="G6" s="51"/>
-      <c r="H6" s="62" t="s">
+      <c r="F6" s="38"/>
+      <c r="G6" s="38"/>
+      <c r="H6" s="48" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="62"/>
-      <c r="J6" s="62"/>
-      <c r="K6" s="70" t="s">
+      <c r="I6" s="48"/>
+      <c r="J6" s="48"/>
+      <c r="K6" s="56" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="71"/>
-      <c r="M6" s="71"/>
-      <c r="N6" s="72" t="s">
+      <c r="L6" s="57"/>
+      <c r="M6" s="57"/>
+      <c r="N6" s="58" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="73"/>
-      <c r="P6" s="73"/>
-      <c r="Q6" s="66" t="s">
+      <c r="O6" s="59"/>
+      <c r="P6" s="59"/>
+      <c r="Q6" s="52" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="67"/>
-      <c r="S6" s="67"/>
-      <c r="T6" s="68" t="s">
+      <c r="R6" s="53"/>
+      <c r="S6" s="53"/>
+      <c r="T6" s="54" t="s">
         <v>12</v>
       </c>
-      <c r="U6" s="69"/>
-      <c r="V6" s="69"/>
-      <c r="W6" s="63" t="s">
+      <c r="U6" s="55"/>
+      <c r="V6" s="55"/>
+      <c r="W6" s="49" t="s">
         <v>13</v>
       </c>
-      <c r="X6" s="64"/>
-      <c r="Y6" s="65"/>
-      <c r="Z6" s="52" t="s">
+      <c r="X6" s="50"/>
+      <c r="Y6" s="51"/>
+      <c r="Z6" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="AA6" s="53"/>
-      <c r="AB6" s="54"/>
+      <c r="AA6" s="40"/>
+      <c r="AB6" s="41"/>
     </row>
     <row r="7" spans="2:28" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="59"/>
-      <c r="C7" s="60"/>
-      <c r="D7" s="61"/>
-      <c r="E7" s="23" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="46"/>
+      <c r="D7" s="47"/>
+      <c r="E7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="23" t="s">
+      <c r="J7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="24" t="s">
+      <c r="M7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="24" t="s">
+      <c r="N7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="24" t="s">
+      <c r="O7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="24" t="s">
+      <c r="P7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="24" t="s">
+      <c r="Q7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="R7" s="24" t="s">
+      <c r="R7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="24" t="s">
+      <c r="S7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="T7" s="24" t="s">
+      <c r="T7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="U7" s="24" t="s">
+      <c r="U7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="24" t="s">
+      <c r="V7" s="23" t="s">
         <v>7</v>
       </c>
-      <c r="W7" s="24" t="s">
+      <c r="W7" s="23" t="s">
         <v>5</v>
       </c>
-      <c r="X7" s="24" t="s">
+      <c r="X7" s="23" t="s">
         <v>6</v>
       </c>
-      <c r="Y7" s="23" t="s">
+      <c r="Y7" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Z7" s="23" t="s">
+      <c r="Z7" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AA7" s="23" t="s">
+      <c r="AA7" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB7" s="23" t="s">
+      <c r="AB7" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="75" t="s">
+      <c r="B8" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="76"/>
-      <c r="D8" s="77"/>
-      <c r="E8" s="31" t="s">
+      <c r="C8" s="32"/>
+      <c r="D8" s="33"/>
+      <c r="E8" s="82" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="29" t="s">
+      <c r="F8" s="83" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="29" t="s">
+      <c r="G8" s="83" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="29" t="s">
+      <c r="H8" s="83" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="29" t="s">
+      <c r="I8" s="83" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="29" t="s">
+      <c r="J8" s="83" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="29" t="s">
+      <c r="K8" s="83" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="29" t="s">
+      <c r="L8" s="83" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="29" t="s">
+      <c r="M8" s="83" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="29" t="s">
+      <c r="N8" s="83" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="29" t="s">
+      <c r="O8" s="83" t="s">
         <v>40</v>
       </c>
-      <c r="P8" s="29" t="s">
+      <c r="P8" s="83" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="29" t="s">
+      <c r="Q8" s="83" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="29" t="s">
+      <c r="R8" s="83" t="s">
         <v>43</v>
       </c>
-      <c r="S8" s="29" t="s">
+      <c r="S8" s="83" t="s">
         <v>44</v>
       </c>
-      <c r="T8" s="29" t="s">
+      <c r="T8" s="83" t="s">
         <v>45</v>
       </c>
-      <c r="U8" s="29" t="s">
+      <c r="U8" s="83" t="s">
         <v>46</v>
       </c>
-      <c r="V8" s="29" t="s">
+      <c r="V8" s="83" t="s">
         <v>57</v>
       </c>
-      <c r="W8" s="29" t="s">
+      <c r="W8" s="83" t="s">
         <v>47</v>
       </c>
-      <c r="X8" s="29" t="s">
+      <c r="X8" s="83" t="s">
         <v>48</v>
       </c>
-      <c r="Y8" s="29" t="s">
+      <c r="Y8" s="83" t="s">
         <v>49</v>
       </c>
-      <c r="Z8" s="29" t="s">
+      <c r="Z8" s="83" t="s">
         <v>50</v>
       </c>
-      <c r="AA8" s="29" t="s">
+      <c r="AA8" s="83" t="s">
         <v>51</v>
       </c>
-      <c r="AB8" s="29" t="s">
+      <c r="AB8" s="83" t="s">
         <v>52</v>
       </c>
     </row>
     <row r="9" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B9" s="75"/>
-      <c r="C9" s="76"/>
-      <c r="D9" s="77"/>
-      <c r="E9" s="28"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
-      <c r="M9" s="1"/>
-      <c r="N9" s="1"/>
-      <c r="O9" s="1"/>
-      <c r="P9" s="1"/>
-      <c r="Q9" s="1"/>
-      <c r="R9" s="1"/>
-      <c r="S9" s="1"/>
-      <c r="T9" s="1"/>
-      <c r="U9" s="1"/>
-      <c r="V9" s="1"/>
-      <c r="W9" s="1"/>
-      <c r="X9" s="1"/>
-      <c r="Y9" s="1"/>
-      <c r="Z9" s="1"/>
-      <c r="AA9" s="1"/>
-      <c r="AB9" s="1"/>
+      <c r="B9" s="31"/>
+      <c r="C9" s="32"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
+      <c r="M9" s="85"/>
+      <c r="N9" s="85"/>
+      <c r="O9" s="85"/>
+      <c r="P9" s="85"/>
+      <c r="Q9" s="85"/>
+      <c r="R9" s="85"/>
+      <c r="S9" s="85"/>
+      <c r="T9" s="85"/>
+      <c r="U9" s="85"/>
+      <c r="V9" s="85"/>
+      <c r="W9" s="85"/>
+      <c r="X9" s="85"/>
+      <c r="Y9" s="85"/>
+      <c r="Z9" s="85"/>
+      <c r="AA9" s="85"/>
+      <c r="AB9" s="85"/>
     </row>
     <row r="12" spans="2:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="78" t="s">
+      <c r="B12" s="34" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="78"/>
-      <c r="D12" s="78"/>
-      <c r="E12" s="23" t="s">
+      <c r="C12" s="34"/>
+      <c r="D12" s="34"/>
+      <c r="E12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="23" t="s">
+      <c r="F12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="23" t="s">
+      <c r="G12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="23" t="s">
+      <c r="H12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="23" t="s">
+      <c r="I12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="23" t="s">
+      <c r="J12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="23" t="s">
+      <c r="K12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="23" t="s">
+      <c r="L12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="M12" s="23" t="s">
+      <c r="M12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="23" t="s">
+      <c r="N12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="O12" s="23" t="s">
+      <c r="O12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="P12" s="23" t="s">
+      <c r="P12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="23" t="s">
+      <c r="Q12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="R12" s="23" t="s">
+      <c r="R12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="S12" s="23" t="s">
+      <c r="S12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T12" s="23" t="s">
+      <c r="T12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="U12" s="23" t="s">
+      <c r="U12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="V12" s="23" t="s">
+      <c r="V12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="W12" s="23" t="s">
+      <c r="W12" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="X12" s="23" t="s">
+      <c r="X12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="Y12" s="23" t="s">
+      <c r="Y12" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Z12" s="25" t="s">
+      <c r="Z12" s="24" t="s">
         <v>5</v>
       </c>
-      <c r="AA12" s="23" t="s">
+      <c r="AA12" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB12" s="23" t="s">
+      <c r="AB12" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="79" t="s">
+      <c r="B13" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="79"/>
-      <c r="D13" s="79"/>
-      <c r="E13" s="29" t="s">
+      <c r="C13" s="35"/>
+      <c r="D13" s="35"/>
+      <c r="E13" s="83" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="29" t="s">
+      <c r="F13" s="83" t="s">
         <v>108</v>
       </c>
-      <c r="G13" s="38" t="s">
+      <c r="G13" s="86" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="29" t="s">
+      <c r="H13" s="83" t="s">
         <v>110</v>
       </c>
-      <c r="I13" s="29" t="s">
+      <c r="I13" s="83" t="s">
         <v>111</v>
       </c>
-      <c r="J13" s="38" t="s">
+      <c r="J13" s="86" t="s">
         <v>112</v>
       </c>
-      <c r="K13" s="29" t="s">
+      <c r="K13" s="83" t="s">
         <v>113</v>
       </c>
-      <c r="L13" s="29" t="s">
+      <c r="L13" s="83" t="s">
         <v>114</v>
       </c>
-      <c r="M13" s="38" t="s">
+      <c r="M13" s="86" t="s">
         <v>115</v>
       </c>
-      <c r="N13" s="29" t="s">
+      <c r="N13" s="83" t="s">
         <v>116</v>
       </c>
-      <c r="O13" s="29" t="s">
+      <c r="O13" s="83" t="s">
         <v>117</v>
       </c>
-      <c r="P13" s="38" t="s">
+      <c r="P13" s="86" t="s">
         <v>118</v>
       </c>
-      <c r="Q13" s="29" t="s">
+      <c r="Q13" s="83" t="s">
         <v>119</v>
       </c>
-      <c r="R13" s="29" t="s">
+      <c r="R13" s="83" t="s">
         <v>120</v>
       </c>
-      <c r="S13" s="38" t="s">
+      <c r="S13" s="86" t="s">
         <v>121</v>
       </c>
-      <c r="T13" s="29" t="s">
+      <c r="T13" s="83" t="s">
         <v>122</v>
       </c>
-      <c r="U13" s="29" t="s">
+      <c r="U13" s="83" t="s">
         <v>123</v>
       </c>
-      <c r="V13" s="38" t="s">
+      <c r="V13" s="86" t="s">
         <v>124</v>
       </c>
-      <c r="W13" s="29" t="s">
+      <c r="W13" s="83" t="s">
         <v>125</v>
       </c>
-      <c r="X13" s="29" t="s">
+      <c r="X13" s="83" t="s">
         <v>126</v>
       </c>
-      <c r="Y13" s="38" t="s">
+      <c r="Y13" s="86" t="s">
         <v>127</v>
       </c>
-      <c r="Z13" s="29" t="s">
+      <c r="Z13" s="83" t="s">
         <v>128</v>
       </c>
-      <c r="AA13" s="29" t="s">
+      <c r="AA13" s="83" t="s">
         <v>129</v>
       </c>
-      <c r="AB13" s="38" t="s">
+      <c r="AB13" s="86" t="s">
         <v>130</v>
       </c>
     </row>
     <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="79" t="s">
+      <c r="B14" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="79"/>
-      <c r="D14" s="79"/>
-      <c r="E14" s="29" t="s">
+      <c r="C14" s="35"/>
+      <c r="D14" s="35"/>
+      <c r="E14" s="83" t="s">
         <v>131</v>
       </c>
-      <c r="F14" s="29" t="s">
+      <c r="F14" s="83" t="s">
         <v>132</v>
       </c>
-      <c r="G14" s="38" t="s">
+      <c r="G14" s="86" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="29" t="s">
+      <c r="H14" s="83" t="s">
         <v>134</v>
       </c>
-      <c r="I14" s="29" t="s">
+      <c r="I14" s="83" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="38" t="s">
+      <c r="J14" s="86" t="s">
         <v>136</v>
       </c>
-      <c r="K14" s="29" t="s">
+      <c r="K14" s="83" t="s">
         <v>137</v>
       </c>
-      <c r="L14" s="29" t="s">
+      <c r="L14" s="83" t="s">
         <v>138</v>
       </c>
-      <c r="M14" s="38" t="s">
+      <c r="M14" s="86" t="s">
         <v>139</v>
       </c>
-      <c r="N14" s="29" t="s">
+      <c r="N14" s="83" t="s">
         <v>140</v>
       </c>
-      <c r="O14" s="29" t="s">
+      <c r="O14" s="83" t="s">
         <v>141</v>
       </c>
-      <c r="P14" s="38" t="s">
+      <c r="P14" s="86" t="s">
         <v>142</v>
       </c>
-      <c r="Q14" s="29" t="s">
+      <c r="Q14" s="83" t="s">
         <v>143</v>
       </c>
-      <c r="R14" s="29" t="s">
+      <c r="R14" s="83" t="s">
         <v>144</v>
       </c>
-      <c r="S14" s="38" t="s">
+      <c r="S14" s="86" t="s">
         <v>145</v>
       </c>
-      <c r="T14" s="29" t="s">
+      <c r="T14" s="83" t="s">
         <v>146</v>
       </c>
-      <c r="U14" s="29" t="s">
+      <c r="U14" s="83" t="s">
         <v>147</v>
       </c>
-      <c r="V14" s="38" t="s">
+      <c r="V14" s="86" t="s">
         <v>148</v>
       </c>
-      <c r="W14" s="29" t="s">
+      <c r="W14" s="83" t="s">
         <v>149</v>
       </c>
-      <c r="X14" s="29" t="s">
+      <c r="X14" s="83" t="s">
         <v>150</v>
       </c>
-      <c r="Y14" s="38" t="s">
+      <c r="Y14" s="86" t="s">
         <v>151</v>
       </c>
-      <c r="Z14" s="29" t="s">
+      <c r="Z14" s="83" t="s">
         <v>152</v>
       </c>
-      <c r="AA14" s="29" t="s">
+      <c r="AA14" s="83" t="s">
         <v>153</v>
       </c>
-      <c r="AB14" s="38" t="s">
+      <c r="AB14" s="86" t="s">
         <v>154</v>
       </c>
     </row>
+    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="E15" s="87"/>
+      <c r="F15" s="87"/>
+      <c r="G15" s="87"/>
+      <c r="H15" s="87"/>
+      <c r="I15" s="87"/>
+      <c r="J15" s="87"/>
+      <c r="K15" s="87"/>
+      <c r="L15" s="87"/>
+      <c r="M15" s="87"/>
+      <c r="N15" s="87"/>
+      <c r="O15" s="87"/>
+      <c r="P15" s="87"/>
+      <c r="Q15" s="87"/>
+      <c r="R15" s="87"/>
+      <c r="S15" s="87"/>
+      <c r="T15" s="87"/>
+      <c r="U15" s="87"/>
+      <c r="V15" s="87"/>
+      <c r="W15" s="87"/>
+      <c r="X15" s="87"/>
+      <c r="Y15" s="87"/>
+      <c r="Z15" s="87"/>
+      <c r="AA15" s="87"/>
+      <c r="AB15" s="87"/>
+    </row>
     <row r="16" spans="2:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="78" t="s">
+      <c r="B16" s="34" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="78"/>
-      <c r="D16" s="78"/>
-      <c r="E16" s="23" t="s">
+      <c r="C16" s="34"/>
+      <c r="D16" s="34"/>
+      <c r="E16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="23" t="s">
+      <c r="F16" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="23" t="s">
+      <c r="G16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="23" t="s">
+      <c r="H16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="23" t="s">
+      <c r="I16" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="23" t="s">
+      <c r="J16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="23" t="s">
+      <c r="K16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="L16" s="23" t="s">
+      <c r="L16" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="23" t="s">
+      <c r="M16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="23" t="s">
+      <c r="N16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="23" t="s">
+      <c r="O16" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="23" t="s">
+      <c r="P16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Q16" s="23" t="s">
+      <c r="Q16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="R16" s="23" t="s">
+      <c r="R16" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="S16" s="23" t="s">
+      <c r="S16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="T16" s="23" t="s">
+      <c r="T16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="U16" s="23" t="s">
+      <c r="U16" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="V16" s="23" t="s">
+      <c r="V16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="W16" s="23" t="s">
+      <c r="W16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="X16" s="23" t="s">
+      <c r="X16" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="Y16" s="23" t="s">
+      <c r="Y16" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="Z16" s="23" t="s">
+      <c r="Z16" s="22" t="s">
         <v>5</v>
       </c>
-      <c r="AA16" s="23" t="s">
+      <c r="AA16" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="AB16" s="23" t="s">
+      <c r="AB16" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B17" s="79" t="s">
+      <c r="B17" s="35" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="79"/>
-      <c r="D17" s="79"/>
-      <c r="E17" s="1" t="s">
+      <c r="C17" s="35"/>
+      <c r="D17" s="35"/>
+      <c r="E17" s="85" t="s">
         <v>156</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="85" t="s">
         <v>157</v>
       </c>
-      <c r="G17" s="39" t="s">
+      <c r="G17" s="88" t="s">
         <v>158</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="85" t="s">
         <v>159</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="85" t="s">
         <v>160</v>
       </c>
-      <c r="J17" s="39" t="s">
+      <c r="J17" s="88" t="s">
         <v>161</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="85" t="s">
         <v>162</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="85" t="s">
         <v>163</v>
       </c>
-      <c r="M17" s="39" t="s">
+      <c r="M17" s="88" t="s">
         <v>164</v>
       </c>
-      <c r="N17" s="1" t="s">
+      <c r="N17" s="85" t="s">
         <v>165</v>
       </c>
-      <c r="O17" s="1" t="s">
+      <c r="O17" s="85" t="s">
         <v>166</v>
       </c>
-      <c r="P17" s="39" t="s">
+      <c r="P17" s="88" t="s">
         <v>167</v>
       </c>
-      <c r="Q17" s="1" t="s">
+      <c r="Q17" s="85" t="s">
         <v>168</v>
       </c>
-      <c r="R17" s="1" t="s">
+      <c r="R17" s="85" t="s">
         <v>169</v>
       </c>
-      <c r="S17" s="39" t="s">
+      <c r="S17" s="88" t="s">
         <v>170</v>
       </c>
-      <c r="T17" s="1" t="s">
+      <c r="T17" s="85" t="s">
         <v>171</v>
       </c>
-      <c r="U17" s="1" t="s">
+      <c r="U17" s="85" t="s">
         <v>172</v>
       </c>
-      <c r="V17" s="39" t="s">
+      <c r="V17" s="88" t="s">
         <v>173</v>
       </c>
-      <c r="W17" s="1" t="s">
+      <c r="W17" s="85" t="s">
         <v>174</v>
       </c>
-      <c r="X17" s="1" t="s">
+      <c r="X17" s="85" t="s">
         <v>175</v>
       </c>
-      <c r="Y17" s="39" t="s">
+      <c r="Y17" s="88" t="s">
         <v>176</v>
       </c>
-      <c r="Z17" s="1" t="s">
+      <c r="Z17" s="85" t="s">
         <v>177</v>
       </c>
-      <c r="AA17" s="1" t="s">
+      <c r="AA17" s="85" t="s">
         <v>178</v>
       </c>
-      <c r="AB17" s="39" t="s">
+      <c r="AB17" s="88" t="s">
         <v>179</v>
       </c>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B18" s="79" t="s">
+      <c r="B18" s="35" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="79"/>
-      <c r="D18" s="79"/>
-      <c r="E18" s="1" t="s">
+      <c r="C18" s="35"/>
+      <c r="D18" s="35"/>
+      <c r="E18" s="85" t="s">
         <v>180</v>
       </c>
-      <c r="F18" s="1" t="s">
+      <c r="F18" s="85" t="s">
         <v>181</v>
       </c>
-      <c r="G18" s="39" t="s">
+      <c r="G18" s="88" t="s">
         <v>182</v>
       </c>
-      <c r="H18" s="1" t="s">
+      <c r="H18" s="85" t="s">
         <v>183</v>
       </c>
-      <c r="I18" s="1" t="s">
+      <c r="I18" s="85" t="s">
         <v>184</v>
       </c>
-      <c r="J18" s="39" t="s">
+      <c r="J18" s="88" t="s">
         <v>185</v>
       </c>
-      <c r="K18" s="1" t="s">
+      <c r="K18" s="85" t="s">
         <v>186</v>
       </c>
-      <c r="L18" s="1" t="s">
+      <c r="L18" s="85" t="s">
         <v>187</v>
       </c>
-      <c r="M18" s="39" t="s">
+      <c r="M18" s="88" t="s">
         <v>188</v>
       </c>
-      <c r="N18" s="1" t="s">
+      <c r="N18" s="85" t="s">
         <v>189</v>
       </c>
-      <c r="O18" s="1" t="s">
+      <c r="O18" s="85" t="s">
         <v>190</v>
       </c>
-      <c r="P18" s="39" t="s">
+      <c r="P18" s="88" t="s">
         <v>191</v>
       </c>
-      <c r="Q18" s="1" t="s">
+      <c r="Q18" s="85" t="s">
         <v>192</v>
       </c>
-      <c r="R18" s="1" t="s">
+      <c r="R18" s="85" t="s">
         <v>193</v>
       </c>
-      <c r="S18" s="39" t="s">
+      <c r="S18" s="88" t="s">
         <v>194</v>
       </c>
-      <c r="T18" s="1" t="s">
+      <c r="T18" s="85" t="s">
         <v>195</v>
       </c>
-      <c r="U18" s="1" t="s">
+      <c r="U18" s="85" t="s">
         <v>196</v>
       </c>
-      <c r="V18" s="39" t="s">
+      <c r="V18" s="88" t="s">
         <v>197</v>
       </c>
-      <c r="W18" s="1" t="s">
+      <c r="W18" s="85" t="s">
         <v>198</v>
       </c>
-      <c r="X18" s="1" t="s">
+      <c r="X18" s="85" t="s">
         <v>199</v>
       </c>
-      <c r="Y18" s="39" t="s">
+      <c r="Y18" s="88" t="s">
         <v>200</v>
       </c>
-      <c r="Z18" s="1" t="s">
+      <c r="Z18" s="85" t="s">
         <v>201</v>
       </c>
-      <c r="AA18" s="1" t="s">
+      <c r="AA18" s="85" t="s">
         <v>202</v>
       </c>
-      <c r="AB18" s="39" t="s">
+      <c r="AB18" s="88" t="s">
         <v>203</v>
       </c>
     </row>
     <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" s="79" t="s">
+      <c r="B20" s="35" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="79"/>
-      <c r="D20" s="79"/>
-      <c r="E20" s="1" t="s">
+      <c r="C20" s="35"/>
+      <c r="D20" s="35"/>
+      <c r="E20" s="85" t="s">
         <v>204</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="85" t="s">
         <v>205</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="85" t="s">
         <v>206</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="85" t="s">
         <v>207</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="85" t="s">
         <v>208</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="85" t="s">
         <v>209</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" s="85" t="s">
         <v>210</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" s="85" t="s">
         <v>211</v>
       </c>
-      <c r="M20" s="1" t="s">
+      <c r="M20" s="85" t="s">
         <v>212</v>
       </c>
-      <c r="N20" s="1" t="s">
+      <c r="N20" s="85" t="s">
         <v>213</v>
       </c>
-      <c r="O20" s="1" t="s">
+      <c r="O20" s="85" t="s">
         <v>214</v>
       </c>
-      <c r="P20" s="1" t="s">
+      <c r="P20" s="85" t="s">
         <v>215</v>
       </c>
-      <c r="Q20" s="1" t="s">
+      <c r="Q20" s="85" t="s">
         <v>216</v>
       </c>
-      <c r="R20" s="1" t="s">
+      <c r="R20" s="85" t="s">
         <v>217</v>
       </c>
-      <c r="S20" s="1" t="s">
+      <c r="S20" s="85" t="s">
         <v>218</v>
       </c>
-      <c r="T20" s="1" t="s">
+      <c r="T20" s="85" t="s">
         <v>219</v>
       </c>
-      <c r="U20" s="1" t="s">
+      <c r="U20" s="85" t="s">
         <v>220</v>
       </c>
-      <c r="V20" s="1" t="s">
+      <c r="V20" s="85" t="s">
         <v>221</v>
       </c>
-      <c r="W20" s="1" t="s">
+      <c r="W20" s="85" t="s">
         <v>222</v>
       </c>
-      <c r="X20" s="1" t="s">
+      <c r="X20" s="85" t="s">
         <v>223</v>
       </c>
-      <c r="Y20" s="1" t="s">
+      <c r="Y20" s="85" t="s">
         <v>224</v>
       </c>
-      <c r="Z20" s="1" t="s">
+      <c r="Z20" s="85" t="s">
         <v>225</v>
       </c>
-      <c r="AA20" s="1" t="s">
+      <c r="AA20" s="85" t="s">
         <v>226</v>
       </c>
-      <c r="AB20" s="1" t="s">
+      <c r="AB20" s="85" t="s">
         <v>227</v>
       </c>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B21" s="79" t="s">
+      <c r="B21" s="35" t="s">
         <v>228</v>
       </c>
-      <c r="C21" s="79"/>
-      <c r="D21" s="79"/>
-      <c r="E21" s="1" t="s">
+      <c r="C21" s="35"/>
+      <c r="D21" s="35"/>
+      <c r="E21" s="85" t="s">
         <v>229</v>
       </c>
-      <c r="F21" s="1" t="s">
+      <c r="F21" s="85" t="s">
         <v>230</v>
       </c>
-      <c r="G21" s="1" t="s">
+      <c r="G21" s="85" t="s">
         <v>231</v>
       </c>
-      <c r="H21" s="1" t="s">
+      <c r="H21" s="85" t="s">
         <v>232</v>
       </c>
-      <c r="I21" s="1" t="s">
+      <c r="I21" s="85" t="s">
         <v>233</v>
       </c>
-      <c r="J21" s="1" t="s">
+      <c r="J21" s="85" t="s">
         <v>234</v>
       </c>
-      <c r="K21" s="1" t="s">
+      <c r="K21" s="85" t="s">
         <v>235</v>
       </c>
-      <c r="L21" s="1" t="s">
+      <c r="L21" s="85" t="s">
         <v>236</v>
       </c>
-      <c r="M21" s="1" t="s">
+      <c r="M21" s="85" t="s">
         <v>237</v>
       </c>
-      <c r="N21" s="1" t="s">
+      <c r="N21" s="85" t="s">
         <v>238</v>
       </c>
-      <c r="O21" s="1" t="s">
+      <c r="O21" s="85" t="s">
         <v>239</v>
       </c>
-      <c r="P21" s="1" t="s">
+      <c r="P21" s="85" t="s">
         <v>240</v>
       </c>
-      <c r="Q21" s="1" t="s">
+      <c r="Q21" s="85" t="s">
         <v>241</v>
       </c>
-      <c r="R21" s="1" t="s">
+      <c r="R21" s="85" t="s">
         <v>242</v>
       </c>
-      <c r="S21" s="1" t="s">
+      <c r="S21" s="85" t="s">
         <v>243</v>
       </c>
-      <c r="T21" s="1" t="s">
+      <c r="T21" s="85" t="s">
         <v>244</v>
       </c>
-      <c r="U21" s="1" t="s">
+      <c r="U21" s="85" t="s">
         <v>245</v>
       </c>
-      <c r="V21" s="1" t="s">
+      <c r="V21" s="85" t="s">
         <v>246</v>
       </c>
-      <c r="W21" s="1" t="s">
+      <c r="W21" s="85" t="s">
         <v>247</v>
       </c>
-      <c r="X21" s="1" t="s">
+      <c r="X21" s="85" t="s">
         <v>248</v>
       </c>
-      <c r="Y21" s="1" t="s">
+      <c r="Y21" s="85" t="s">
         <v>249</v>
       </c>
-      <c r="Z21" s="1" t="s">
+      <c r="Z21" s="85" t="s">
         <v>250</v>
       </c>
-      <c r="AA21" s="1" t="s">
+      <c r="AA21" s="85" t="s">
         <v>251</v>
       </c>
-      <c r="AB21" s="1" t="s">
+      <c r="AB21" s="85" t="s">
         <v>252</v>
       </c>
     </row>
     <row r="24" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="55" t="s">
+      <c r="B24" s="36" t="s">
         <v>26</v>
       </c>
-      <c r="C24" s="55"/>
-      <c r="D24" s="55"/>
-      <c r="E24" s="55"/>
-      <c r="F24" s="55"/>
-      <c r="G24" s="55"/>
-      <c r="H24" s="55"/>
-      <c r="I24" s="55"/>
-      <c r="J24" s="55"/>
-      <c r="K24" s="55"/>
-      <c r="L24" s="55"/>
-      <c r="M24" s="55"/>
-      <c r="N24" s="55"/>
-      <c r="O24" s="55"/>
-      <c r="P24" s="55"/>
-      <c r="Q24" s="55"/>
-      <c r="R24" s="55"/>
-      <c r="S24" s="55"/>
-      <c r="T24" s="55"/>
-      <c r="U24" s="55"/>
-      <c r="V24" s="55"/>
-      <c r="W24" s="55"/>
-      <c r="X24" s="55"/>
-      <c r="Y24" s="55"/>
-      <c r="Z24" s="55"/>
-      <c r="AA24" s="55"/>
-      <c r="AB24" s="55"/>
+      <c r="C24" s="36"/>
+      <c r="D24" s="36"/>
+      <c r="E24" s="36"/>
+      <c r="F24" s="36"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="36"/>
+      <c r="R24" s="36"/>
+      <c r="S24" s="36"/>
+      <c r="T24" s="36"/>
+      <c r="U24" s="36"/>
+      <c r="V24" s="36"/>
+      <c r="W24" s="36"/>
+      <c r="X24" s="36"/>
+      <c r="Y24" s="36"/>
+      <c r="Z24" s="36"/>
+      <c r="AA24" s="36"/>
+      <c r="AB24" s="36"/>
     </row>
     <row r="26" spans="2:28" ht="75" x14ac:dyDescent="0.25">
-      <c r="B26" s="44" t="s">
+      <c r="B26" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="C26" s="44"/>
-      <c r="D26" s="23" t="s">
+      <c r="C26" s="29"/>
+      <c r="D26" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E26" s="23" t="s">
+      <c r="E26" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F26" s="23" t="s">
+      <c r="F26" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G26" s="23" t="s">
+      <c r="G26" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H26" s="23" t="s">
+      <c r="H26" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I26" s="23" t="s">
+      <c r="I26" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J26" s="23" t="s">
+      <c r="J26" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K26" s="23" t="s">
+      <c r="K26" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L26" s="23" t="s">
+      <c r="L26" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="M26" s="23" t="s">
+      <c r="M26" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="N26" s="23" t="s">
+      <c r="N26" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="O26" s="23" t="s">
+      <c r="O26" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P26" s="23" t="s">
+      <c r="P26" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Q26" s="23" t="s">
+      <c r="Q26" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R26" s="23" t="s">
+      <c r="R26" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="S26" s="23" t="s">
+      <c r="S26" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T26" s="23" t="s">
+      <c r="T26" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U26" s="23" t="s">
+      <c r="U26" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="V26" s="32" t="s">
+      <c r="V26" s="27" t="s">
         <v>24</v>
       </c>
-      <c r="W26" s="32" t="s">
+      <c r="W26" s="27" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="27" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B27" s="74" t="s">
+      <c r="B27" s="30" t="s">
         <v>29</v>
       </c>
-      <c r="C27" s="74"/>
-      <c r="D27" s="29" t="s">
+      <c r="C27" s="30"/>
+      <c r="D27" s="83" t="s">
         <v>87</v>
       </c>
-      <c r="E27" s="29" t="s">
+      <c r="E27" s="83" t="s">
         <v>88</v>
       </c>
-      <c r="F27" s="29" t="s">
+      <c r="F27" s="83" t="s">
         <v>89</v>
       </c>
-      <c r="G27" s="29" t="s">
+      <c r="G27" s="83" t="s">
         <v>90</v>
       </c>
-      <c r="H27" s="29" t="s">
+      <c r="H27" s="83" t="s">
         <v>91</v>
       </c>
-      <c r="I27" s="29" t="s">
+      <c r="I27" s="83" t="s">
         <v>92</v>
       </c>
-      <c r="J27" s="29" t="s">
+      <c r="J27" s="83" t="s">
         <v>93</v>
       </c>
-      <c r="K27" s="29" t="s">
+      <c r="K27" s="83" t="s">
         <v>94</v>
       </c>
-      <c r="L27" s="29" t="s">
+      <c r="L27" s="83" t="s">
         <v>95</v>
       </c>
-      <c r="M27" s="29" t="s">
+      <c r="M27" s="83" t="s">
         <v>96</v>
       </c>
-      <c r="N27" s="29" t="s">
+      <c r="N27" s="83" t="s">
         <v>97</v>
       </c>
-      <c r="O27" s="29" t="s">
+      <c r="O27" s="83" t="s">
         <v>98</v>
       </c>
-      <c r="P27" s="29" t="s">
+      <c r="P27" s="83" t="s">
         <v>99</v>
       </c>
-      <c r="Q27" s="29" t="s">
+      <c r="Q27" s="83" t="s">
         <v>100</v>
       </c>
-      <c r="R27" s="29" t="s">
+      <c r="R27" s="83" t="s">
         <v>101</v>
       </c>
-      <c r="S27" s="29" t="s">
+      <c r="S27" s="83" t="s">
         <v>102</v>
       </c>
-      <c r="T27" s="29" t="s">
+      <c r="T27" s="83" t="s">
         <v>103</v>
       </c>
-      <c r="U27" s="29" t="s">
+      <c r="U27" s="83" t="s">
         <v>104</v>
       </c>
-      <c r="V27" s="29" t="s">
+      <c r="V27" s="83" t="s">
         <v>105</v>
       </c>
-      <c r="W27" s="29" t="s">
+      <c r="W27" s="83" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="28" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B28" s="74"/>
-      <c r="C28" s="74"/>
-      <c r="D28" s="1"/>
-      <c r="E28" s="1"/>
-      <c r="F28" s="1"/>
-      <c r="G28" s="1"/>
-      <c r="H28" s="1"/>
-      <c r="I28" s="1"/>
-      <c r="J28" s="1"/>
-      <c r="K28" s="1"/>
-      <c r="L28" s="1"/>
-      <c r="M28" s="1"/>
-      <c r="N28" s="1"/>
-      <c r="O28" s="1"/>
-      <c r="P28" s="1"/>
-      <c r="Q28" s="1"/>
-      <c r="R28" s="1"/>
-      <c r="S28" s="1"/>
-      <c r="T28" s="1"/>
-      <c r="U28" s="1"/>
-      <c r="V28" s="1"/>
-      <c r="W28" s="1"/>
+      <c r="B28" s="30"/>
+      <c r="C28" s="30"/>
+      <c r="D28" s="85"/>
+      <c r="E28" s="85"/>
+      <c r="F28" s="85"/>
+      <c r="G28" s="85"/>
+      <c r="H28" s="85"/>
+      <c r="I28" s="85"/>
+      <c r="J28" s="85"/>
+      <c r="K28" s="85"/>
+      <c r="L28" s="85"/>
+      <c r="M28" s="85"/>
+      <c r="N28" s="85"/>
+      <c r="O28" s="85"/>
+      <c r="P28" s="85"/>
+      <c r="Q28" s="85"/>
+      <c r="R28" s="85"/>
+      <c r="S28" s="85"/>
+      <c r="T28" s="85"/>
+      <c r="U28" s="85"/>
+      <c r="V28" s="85"/>
+      <c r="W28" s="85"/>
     </row>
     <row r="30" spans="2:28" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="42"/>
-      <c r="C30" s="42"/>
-      <c r="D30" s="33" t="s">
+      <c r="B30" s="62"/>
+      <c r="C30" s="62"/>
+      <c r="D30" s="28" t="s">
         <v>18</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F30" s="23" t="s">
+      <c r="F30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G30" s="23" t="s">
+      <c r="G30" s="22" t="s">
         <v>19</v>
       </c>
-      <c r="H30" s="23" t="s">
+      <c r="H30" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="I30" s="23" t="s">
+      <c r="I30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="J30" s="23" t="s">
+      <c r="J30" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="K30" s="23" t="s">
+      <c r="K30" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="L30" s="23" t="s">
+      <c r="L30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="M30" s="23" t="s">
+      <c r="M30" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="N30" s="23" t="s">
+      <c r="N30" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="O30" s="23" t="s">
+      <c r="O30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P30" s="23" t="s">
+      <c r="P30" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Q30" s="23" t="s">
+      <c r="Q30" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R30" s="23" t="s">
+      <c r="R30" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="S30" s="23" t="s">
+      <c r="S30" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T30" s="23" t="s">
+      <c r="T30" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U30" s="23" t="s">
+      <c r="U30" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B31" s="43" t="s">
+      <c r="B31" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="C31" s="43"/>
-      <c r="D31" s="36" t="s">
+      <c r="C31" s="63"/>
+      <c r="D31" s="89" t="s">
         <v>253</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E31" s="90" t="s">
         <v>254</v>
       </c>
-      <c r="F31" s="36" t="s">
+      <c r="F31" s="89" t="s">
         <v>255</v>
       </c>
-      <c r="G31" s="36" t="s">
+      <c r="G31" s="89" t="s">
         <v>256</v>
       </c>
-      <c r="H31" s="30" t="s">
+      <c r="H31" s="90" t="s">
         <v>257</v>
       </c>
-      <c r="I31" s="36" t="s">
+      <c r="I31" s="89" t="s">
         <v>258</v>
       </c>
-      <c r="J31" s="36" t="s">
+      <c r="J31" s="89" t="s">
         <v>259</v>
       </c>
-      <c r="K31" s="30" t="s">
+      <c r="K31" s="90" t="s">
         <v>260</v>
       </c>
-      <c r="L31" s="36" t="s">
+      <c r="L31" s="89" t="s">
         <v>261</v>
       </c>
-      <c r="M31" s="36" t="s">
+      <c r="M31" s="89" t="s">
         <v>262</v>
       </c>
-      <c r="N31" s="30" t="s">
+      <c r="N31" s="90" t="s">
         <v>263</v>
       </c>
-      <c r="O31" s="36" t="s">
+      <c r="O31" s="89" t="s">
         <v>264</v>
       </c>
-      <c r="P31" s="36" t="s">
+      <c r="P31" s="89" t="s">
         <v>265</v>
       </c>
-      <c r="Q31" s="30" t="s">
+      <c r="Q31" s="90" t="s">
         <v>266</v>
       </c>
-      <c r="R31" s="36" t="s">
+      <c r="R31" s="89" t="s">
         <v>267</v>
       </c>
-      <c r="S31" s="36" t="s">
+      <c r="S31" s="89" t="s">
         <v>268</v>
       </c>
-      <c r="T31" s="30" t="s">
+      <c r="T31" s="90" t="s">
         <v>269</v>
       </c>
-      <c r="U31" s="36" t="s">
+      <c r="U31" s="89" t="s">
         <v>270</v>
       </c>
     </row>
     <row r="32" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B32" s="43" t="s">
+      <c r="B32" s="63" t="s">
         <v>56</v>
       </c>
-      <c r="C32" s="43"/>
-      <c r="D32" s="36" t="s">
+      <c r="C32" s="63"/>
+      <c r="D32" s="89" t="s">
         <v>271</v>
       </c>
-      <c r="E32" s="30" t="s">
+      <c r="E32" s="90" t="s">
         <v>272</v>
       </c>
-      <c r="F32" s="36" t="s">
+      <c r="F32" s="89" t="s">
         <v>273</v>
       </c>
-      <c r="G32" s="36" t="s">
+      <c r="G32" s="89" t="s">
         <v>274</v>
       </c>
-      <c r="H32" s="30" t="s">
+      <c r="H32" s="90" t="s">
         <v>275</v>
       </c>
-      <c r="I32" s="36" t="s">
+      <c r="I32" s="89" t="s">
         <v>276</v>
       </c>
-      <c r="J32" s="36" t="s">
+      <c r="J32" s="89" t="s">
         <v>277</v>
       </c>
-      <c r="K32" s="30" t="s">
+      <c r="K32" s="90" t="s">
         <v>278</v>
       </c>
-      <c r="L32" s="36" t="s">
+      <c r="L32" s="89" t="s">
         <v>279</v>
       </c>
-      <c r="M32" s="36" t="s">
+      <c r="M32" s="89" t="s">
         <v>280</v>
       </c>
-      <c r="N32" s="30" t="s">
+      <c r="N32" s="90" t="s">
         <v>281</v>
       </c>
-      <c r="O32" s="36" t="s">
+      <c r="O32" s="89" t="s">
         <v>282</v>
       </c>
-      <c r="P32" s="36" t="s">
+      <c r="P32" s="89" t="s">
         <v>283</v>
       </c>
-      <c r="Q32" s="30" t="s">
+      <c r="Q32" s="90" t="s">
         <v>284</v>
       </c>
-      <c r="R32" s="36" t="s">
+      <c r="R32" s="89" t="s">
         <v>285</v>
       </c>
-      <c r="S32" s="36" t="s">
+      <c r="S32" s="89" t="s">
         <v>286</v>
       </c>
-      <c r="T32" s="30" t="s">
+      <c r="T32" s="90" t="s">
         <v>287</v>
       </c>
-      <c r="U32" s="36" t="s">
+      <c r="U32" s="89" t="s">
         <v>288</v>
       </c>
     </row>
     <row r="33" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B33" s="45" t="s">
+      <c r="B33" s="64" t="s">
         <v>27</v>
       </c>
-      <c r="C33" s="45"/>
-      <c r="D33" s="34" t="s">
+      <c r="C33" s="64"/>
+      <c r="D33" s="91" t="s">
         <v>289</v>
       </c>
-      <c r="E33" s="30" t="s">
+      <c r="E33" s="90" t="s">
         <v>290</v>
       </c>
-      <c r="F33" s="34" t="s">
+      <c r="F33" s="91" t="s">
         <v>291</v>
       </c>
-      <c r="G33" s="34" t="s">
+      <c r="G33" s="91" t="s">
         <v>292</v>
       </c>
-      <c r="H33" s="34" t="s">
+      <c r="H33" s="91" t="s">
         <v>293</v>
       </c>
-      <c r="I33" s="34" t="s">
+      <c r="I33" s="91" t="s">
         <v>294</v>
       </c>
-      <c r="J33" s="34" t="s">
+      <c r="J33" s="91" t="s">
         <v>295</v>
       </c>
-      <c r="K33" s="34" t="s">
+      <c r="K33" s="91" t="s">
         <v>296</v>
       </c>
-      <c r="L33" s="34" t="s">
+      <c r="L33" s="91" t="s">
         <v>297</v>
       </c>
-      <c r="M33" s="34" t="s">
+      <c r="M33" s="91" t="s">
         <v>298</v>
       </c>
-      <c r="N33" s="30" t="s">
+      <c r="N33" s="90" t="s">
         <v>299</v>
       </c>
-      <c r="O33" s="34" t="s">
+      <c r="O33" s="91" t="s">
         <v>300</v>
       </c>
-      <c r="P33" s="34" t="s">
+      <c r="P33" s="91" t="s">
         <v>301</v>
       </c>
-      <c r="Q33" s="30" t="s">
+      <c r="Q33" s="90" t="s">
         <v>302</v>
       </c>
-      <c r="R33" s="34" t="s">
+      <c r="R33" s="91" t="s">
         <v>303</v>
       </c>
-      <c r="S33" s="34" t="s">
+      <c r="S33" s="91" t="s">
         <v>304</v>
       </c>
-      <c r="T33" s="30" t="s">
+      <c r="T33" s="90" t="s">
         <v>305</v>
       </c>
-      <c r="U33" s="34" t="s">
+      <c r="U33" s="91" t="s">
         <v>306</v>
       </c>
     </row>
     <row r="34" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="K34" s="22"/>
+      <c r="K34" s="21"/>
     </row>
     <row r="35" spans="2:21" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="44"/>
-      <c r="C35" s="44"/>
-      <c r="D35" s="23" t="s">
+      <c r="B35" s="29"/>
+      <c r="C35" s="29"/>
+      <c r="D35" s="22" t="s">
         <v>18</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="23" t="s">
+      <c r="F35" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="G35" s="23"/>
-      <c r="H35" s="23"/>
-      <c r="I35" s="23"/>
-      <c r="J35" s="23"/>
-      <c r="K35" s="23"/>
-      <c r="L35" s="23"/>
-      <c r="M35" s="23" t="s">
+      <c r="G35" s="22"/>
+      <c r="H35" s="22"/>
+      <c r="I35" s="22"/>
+      <c r="J35" s="22"/>
+      <c r="K35" s="22"/>
+      <c r="L35" s="22"/>
+      <c r="M35" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="N35" s="23" t="s">
+      <c r="N35" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="O35" s="23" t="s">
+      <c r="O35" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="P35" s="23" t="s">
+      <c r="P35" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="Q35" s="23" t="s">
+      <c r="Q35" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="R35" s="23" t="s">
+      <c r="R35" s="22" t="s">
         <v>7</v>
       </c>
-      <c r="S35" s="23" t="s">
+      <c r="S35" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="T35" s="23" t="s">
+      <c r="T35" s="22" t="s">
         <v>6</v>
       </c>
-      <c r="U35" s="23" t="s">
+      <c r="U35" s="22" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="36" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B36" s="43" t="s">
+      <c r="B36" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="C36" s="43"/>
-      <c r="D36" s="36" t="s">
+      <c r="C36" s="63"/>
+      <c r="D36" s="89" t="s">
         <v>307</v>
       </c>
-      <c r="E36" s="30" t="s">
+      <c r="E36" s="90" t="s">
         <v>308</v>
       </c>
-      <c r="F36" s="36" t="s">
+      <c r="F36" s="89" t="s">
         <v>309</v>
       </c>
-      <c r="G36" s="36" t="s">
+      <c r="G36" s="89" t="s">
         <v>310</v>
       </c>
-      <c r="H36" s="30" t="s">
+      <c r="H36" s="90" t="s">
         <v>311</v>
       </c>
-      <c r="I36" s="36" t="s">
+      <c r="I36" s="89" t="s">
         <v>312</v>
       </c>
-      <c r="J36" s="36" t="s">
+      <c r="J36" s="89" t="s">
         <v>313</v>
       </c>
-      <c r="K36" s="30" t="s">
+      <c r="K36" s="90" t="s">
         <v>314</v>
       </c>
-      <c r="L36" s="36" t="s">
+      <c r="L36" s="89" t="s">
         <v>315</v>
       </c>
-      <c r="M36" s="36" t="s">
+      <c r="M36" s="89" t="s">
         <v>316</v>
       </c>
-      <c r="N36" s="30" t="s">
+      <c r="N36" s="90" t="s">
         <v>317</v>
       </c>
-      <c r="O36" s="36" t="s">
+      <c r="O36" s="89" t="s">
         <v>318</v>
       </c>
-      <c r="P36" s="36" t="s">
+      <c r="P36" s="89" t="s">
         <v>319</v>
       </c>
-      <c r="Q36" s="30" t="s">
+      <c r="Q36" s="90" t="s">
         <v>320</v>
       </c>
-      <c r="R36" s="36" t="s">
+      <c r="R36" s="89" t="s">
         <v>321</v>
       </c>
-      <c r="S36" s="36" t="s">
+      <c r="S36" s="89" t="s">
         <v>322</v>
       </c>
-      <c r="T36" s="30" t="s">
+      <c r="T36" s="90" t="s">
         <v>323</v>
       </c>
-      <c r="U36" s="36" t="s">
+      <c r="U36" s="89" t="s">
         <v>324</v>
       </c>
     </row>
     <row r="37" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B37" s="46" t="s">
+      <c r="B37" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C37" s="47"/>
-      <c r="D37" s="36" t="s">
+      <c r="C37" s="66"/>
+      <c r="D37" s="89" t="s">
         <v>325</v>
       </c>
-      <c r="E37" s="30" t="s">
+      <c r="E37" s="90" t="s">
         <v>326</v>
       </c>
-      <c r="F37" s="36" t="s">
+      <c r="F37" s="89" t="s">
         <v>327</v>
       </c>
-      <c r="G37" s="36" t="s">
+      <c r="G37" s="89" t="s">
         <v>328</v>
       </c>
-      <c r="H37" s="36" t="s">
+      <c r="H37" s="89" t="s">
         <v>329</v>
       </c>
-      <c r="I37" s="36" t="s">
+      <c r="I37" s="89" t="s">
         <v>330</v>
       </c>
-      <c r="J37" s="36" t="s">
+      <c r="J37" s="89" t="s">
         <v>331</v>
       </c>
-      <c r="K37" s="36" t="s">
+      <c r="K37" s="89" t="s">
         <v>332</v>
       </c>
-      <c r="L37" s="36" t="s">
+      <c r="L37" s="89" t="s">
         <v>333</v>
       </c>
-      <c r="M37" s="36" t="s">
+      <c r="M37" s="89" t="s">
         <v>334</v>
       </c>
-      <c r="N37" s="30" t="s">
+      <c r="N37" s="90" t="s">
         <v>335</v>
       </c>
-      <c r="O37" s="36" t="s">
+      <c r="O37" s="89" t="s">
         <v>336</v>
       </c>
-      <c r="P37" s="36" t="s">
+      <c r="P37" s="89" t="s">
         <v>337</v>
       </c>
-      <c r="Q37" s="30" t="s">
+      <c r="Q37" s="90" t="s">
         <v>338</v>
       </c>
-      <c r="R37" s="36" t="s">
+      <c r="R37" s="89" t="s">
         <v>339</v>
       </c>
-      <c r="S37" s="36" t="s">
+      <c r="S37" s="89" t="s">
         <v>340</v>
       </c>
-      <c r="T37" s="30" t="s">
+      <c r="T37" s="90" t="s">
         <v>341</v>
       </c>
-      <c r="U37" s="37" t="s">
+      <c r="U37" s="92" t="s">
         <v>342</v>
       </c>
     </row>
     <row r="38" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B38" s="48" t="s">
+      <c r="B38" s="67" t="s">
         <v>27</v>
       </c>
-      <c r="C38" s="49"/>
-      <c r="D38" s="34" t="s">
+      <c r="C38" s="68"/>
+      <c r="D38" s="91" t="s">
         <v>343</v>
       </c>
-      <c r="E38" s="30" t="s">
+      <c r="E38" s="90" t="s">
         <v>344</v>
       </c>
-      <c r="F38" s="34" t="s">
+      <c r="F38" s="91" t="s">
         <v>345</v>
       </c>
-      <c r="G38" s="34" t="s">
+      <c r="G38" s="91" t="s">
         <v>346</v>
       </c>
-      <c r="H38" s="34" t="s">
+      <c r="H38" s="91" t="s">
         <v>347</v>
       </c>
-      <c r="I38" s="34" t="s">
+      <c r="I38" s="91" t="s">
         <v>348</v>
       </c>
-      <c r="J38" s="34" t="s">
+      <c r="J38" s="91" t="s">
         <v>349</v>
       </c>
-      <c r="K38" s="34" t="s">
+      <c r="K38" s="91" t="s">
         <v>350</v>
       </c>
-      <c r="L38" s="34" t="s">
+      <c r="L38" s="91" t="s">
         <v>351</v>
       </c>
-      <c r="M38" s="34" t="s">
+      <c r="M38" s="91" t="s">
         <v>352</v>
       </c>
-      <c r="N38" s="30" t="s">
+      <c r="N38" s="90" t="s">
         <v>353</v>
       </c>
-      <c r="O38" s="34" t="s">
+      <c r="O38" s="91" t="s">
         <v>354</v>
       </c>
-      <c r="P38" s="34" t="s">
+      <c r="P38" s="91" t="s">
         <v>355</v>
       </c>
-      <c r="Q38" s="30" t="s">
+      <c r="Q38" s="90" t="s">
         <v>356</v>
       </c>
-      <c r="R38" s="34" t="s">
+      <c r="R38" s="91" t="s">
         <v>357</v>
       </c>
-      <c r="S38" s="34" t="s">
+      <c r="S38" s="91" t="s">
         <v>358</v>
       </c>
-      <c r="T38" s="30" t="s">
+      <c r="T38" s="90" t="s">
         <v>359</v>
       </c>
-      <c r="U38" s="34" t="s">
+      <c r="U38" s="91" t="s">
         <v>360</v>
       </c>
     </row>
     <row r="40" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B40" s="40" t="s">
+      <c r="B40" s="60" t="s">
         <v>28</v>
       </c>
-      <c r="C40" s="41"/>
-      <c r="D40" s="35" t="s">
+      <c r="C40" s="61"/>
+      <c r="D40" s="93" t="s">
         <v>361</v>
       </c>
-      <c r="E40" s="35" t="s">
+      <c r="E40" s="93" t="s">
         <v>362</v>
       </c>
-      <c r="F40" s="35" t="s">
+      <c r="F40" s="93" t="s">
         <v>363</v>
       </c>
-      <c r="G40" s="35" t="s">
+      <c r="G40" s="93" t="s">
         <v>364</v>
       </c>
-      <c r="H40" s="35" t="s">
+      <c r="H40" s="93" t="s">
         <v>365</v>
       </c>
-      <c r="I40" s="35" t="s">
+      <c r="I40" s="93" t="s">
         <v>366</v>
       </c>
-      <c r="J40" s="35" t="s">
+      <c r="J40" s="93" t="s">
         <v>367</v>
       </c>
-      <c r="K40" s="35" t="s">
+      <c r="K40" s="93" t="s">
         <v>368</v>
       </c>
-      <c r="L40" s="35" t="s">
+      <c r="L40" s="93" t="s">
         <v>369</v>
       </c>
-      <c r="M40" s="35" t="s">
+      <c r="M40" s="93" t="s">
         <v>370</v>
       </c>
-      <c r="N40" s="35" t="s">
+      <c r="N40" s="93" t="s">
         <v>371</v>
       </c>
-      <c r="O40" s="35" t="s">
+      <c r="O40" s="93" t="s">
         <v>372</v>
       </c>
-      <c r="P40" s="35" t="s">
+      <c r="P40" s="93" t="s">
         <v>373</v>
       </c>
-      <c r="Q40" s="35" t="s">
+      <c r="Q40" s="93" t="s">
         <v>374</v>
       </c>
-      <c r="R40" s="35" t="s">
+      <c r="R40" s="93" t="s">
         <v>375</v>
       </c>
-      <c r="S40" s="35" t="s">
+      <c r="S40" s="93" t="s">
         <v>376</v>
       </c>
-      <c r="T40" s="35" t="s">
+      <c r="T40" s="93" t="s">
         <v>377</v>
       </c>
-      <c r="U40" s="35" t="s">
+      <c r="U40" s="93" t="s">
         <v>378</v>
       </c>
     </row>
     <row r="41" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B41" s="40" t="s">
+      <c r="B41" s="60" t="s">
         <v>228</v>
       </c>
-      <c r="C41" s="41"/>
-      <c r="D41" s="35" t="s">
+      <c r="C41" s="61"/>
+      <c r="D41" s="93" t="s">
         <v>379</v>
       </c>
-      <c r="E41" s="35" t="s">
+      <c r="E41" s="93" t="s">
         <v>380</v>
       </c>
-      <c r="F41" s="35" t="s">
+      <c r="F41" s="93" t="s">
         <v>381</v>
       </c>
-      <c r="G41" s="35" t="s">
+      <c r="G41" s="93" t="s">
         <v>382</v>
       </c>
-      <c r="H41" s="35" t="s">
+      <c r="H41" s="93" t="s">
         <v>383</v>
       </c>
-      <c r="I41" s="35" t="s">
+      <c r="I41" s="93" t="s">
         <v>384</v>
       </c>
-      <c r="J41" s="35" t="s">
+      <c r="J41" s="93" t="s">
         <v>385</v>
       </c>
-      <c r="K41" s="35" t="s">
+      <c r="K41" s="93" t="s">
         <v>386</v>
       </c>
-      <c r="L41" s="35" t="s">
+      <c r="L41" s="93" t="s">
         <v>387</v>
       </c>
-      <c r="M41" s="35" t="s">
+      <c r="M41" s="93" t="s">
         <v>388</v>
       </c>
-      <c r="N41" s="35" t="s">
+      <c r="N41" s="93" t="s">
         <v>389</v>
       </c>
-      <c r="O41" s="35" t="s">
+      <c r="O41" s="93" t="s">
         <v>390</v>
       </c>
-      <c r="P41" s="35" t="s">
+      <c r="P41" s="93" t="s">
         <v>391</v>
       </c>
-      <c r="Q41" s="35" t="s">
+      <c r="Q41" s="93" t="s">
         <v>392</v>
       </c>
-      <c r="R41" s="35" t="s">
+      <c r="R41" s="93" t="s">
         <v>393</v>
       </c>
-      <c r="S41" s="35" t="s">
+      <c r="S41" s="93" t="s">
         <v>394</v>
       </c>
-      <c r="T41" s="35" t="s">
+      <c r="T41" s="93" t="s">
         <v>395</v>
       </c>
-      <c r="U41" s="35" t="s">
+      <c r="U41" s="93" t="s">
         <v>396</v>
       </c>
     </row>
     <row r="42" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E42" s="22"/>
+      <c r="E42" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B41:C41"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B40:C40"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B32:C32"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B37:C37"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="Z6:AB6"/>
+    <mergeCell ref="B4:AB4"/>
+    <mergeCell ref="B6:D7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="W6:Y6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
     <mergeCell ref="B26:C26"/>
     <mergeCell ref="B27:C27"/>
     <mergeCell ref="B28:C28"/>
@@ -4286,27 +4347,6 @@
     <mergeCell ref="B24:AB24"/>
     <mergeCell ref="B20:D20"/>
     <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="Z6:AB6"/>
-    <mergeCell ref="B4:AB4"/>
-    <mergeCell ref="B6:D7"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="W6:Y6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4321,7 +4361,7 @@
   <dimension ref="B2:L31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="B2" sqref="B2:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4337,10 +4377,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="88" t="s">
+      <c r="B2" s="77" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="88"/>
+      <c r="C2" s="77"/>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4352,71 +4392,71 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="55" t="s">
+      <c r="B4" s="36" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="55"/>
-      <c r="D4" s="55"/>
-      <c r="E4" s="55"/>
-      <c r="F4" s="55"/>
-      <c r="G4" s="55"/>
-      <c r="H4" s="55"/>
-      <c r="I4" s="55"/>
-      <c r="J4" s="55"/>
-      <c r="K4" s="55"/>
-      <c r="L4" s="55"/>
+      <c r="C4" s="36"/>
+      <c r="D4" s="36"/>
+      <c r="E4" s="36"/>
+      <c r="F4" s="36"/>
+      <c r="G4" s="36"/>
+      <c r="H4" s="36"/>
+      <c r="I4" s="36"/>
+      <c r="J4" s="36"/>
+      <c r="K4" s="36"/>
+      <c r="L4" s="36"/>
     </row>
     <row r="6" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="56" t="s">
+      <c r="B6" s="42" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="90" t="s">
+      <c r="C6" s="79" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="91"/>
-      <c r="E6" s="91"/>
-      <c r="F6" s="92"/>
-      <c r="G6" s="89" t="s">
+      <c r="D6" s="80"/>
+      <c r="E6" s="80"/>
+      <c r="F6" s="81"/>
+      <c r="G6" s="78" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="89"/>
-      <c r="I6" s="89"/>
-      <c r="J6" s="70" t="s">
+      <c r="H6" s="78"/>
+      <c r="I6" s="78"/>
+      <c r="J6" s="56" t="s">
         <v>73</v>
       </c>
-      <c r="K6" s="71"/>
-      <c r="L6" s="71"/>
+      <c r="K6" s="57"/>
+      <c r="L6" s="57"/>
     </row>
     <row r="7" spans="2:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="59"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="45"/>
+      <c r="C7" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E7" s="23" t="s">
+      <c r="E7" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F7" s="23" t="s">
+      <c r="F7" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H7" s="23" t="s">
+      <c r="H7" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="I7" s="23" t="s">
+      <c r="I7" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="J7" s="24" t="s">
+      <c r="J7" s="23" t="s">
         <v>71</v>
       </c>
-      <c r="K7" s="24" t="s">
+      <c r="K7" s="23" t="s">
         <v>70</v>
       </c>
-      <c r="L7" s="24" t="s">
+      <c r="L7" s="23" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4424,82 +4464,82 @@
       <c r="B8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="C8" s="94" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="1" t="s">
+      <c r="D8" s="85" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="1" t="s">
+      <c r="E8" s="85" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="1" t="s">
+      <c r="F8" s="85" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="1" t="s">
+      <c r="G8" s="85" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="1" t="s">
+      <c r="H8" s="85" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="1" t="s">
+      <c r="I8" s="85" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="1" t="s">
+      <c r="J8" s="85" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="1" t="s">
+      <c r="K8" s="85" t="s">
         <v>85</v>
       </c>
-      <c r="L8" s="1" t="s">
+      <c r="L8" s="85" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
-      <c r="C9" s="6"/>
-      <c r="D9" s="1"/>
-      <c r="E9" s="1"/>
-      <c r="F9" s="1"/>
-      <c r="G9" s="1"/>
-      <c r="H9" s="1"/>
-      <c r="I9" s="1"/>
-      <c r="J9" s="1"/>
-      <c r="K9" s="1"/>
-      <c r="L9" s="1"/>
+      <c r="C9" s="94"/>
+      <c r="D9" s="85"/>
+      <c r="E9" s="85"/>
+      <c r="F9" s="85"/>
+      <c r="G9" s="85"/>
+      <c r="H9" s="85"/>
+      <c r="I9" s="85"/>
+      <c r="J9" s="85"/>
+      <c r="K9" s="85"/>
+      <c r="L9" s="85"/>
     </row>
     <row r="11" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C11" s="23" t="s">
+      <c r="C11" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D11" s="23" t="s">
+      <c r="D11" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E11" s="23" t="s">
+      <c r="E11" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F11" s="23" t="s">
+      <c r="F11" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="G11" s="23" t="s">
+      <c r="G11" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H11" s="23" t="s">
+      <c r="H11" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="I11" s="23" t="s">
+      <c r="I11" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="J11" s="23" t="s">
+      <c r="J11" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="K11" s="23" t="s">
+      <c r="K11" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="L11" s="23" t="s">
+      <c r="L11" s="22" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4507,34 +4547,34 @@
       <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="1" t="s">
+      <c r="C12" s="85" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="1" t="s">
+      <c r="D12" s="85" t="s">
         <v>398</v>
       </c>
-      <c r="E12" s="1" t="s">
+      <c r="E12" s="85" t="s">
         <v>399</v>
       </c>
-      <c r="F12" s="1" t="s">
+      <c r="F12" s="85" t="s">
         <v>400</v>
       </c>
-      <c r="G12" s="1" t="s">
+      <c r="G12" s="85" t="s">
         <v>401</v>
       </c>
-      <c r="H12" s="1" t="s">
+      <c r="H12" s="85" t="s">
         <v>402</v>
       </c>
-      <c r="I12" s="1" t="s">
+      <c r="I12" s="85" t="s">
         <v>403</v>
       </c>
-      <c r="J12" s="1" t="s">
+      <c r="J12" s="85" t="s">
         <v>404</v>
       </c>
-      <c r="K12" s="1" t="s">
+      <c r="K12" s="85" t="s">
         <v>405</v>
       </c>
-      <c r="L12" s="93" t="s">
+      <c r="L12" s="85" t="s">
         <v>406</v>
       </c>
     </row>
@@ -4542,34 +4582,34 @@
       <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="1" t="s">
+      <c r="C13" s="85" t="s">
         <v>407</v>
       </c>
-      <c r="D13" s="1" t="s">
+      <c r="D13" s="85" t="s">
         <v>408</v>
       </c>
-      <c r="E13" s="1" t="s">
+      <c r="E13" s="85" t="s">
         <v>409</v>
       </c>
-      <c r="F13" s="1" t="s">
+      <c r="F13" s="85" t="s">
         <v>410</v>
       </c>
-      <c r="G13" s="1" t="s">
+      <c r="G13" s="85" t="s">
         <v>411</v>
       </c>
-      <c r="H13" s="1" t="s">
+      <c r="H13" s="85" t="s">
         <v>412</v>
       </c>
-      <c r="I13" s="1" t="s">
+      <c r="I13" s="85" t="s">
         <v>413</v>
       </c>
-      <c r="J13" s="1" t="s">
+      <c r="J13" s="85" t="s">
         <v>414</v>
       </c>
-      <c r="K13" s="1" t="s">
+      <c r="K13" s="85" t="s">
         <v>415</v>
       </c>
-      <c r="L13" s="1" t="s">
+      <c r="L13" s="85" t="s">
         <v>416</v>
       </c>
     </row>
@@ -4577,34 +4617,34 @@
       <c r="B15" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="23" t="s">
+      <c r="C15" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="D15" s="23" t="s">
+      <c r="D15" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="E15" s="23" t="s">
+      <c r="E15" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="F15" s="23" t="s">
+      <c r="F15" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="G15" s="23" t="s">
+      <c r="G15" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="H15" s="23" t="s">
+      <c r="H15" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="I15" s="23" t="s">
+      <c r="I15" s="22" t="s">
         <v>69</v>
       </c>
-      <c r="J15" s="23" t="s">
+      <c r="J15" s="22" t="s">
         <v>71</v>
       </c>
-      <c r="K15" s="23" t="s">
+      <c r="K15" s="22" t="s">
         <v>70</v>
       </c>
-      <c r="L15" s="23" t="s">
+      <c r="L15" s="22" t="s">
         <v>69</v>
       </c>
     </row>
@@ -4612,34 +4652,34 @@
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="1" t="s">
+      <c r="C16" s="85" t="s">
         <v>417</v>
       </c>
-      <c r="D16" s="1" t="s">
+      <c r="D16" s="85" t="s">
         <v>418</v>
       </c>
-      <c r="E16" s="1" t="s">
+      <c r="E16" s="85" t="s">
         <v>419</v>
       </c>
-      <c r="F16" s="1" t="s">
+      <c r="F16" s="85" t="s">
         <v>420</v>
       </c>
-      <c r="G16" s="1" t="s">
+      <c r="G16" s="85" t="s">
         <v>421</v>
       </c>
-      <c r="H16" s="1" t="s">
+      <c r="H16" s="85" t="s">
         <v>422</v>
       </c>
-      <c r="I16" s="1" t="s">
+      <c r="I16" s="85" t="s">
         <v>423</v>
       </c>
-      <c r="J16" s="1" t="s">
+      <c r="J16" s="85" t="s">
         <v>424</v>
       </c>
-      <c r="K16" s="1" t="s">
+      <c r="K16" s="85" t="s">
         <v>425</v>
       </c>
-      <c r="L16" s="1" t="s">
+      <c r="L16" s="85" t="s">
         <v>426</v>
       </c>
     </row>
@@ -4647,34 +4687,34 @@
       <c r="B17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="1" t="s">
+      <c r="C17" s="85" t="s">
         <v>427</v>
       </c>
-      <c r="D17" s="1" t="s">
+      <c r="D17" s="85" t="s">
         <v>428</v>
       </c>
-      <c r="E17" s="1" t="s">
+      <c r="E17" s="85" t="s">
         <v>429</v>
       </c>
-      <c r="F17" s="1" t="s">
+      <c r="F17" s="85" t="s">
         <v>430</v>
       </c>
-      <c r="G17" s="1" t="s">
+      <c r="G17" s="85" t="s">
         <v>431</v>
       </c>
-      <c r="H17" s="1" t="s">
+      <c r="H17" s="85" t="s">
         <v>432</v>
       </c>
-      <c r="I17" s="1" t="s">
+      <c r="I17" s="85" t="s">
         <v>433</v>
       </c>
-      <c r="J17" s="1" t="s">
+      <c r="J17" s="85" t="s">
         <v>434</v>
       </c>
-      <c r="K17" s="1" t="s">
+      <c r="K17" s="85" t="s">
         <v>435</v>
       </c>
-      <c r="L17" s="1" t="s">
+      <c r="L17" s="85" t="s">
         <v>436</v>
       </c>
     </row>
@@ -4682,34 +4722,34 @@
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="1" t="s">
+      <c r="C19" s="85" t="s">
         <v>437</v>
       </c>
-      <c r="D19" s="1" t="s">
+      <c r="D19" s="85" t="s">
         <v>438</v>
       </c>
-      <c r="E19" s="1" t="s">
+      <c r="E19" s="85" t="s">
         <v>439</v>
       </c>
-      <c r="F19" s="1" t="s">
+      <c r="F19" s="85" t="s">
         <v>440</v>
       </c>
-      <c r="G19" s="1" t="s">
+      <c r="G19" s="85" t="s">
         <v>441</v>
       </c>
-      <c r="H19" s="1" t="s">
+      <c r="H19" s="85" t="s">
         <v>442</v>
       </c>
-      <c r="I19" s="1" t="s">
+      <c r="I19" s="85" t="s">
         <v>443</v>
       </c>
-      <c r="J19" s="1" t="s">
+      <c r="J19" s="85" t="s">
         <v>444</v>
       </c>
-      <c r="K19" s="1" t="s">
+      <c r="K19" s="85" t="s">
         <v>445</v>
       </c>
-      <c r="L19" s="1" t="s">
+      <c r="L19" s="85" t="s">
         <v>446</v>
       </c>
     </row>
@@ -4717,199 +4757,207 @@
       <c r="B20" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C20" s="1" t="s">
+      <c r="C20" s="85" t="s">
         <v>447</v>
       </c>
-      <c r="D20" s="1" t="s">
+      <c r="D20" s="85" t="s">
         <v>448</v>
       </c>
-      <c r="E20" s="1" t="s">
+      <c r="E20" s="85" t="s">
         <v>449</v>
       </c>
-      <c r="F20" s="1" t="s">
+      <c r="F20" s="85" t="s">
         <v>450</v>
       </c>
-      <c r="G20" s="1" t="s">
+      <c r="G20" s="85" t="s">
         <v>451</v>
       </c>
-      <c r="H20" s="1" t="s">
+      <c r="H20" s="85" t="s">
         <v>452</v>
       </c>
-      <c r="I20" s="1" t="s">
+      <c r="I20" s="85" t="s">
         <v>453</v>
       </c>
-      <c r="J20" s="1" t="s">
+      <c r="J20" s="85" t="s">
         <v>454</v>
       </c>
-      <c r="K20" s="1" t="s">
+      <c r="K20" s="85" t="s">
         <v>455</v>
       </c>
-      <c r="L20" s="1" t="s">
+      <c r="L20" s="85" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="D22" s="22"/>
-      <c r="F22" s="80" t="s">
+      <c r="D22" s="21"/>
+      <c r="F22" s="69" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="81"/>
-      <c r="H22" s="82"/>
-      <c r="I22" s="9"/>
-      <c r="J22" s="80" t="s">
+      <c r="G22" s="70"/>
+      <c r="H22" s="71"/>
+      <c r="I22" s="8"/>
+      <c r="J22" s="69" t="s">
         <v>58</v>
       </c>
-      <c r="K22" s="85"/>
-      <c r="L22" s="86"/>
+      <c r="K22" s="74"/>
+      <c r="L22" s="75"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F23" s="18" t="s">
+      <c r="F23" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="G23" s="21"/>
-      <c r="H23" s="94" t="s">
+      <c r="G23" s="20"/>
+      <c r="H23" s="95" t="s">
         <v>457</v>
       </c>
-      <c r="I23" s="9"/>
-      <c r="J23" s="18" t="s">
+      <c r="I23" s="8"/>
+      <c r="J23" s="17" t="s">
         <v>68</v>
       </c>
-      <c r="K23" s="17"/>
-      <c r="L23" s="94" t="s">
+      <c r="K23" s="16"/>
+      <c r="L23" s="95" t="s">
         <v>462</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F24" s="18" t="s">
+      <c r="F24" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="G24" s="21"/>
-      <c r="H24" s="94" t="s">
+      <c r="G24" s="20"/>
+      <c r="H24" s="95" t="s">
         <v>458</v>
       </c>
-      <c r="I24" s="9"/>
-      <c r="J24" s="18" t="s">
+      <c r="I24" s="8"/>
+      <c r="J24" s="17" t="s">
         <v>67</v>
       </c>
-      <c r="K24" s="17"/>
-      <c r="L24" s="94" t="s">
+      <c r="K24" s="16"/>
+      <c r="L24" s="95" t="s">
         <v>463</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F25" s="18" t="s">
+      <c r="F25" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="G25" s="21"/>
-      <c r="H25" s="94" t="s">
+      <c r="G25" s="20"/>
+      <c r="H25" s="95" t="s">
         <v>459</v>
       </c>
-      <c r="I25" s="9"/>
-      <c r="J25" s="18" t="s">
+      <c r="I25" s="8"/>
+      <c r="J25" s="17" t="s">
         <v>66</v>
       </c>
-      <c r="K25" s="17"/>
-      <c r="L25" s="94" t="s">
+      <c r="K25" s="16"/>
+      <c r="L25" s="95" t="s">
         <v>464</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F26" s="20" t="s">
+      <c r="F26" s="19" t="s">
         <v>65</v>
       </c>
-      <c r="G26" s="19"/>
-      <c r="H26" s="94" t="s">
+      <c r="G26" s="18"/>
+      <c r="H26" s="95" t="s">
         <v>460</v>
       </c>
-      <c r="I26" s="9"/>
-      <c r="J26" s="18" t="s">
+      <c r="I26" s="8"/>
+      <c r="J26" s="17" t="s">
         <v>65</v>
       </c>
-      <c r="K26" s="17"/>
-      <c r="L26" s="94" t="s">
+      <c r="K26" s="16"/>
+      <c r="L26" s="95" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F27" s="83" t="s">
+      <c r="F27" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="84"/>
+      <c r="G27" s="73"/>
       <c r="H27" s="95" t="s">
         <v>461</v>
       </c>
-      <c r="I27" s="9"/>
-      <c r="J27" s="83" t="s">
+      <c r="I27" s="8"/>
+      <c r="J27" s="72" t="s">
         <v>64</v>
       </c>
-      <c r="K27" s="87"/>
-      <c r="L27" s="94" t="s">
+      <c r="K27" s="76"/>
+      <c r="L27" s="95" t="s">
         <v>466</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F28" s="12"/>
-      <c r="G28" s="16" t="s">
+      <c r="F28" s="11"/>
+      <c r="G28" s="15" t="s">
         <v>63</v>
       </c>
-      <c r="H28" s="15" t="s">
+      <c r="H28" s="14" t="s">
         <v>62</v>
       </c>
-      <c r="I28" s="9"/>
-      <c r="J28" s="9"/>
-      <c r="K28" s="14" t="s">
+      <c r="I28" s="8"/>
+      <c r="J28" s="8"/>
+      <c r="K28" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="L28" s="13" t="s">
+      <c r="L28" s="12" t="s">
         <v>62</v>
       </c>
     </row>
     <row r="29" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F29" s="12"/>
-      <c r="G29" s="11" t="s">
+      <c r="F29" s="11"/>
+      <c r="G29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="H29" s="11" t="s">
+      <c r="H29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="I29" s="9"/>
-      <c r="J29" s="9"/>
-      <c r="K29" s="11" t="s">
+      <c r="I29" s="8"/>
+      <c r="J29" s="8"/>
+      <c r="K29" s="10" t="s">
         <v>61</v>
       </c>
-      <c r="L29" s="11" t="s">
+      <c r="L29" s="10" t="s">
         <v>61</v>
       </c>
     </row>
     <row r="30" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F30" s="12"/>
-      <c r="G30" s="11" t="s">
+      <c r="F30" s="11"/>
+      <c r="G30" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="H30" s="11" t="s">
+      <c r="H30" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="I30" s="9"/>
-      <c r="J30" s="9"/>
-      <c r="K30" s="11" t="s">
+      <c r="I30" s="8"/>
+      <c r="J30" s="8"/>
+      <c r="K30" s="10" t="s">
         <v>60</v>
       </c>
-      <c r="L30" s="11" t="s">
+      <c r="L30" s="10" t="s">
         <v>60</v>
       </c>
     </row>
     <row r="31" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F31" s="10" t="s">
+      <c r="F31" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="7"/>
-      <c r="H31" s="7"/>
-      <c r="I31" s="9"/>
-      <c r="J31" s="8" t="s">
+      <c r="G31" s="96" t="s">
+        <v>467</v>
+      </c>
+      <c r="H31" s="96" t="s">
+        <v>468</v>
+      </c>
+      <c r="I31" s="8"/>
+      <c r="J31" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K31" s="7"/>
-      <c r="L31" s="7"/>
+      <c r="K31" s="96" t="s">
+        <v>469</v>
+      </c>
+      <c r="L31" s="96" t="s">
+        <v>470</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="10">

</xml_diff>

<commit_message>
Se realizaron cambios de reporte quincenal
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ResumenBalanceEnergLIV.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ResumenBalanceEnergLIV.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\quincenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17ADFBC3-1FEB-4795-BF66-43DC224C210B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6F9FE8-4890-4F62-825F-78882D6BEA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -19,7 +19,7 @@
   <definedNames>
     <definedName name="dataResult">'Balance Ener'!$B$8:$AB$9</definedName>
     <definedName name="dataResult2">LGN!$B$8:$L$9</definedName>
-    <definedName name="dataResultGNA">'Balance Ener'!$B$27:$W$28</definedName>
+    <definedName name="dataResultGNA">'Balance Ener'!$B$25:$W$26</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -77,7 +77,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="646" uniqueCount="471">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="653" uniqueCount="475">
   <si>
     <t>LOTE IV</t>
   </si>
@@ -1495,6 +1495,18 @@
   </si>
   <si>
     <t>{{dataResultResumen.EnergiaMMBTUQ2CGN}}</t>
+  </si>
+  <si>
+    <t>GNS</t>
+  </si>
+  <si>
+    <t>2da Quincena</t>
+  </si>
+  <si>
+    <t>{{GNSEnergia1Q}}</t>
+  </si>
+  <si>
+    <t>{{GNSEnergia2Q}}</t>
   </si>
 </sst>
 </file>
@@ -1504,9 +1516,9 @@
   <numFmts count="3">
     <numFmt numFmtId="164" formatCode="0.0000"/>
     <numFmt numFmtId="165" formatCode="[$-280A]dddd\ d&quot; de &quot;mmmm&quot; de &quot;yyyy;@"/>
-    <numFmt numFmtId="167" formatCode="#,##0.0000"/>
+    <numFmt numFmtId="166" formatCode="#,##0.0000"/>
   </numFmts>
-  <fonts count="18" x14ac:knownFonts="1">
+  <fonts count="27" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1534,13 +1546,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="0"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -1620,21 +1625,94 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
-      <sz val="11"/>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <u/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FFFF0000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="21">
+  <fills count="23">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1753,6 +1831,18 @@
       <patternFill patternType="solid">
         <fgColor rgb="FF92D050"/>
         <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor rgb="FFFFFF00"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor rgb="FF92D050"/>
       </patternFill>
     </fill>
   </fills>
@@ -2024,9 +2114,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="165" fontId="8" fillId="0" borderId="0"/>
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="97">
+  <cellXfs count="115">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2044,248 +2134,290 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="5" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="7" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="6" fillId="6" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="5" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="8" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="5" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="20" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="166" fontId="16" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="19" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="166" fontId="15" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="16" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="17" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="22" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="166" fontId="23" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="24" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="25" fillId="21" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="26" fillId="22" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="164" fontId="25" fillId="4" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="9" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="13" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="3" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="4" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="18" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="167" fontId="3" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="1" fillId="19" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="13" fillId="20" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="17" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="167" fontId="9" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="167" fontId="6" fillId="4" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2580,10 +2712,10 @@
   <sheetPr>
     <tabColor rgb="FFFFC000"/>
   </sheetPr>
-  <dimension ref="B1:AB42"/>
+  <dimension ref="B1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E2"/>
+    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AE11" sqref="AE11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2592,1736 +2724,2133 @@
     <col min="3" max="3" width="12.28515625" customWidth="1"/>
     <col min="4" max="4" width="16.28515625" customWidth="1"/>
     <col min="5" max="28" width="14.7109375" customWidth="1"/>
+    <col min="30" max="30" width="11.5703125" customWidth="1"/>
+    <col min="31" max="31" width="14.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:28" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="37" t="s">
+    <row r="1" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="2" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="67" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="37"/>
-      <c r="D2" s="37"/>
-      <c r="E2" s="37"/>
-      <c r="F2" s="4" t="s">
+      <c r="C2" s="67"/>
+      <c r="D2" s="67"/>
+      <c r="E2" s="67"/>
+      <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="25" t="s">
+      <c r="G2" s="29" t="s">
         <v>53</v>
       </c>
-      <c r="H2" s="26" t="s">
+      <c r="H2" s="30" t="s">
         <v>54</v>
       </c>
-    </row>
-    <row r="4" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="I2" s="31"/>
+      <c r="J2" s="31"/>
+      <c r="K2" s="31"/>
+      <c r="L2" s="31"/>
+      <c r="M2" s="31"/>
+      <c r="N2" s="31"/>
+      <c r="O2" s="31"/>
+      <c r="P2" s="31"/>
+      <c r="Q2" s="31"/>
+      <c r="R2" s="31"/>
+      <c r="S2" s="31"/>
+      <c r="T2" s="31"/>
+      <c r="U2" s="31"/>
+      <c r="V2" s="31"/>
+      <c r="W2" s="31"/>
+      <c r="X2" s="31"/>
+      <c r="Y2" s="31"/>
+      <c r="Z2" s="31"/>
+      <c r="AA2" s="31"/>
+      <c r="AB2" s="31"/>
+    </row>
+    <row r="3" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B3" s="31"/>
+      <c r="C3" s="31"/>
+      <c r="D3" s="31"/>
+      <c r="E3" s="31"/>
+      <c r="F3" s="31"/>
+      <c r="G3" s="31"/>
+      <c r="H3" s="31"/>
+      <c r="I3" s="31"/>
+      <c r="J3" s="31"/>
+      <c r="K3" s="31"/>
+      <c r="L3" s="31"/>
+      <c r="M3" s="31"/>
+      <c r="N3" s="31"/>
+      <c r="O3" s="31"/>
+      <c r="P3" s="31"/>
+      <c r="Q3" s="31"/>
+      <c r="R3" s="31"/>
+      <c r="S3" s="31"/>
+      <c r="T3" s="31"/>
+      <c r="U3" s="31"/>
+      <c r="V3" s="31"/>
+      <c r="W3" s="31"/>
+      <c r="X3" s="31"/>
+      <c r="Y3" s="31"/>
+      <c r="Z3" s="31"/>
+      <c r="AA3" s="31"/>
+      <c r="AB3" s="31"/>
+    </row>
+    <row r="4" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B4" s="72" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
-      <c r="M4" s="36"/>
-      <c r="N4" s="36"/>
-      <c r="O4" s="36"/>
-      <c r="P4" s="36"/>
-      <c r="Q4" s="36"/>
-      <c r="R4" s="36"/>
-      <c r="S4" s="36"/>
-      <c r="T4" s="36"/>
-      <c r="U4" s="36"/>
-      <c r="V4" s="36"/>
-      <c r="W4" s="36"/>
-      <c r="X4" s="36"/>
-      <c r="Y4" s="36"/>
-      <c r="Z4" s="36"/>
-      <c r="AA4" s="36"/>
-      <c r="AB4" s="36"/>
-    </row>
-    <row r="6" spans="2:28" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="C4" s="72"/>
+      <c r="D4" s="72"/>
+      <c r="E4" s="72"/>
+      <c r="F4" s="72"/>
+      <c r="G4" s="72"/>
+      <c r="H4" s="72"/>
+      <c r="I4" s="72"/>
+      <c r="J4" s="72"/>
+      <c r="K4" s="72"/>
+      <c r="L4" s="72"/>
+      <c r="M4" s="72"/>
+      <c r="N4" s="72"/>
+      <c r="O4" s="72"/>
+      <c r="P4" s="72"/>
+      <c r="Q4" s="72"/>
+      <c r="R4" s="72"/>
+      <c r="S4" s="72"/>
+      <c r="T4" s="72"/>
+      <c r="U4" s="72"/>
+      <c r="V4" s="72"/>
+      <c r="W4" s="72"/>
+      <c r="X4" s="72"/>
+      <c r="Y4" s="72"/>
+      <c r="Z4" s="72"/>
+      <c r="AA4" s="72"/>
+      <c r="AB4" s="72"/>
+    </row>
+    <row r="5" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B5" s="31"/>
+      <c r="C5" s="31"/>
+      <c r="D5" s="31"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="31"/>
+      <c r="H5" s="31"/>
+      <c r="I5" s="31"/>
+      <c r="J5" s="31"/>
+      <c r="K5" s="31"/>
+      <c r="L5" s="31"/>
+      <c r="M5" s="31"/>
+      <c r="N5" s="31"/>
+      <c r="O5" s="31"/>
+      <c r="P5" s="31"/>
+      <c r="Q5" s="31"/>
+      <c r="R5" s="31"/>
+      <c r="S5" s="31"/>
+      <c r="T5" s="31"/>
+      <c r="U5" s="31"/>
+      <c r="V5" s="31"/>
+      <c r="W5" s="31"/>
+      <c r="X5" s="31"/>
+      <c r="Y5" s="31"/>
+      <c r="Z5" s="31"/>
+      <c r="AA5" s="31"/>
+      <c r="AB5" s="31"/>
+    </row>
+    <row r="6" spans="2:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="73" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="43"/>
-      <c r="D6" s="44"/>
-      <c r="E6" s="38" t="s">
+      <c r="C6" s="74"/>
+      <c r="D6" s="75"/>
+      <c r="E6" s="68" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="38"/>
-      <c r="G6" s="38"/>
-      <c r="H6" s="48" t="s">
+      <c r="F6" s="68"/>
+      <c r="G6" s="68"/>
+      <c r="H6" s="79" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="48"/>
-      <c r="J6" s="48"/>
-      <c r="K6" s="56" t="s">
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="87" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="57"/>
-      <c r="M6" s="57"/>
-      <c r="N6" s="58" t="s">
+      <c r="L6" s="88"/>
+      <c r="M6" s="88"/>
+      <c r="N6" s="89" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="59"/>
-      <c r="P6" s="59"/>
-      <c r="Q6" s="52" t="s">
+      <c r="O6" s="90"/>
+      <c r="P6" s="90"/>
+      <c r="Q6" s="83" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="53"/>
-      <c r="S6" s="53"/>
-      <c r="T6" s="54" t="s">
+      <c r="R6" s="84"/>
+      <c r="S6" s="84"/>
+      <c r="T6" s="85" t="s">
         <v>12</v>
       </c>
-      <c r="U6" s="55"/>
-      <c r="V6" s="55"/>
-      <c r="W6" s="49" t="s">
+      <c r="U6" s="86"/>
+      <c r="V6" s="86"/>
+      <c r="W6" s="80" t="s">
         <v>13</v>
       </c>
-      <c r="X6" s="50"/>
-      <c r="Y6" s="51"/>
-      <c r="Z6" s="39" t="s">
+      <c r="X6" s="81"/>
+      <c r="Y6" s="82"/>
+      <c r="Z6" s="69" t="s">
         <v>14</v>
       </c>
-      <c r="AA6" s="40"/>
-      <c r="AB6" s="41"/>
-    </row>
-    <row r="7" spans="2:28" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
-      <c r="C7" s="46"/>
-      <c r="D7" s="47"/>
-      <c r="E7" s="22" t="s">
+      <c r="AA6" s="70"/>
+      <c r="AB6" s="71"/>
+      <c r="AD6" s="50"/>
+      <c r="AE6" s="50" t="s">
+        <v>471</v>
+      </c>
+    </row>
+    <row r="7" spans="2:31" s="3" customFormat="1" ht="39" x14ac:dyDescent="0.25">
+      <c r="B7" s="76"/>
+      <c r="C7" s="77"/>
+      <c r="D7" s="78"/>
+      <c r="E7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G7" s="22" t="s">
+      <c r="G7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="22" t="s">
+      <c r="H7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I7" s="22" t="s">
+      <c r="I7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J7" s="22" t="s">
+      <c r="J7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K7" s="23" t="s">
+      <c r="K7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="L7" s="23" t="s">
+      <c r="L7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="M7" s="23" t="s">
+      <c r="M7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="N7" s="23" t="s">
+      <c r="N7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="O7" s="23" t="s">
+      <c r="O7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="P7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="Q7" s="23" t="s">
+      <c r="Q7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="R7" s="23" t="s">
+      <c r="R7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="S7" s="23" t="s">
+      <c r="S7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="T7" s="23" t="s">
+      <c r="T7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="U7" s="23" t="s">
+      <c r="U7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="V7" s="23" t="s">
+      <c r="V7" s="33" t="s">
         <v>7</v>
       </c>
-      <c r="W7" s="23" t="s">
+      <c r="W7" s="33" t="s">
         <v>5</v>
       </c>
-      <c r="X7" s="23" t="s">
+      <c r="X7" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="Y7" s="22" t="s">
+      <c r="Y7" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="Z7" s="22" t="s">
+      <c r="Z7" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AA7" s="22" t="s">
+      <c r="AA7" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AB7" s="22" t="s">
+      <c r="AB7" s="32" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B8" s="31" t="s">
+      <c r="AD7" s="50"/>
+      <c r="AE7" s="56" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="8" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B8" s="92" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="32"/>
-      <c r="D8" s="33"/>
-      <c r="E8" s="82" t="s">
+      <c r="C8" s="93"/>
+      <c r="D8" s="94"/>
+      <c r="E8" s="34" t="s">
         <v>30</v>
       </c>
-      <c r="F8" s="83" t="s">
+      <c r="F8" s="35" t="s">
         <v>31</v>
       </c>
-      <c r="G8" s="83" t="s">
+      <c r="G8" s="35" t="s">
         <v>32</v>
       </c>
-      <c r="H8" s="83" t="s">
+      <c r="H8" s="35" t="s">
         <v>33</v>
       </c>
-      <c r="I8" s="83" t="s">
+      <c r="I8" s="35" t="s">
         <v>34</v>
       </c>
-      <c r="J8" s="83" t="s">
+      <c r="J8" s="35" t="s">
         <v>35</v>
       </c>
-      <c r="K8" s="83" t="s">
+      <c r="K8" s="35" t="s">
         <v>36</v>
       </c>
-      <c r="L8" s="83" t="s">
+      <c r="L8" s="35" t="s">
         <v>37</v>
       </c>
-      <c r="M8" s="83" t="s">
+      <c r="M8" s="35" t="s">
         <v>38</v>
       </c>
-      <c r="N8" s="83" t="s">
+      <c r="N8" s="35" t="s">
         <v>39</v>
       </c>
-      <c r="O8" s="83" t="s">
+      <c r="O8" s="35" t="s">
         <v>40</v>
       </c>
-      <c r="P8" s="83" t="s">
+      <c r="P8" s="35" t="s">
         <v>41</v>
       </c>
-      <c r="Q8" s="83" t="s">
+      <c r="Q8" s="35" t="s">
         <v>42</v>
       </c>
-      <c r="R8" s="83" t="s">
+      <c r="R8" s="35" t="s">
         <v>43</v>
       </c>
-      <c r="S8" s="83" t="s">
+      <c r="S8" s="35" t="s">
         <v>44</v>
       </c>
-      <c r="T8" s="83" t="s">
+      <c r="T8" s="35" t="s">
         <v>45</v>
       </c>
-      <c r="U8" s="83" t="s">
+      <c r="U8" s="35" t="s">
         <v>46</v>
       </c>
-      <c r="V8" s="83" t="s">
+      <c r="V8" s="35" t="s">
         <v>57</v>
       </c>
-      <c r="W8" s="83" t="s">
+      <c r="W8" s="35" t="s">
         <v>47</v>
       </c>
-      <c r="X8" s="83" t="s">
+      <c r="X8" s="35" t="s">
         <v>48</v>
       </c>
-      <c r="Y8" s="83" t="s">
+      <c r="Y8" s="35" t="s">
         <v>49</v>
       </c>
-      <c r="Z8" s="83" t="s">
+      <c r="Z8" s="35" t="s">
         <v>50</v>
       </c>
-      <c r="AA8" s="83" t="s">
+      <c r="AA8" s="35" t="s">
         <v>51</v>
       </c>
-      <c r="AB8" s="83" t="s">
+      <c r="AB8" s="35" t="s">
         <v>52</v>
       </c>
-    </row>
-    <row r="9" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B9" s="31"/>
-      <c r="C9" s="32"/>
-      <c r="D9" s="33"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
-      <c r="M9" s="85"/>
-      <c r="N9" s="85"/>
-      <c r="O9" s="85"/>
-      <c r="P9" s="85"/>
-      <c r="Q9" s="85"/>
-      <c r="R9" s="85"/>
-      <c r="S9" s="85"/>
-      <c r="T9" s="85"/>
-      <c r="U9" s="85"/>
-      <c r="V9" s="85"/>
-      <c r="W9" s="85"/>
-      <c r="X9" s="85"/>
-      <c r="Y9" s="85"/>
-      <c r="Z9" s="85"/>
-      <c r="AA9" s="85"/>
-      <c r="AB9" s="85"/>
-    </row>
-    <row r="12" spans="2:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="B12" s="34" t="s">
+      <c r="AD8" s="50"/>
+      <c r="AE8" s="55" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="9" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B9" s="92"/>
+      <c r="C9" s="93"/>
+      <c r="D9" s="94"/>
+      <c r="E9" s="36"/>
+      <c r="F9" s="37"/>
+      <c r="G9" s="37"/>
+      <c r="H9" s="37"/>
+      <c r="I9" s="37"/>
+      <c r="J9" s="37"/>
+      <c r="K9" s="37"/>
+      <c r="L9" s="37"/>
+      <c r="M9" s="37"/>
+      <c r="N9" s="37"/>
+      <c r="O9" s="37"/>
+      <c r="P9" s="37"/>
+      <c r="Q9" s="37"/>
+      <c r="R9" s="37"/>
+      <c r="S9" s="37"/>
+      <c r="T9" s="37"/>
+      <c r="U9" s="37"/>
+      <c r="V9" s="37"/>
+      <c r="W9" s="37"/>
+      <c r="X9" s="37"/>
+      <c r="Y9" s="37"/>
+      <c r="Z9" s="37"/>
+      <c r="AA9" s="37"/>
+      <c r="AB9" s="37"/>
+      <c r="AD9" s="51" t="s">
+        <v>59</v>
+      </c>
+      <c r="AE9" s="52" t="s">
+        <v>473</v>
+      </c>
+    </row>
+    <row r="10" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
+      <c r="E10" s="31"/>
+      <c r="F10" s="31"/>
+      <c r="G10" s="31"/>
+      <c r="H10" s="31"/>
+      <c r="I10" s="31"/>
+      <c r="J10" s="31"/>
+      <c r="K10" s="31"/>
+      <c r="L10" s="31"/>
+      <c r="M10" s="31"/>
+      <c r="N10" s="31"/>
+      <c r="O10" s="31"/>
+      <c r="P10" s="31"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="31"/>
+      <c r="S10" s="31"/>
+      <c r="T10" s="31"/>
+      <c r="U10" s="31"/>
+      <c r="V10" s="31"/>
+      <c r="W10" s="31"/>
+      <c r="X10" s="31"/>
+      <c r="Y10" s="31"/>
+      <c r="Z10" s="31"/>
+      <c r="AA10" s="31"/>
+      <c r="AB10" s="31"/>
+      <c r="AD10" s="53" t="s">
+        <v>472</v>
+      </c>
+      <c r="AE10" s="54" t="s">
+        <v>474</v>
+      </c>
+    </row>
+    <row r="11" spans="2:31" ht="39" x14ac:dyDescent="0.25">
+      <c r="B11" s="95" t="s">
         <v>155</v>
       </c>
-      <c r="C12" s="34"/>
-      <c r="D12" s="34"/>
-      <c r="E12" s="22" t="s">
+      <c r="C11" s="95"/>
+      <c r="D11" s="95"/>
+      <c r="E11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F12" s="22" t="s">
+      <c r="F11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G12" s="22" t="s">
+      <c r="G11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H12" s="22" t="s">
+      <c r="H11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I12" s="22" t="s">
+      <c r="I11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J12" s="22" t="s">
+      <c r="J11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K12" s="22" t="s">
+      <c r="K11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L12" s="22" t="s">
+      <c r="L11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M12" s="22" t="s">
+      <c r="M11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N12" s="22" t="s">
+      <c r="N11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="O12" s="22" t="s">
+      <c r="O11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="P12" s="22" t="s">
+      <c r="P11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="Q12" s="22" t="s">
+      <c r="Q11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="R12" s="22" t="s">
+      <c r="R11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="S12" s="22" t="s">
+      <c r="S11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="T12" s="22" t="s">
+      <c r="T11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="U12" s="22" t="s">
+      <c r="U11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="V12" s="22" t="s">
+      <c r="V11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="W12" s="22" t="s">
+      <c r="W11" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="X12" s="22" t="s">
+      <c r="X11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="Y12" s="22" t="s">
+      <c r="Y11" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="Z12" s="24" t="s">
+      <c r="Z11" s="38" t="s">
         <v>5</v>
       </c>
-      <c r="AA12" s="22" t="s">
+      <c r="AA11" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AB12" s="22" t="s">
+      <c r="AB11" s="32" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="13" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B13" s="35" t="s">
+    <row r="12" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B12" s="96" t="s">
         <v>55</v>
       </c>
-      <c r="C13" s="35"/>
-      <c r="D13" s="35"/>
-      <c r="E13" s="83" t="s">
+      <c r="C12" s="96"/>
+      <c r="D12" s="96"/>
+      <c r="E12" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="F13" s="83" t="s">
+      <c r="F12" s="35" t="s">
         <v>108</v>
       </c>
-      <c r="G13" s="86" t="s">
+      <c r="G12" s="39" t="s">
         <v>109</v>
       </c>
-      <c r="H13" s="83" t="s">
+      <c r="H12" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I13" s="83" t="s">
+      <c r="I12" s="35" t="s">
         <v>111</v>
       </c>
-      <c r="J13" s="86" t="s">
+      <c r="J12" s="39" t="s">
         <v>112</v>
       </c>
-      <c r="K13" s="83" t="s">
+      <c r="K12" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="L13" s="83" t="s">
+      <c r="L12" s="35" t="s">
         <v>114</v>
       </c>
-      <c r="M13" s="86" t="s">
+      <c r="M12" s="39" t="s">
         <v>115</v>
       </c>
-      <c r="N13" s="83" t="s">
+      <c r="N12" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="O13" s="83" t="s">
+      <c r="O12" s="35" t="s">
         <v>117</v>
       </c>
-      <c r="P13" s="86" t="s">
+      <c r="P12" s="39" t="s">
         <v>118</v>
       </c>
-      <c r="Q13" s="83" t="s">
+      <c r="Q12" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="R13" s="83" t="s">
+      <c r="R12" s="35" t="s">
         <v>120</v>
       </c>
-      <c r="S13" s="86" t="s">
+      <c r="S12" s="39" t="s">
         <v>121</v>
       </c>
-      <c r="T13" s="83" t="s">
+      <c r="T12" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="U13" s="83" t="s">
+      <c r="U12" s="35" t="s">
         <v>123</v>
       </c>
-      <c r="V13" s="86" t="s">
+      <c r="V12" s="39" t="s">
         <v>124</v>
       </c>
-      <c r="W13" s="83" t="s">
+      <c r="W12" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="X13" s="83" t="s">
+      <c r="X12" s="35" t="s">
         <v>126</v>
       </c>
-      <c r="Y13" s="86" t="s">
+      <c r="Y12" s="39" t="s">
         <v>127</v>
       </c>
-      <c r="Z13" s="83" t="s">
+      <c r="Z12" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="AA13" s="83" t="s">
+      <c r="AA12" s="35" t="s">
         <v>129</v>
       </c>
-      <c r="AB13" s="86" t="s">
+      <c r="AB12" s="39" t="s">
         <v>130</v>
       </c>
     </row>
-    <row r="14" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B14" s="35" t="s">
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B13" s="96" t="s">
         <v>56</v>
       </c>
-      <c r="C14" s="35"/>
-      <c r="D14" s="35"/>
-      <c r="E14" s="83" t="s">
+      <c r="C13" s="96"/>
+      <c r="D13" s="96"/>
+      <c r="E13" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="F14" s="83" t="s">
+      <c r="F13" s="35" t="s">
         <v>132</v>
       </c>
-      <c r="G14" s="86" t="s">
+      <c r="G13" s="39" t="s">
         <v>133</v>
       </c>
-      <c r="H14" s="83" t="s">
+      <c r="H13" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="I14" s="83" t="s">
+      <c r="I13" s="35" t="s">
         <v>135</v>
       </c>
-      <c r="J14" s="86" t="s">
+      <c r="J13" s="39" t="s">
         <v>136</v>
       </c>
-      <c r="K14" s="83" t="s">
+      <c r="K13" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="L14" s="83" t="s">
+      <c r="L13" s="35" t="s">
         <v>138</v>
       </c>
-      <c r="M14" s="86" t="s">
+      <c r="M13" s="39" t="s">
         <v>139</v>
       </c>
-      <c r="N14" s="83" t="s">
+      <c r="N13" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="O14" s="83" t="s">
+      <c r="O13" s="35" t="s">
         <v>141</v>
       </c>
-      <c r="P14" s="86" t="s">
+      <c r="P13" s="39" t="s">
         <v>142</v>
       </c>
-      <c r="Q14" s="83" t="s">
+      <c r="Q13" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="R14" s="83" t="s">
+      <c r="R13" s="35" t="s">
         <v>144</v>
       </c>
-      <c r="S14" s="86" t="s">
+      <c r="S13" s="39" t="s">
         <v>145</v>
       </c>
-      <c r="T14" s="83" t="s">
+      <c r="T13" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="U14" s="83" t="s">
+      <c r="U13" s="35" t="s">
         <v>147</v>
       </c>
-      <c r="V14" s="86" t="s">
+      <c r="V13" s="39" t="s">
         <v>148</v>
       </c>
-      <c r="W14" s="83" t="s">
+      <c r="W13" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="X14" s="83" t="s">
+      <c r="X13" s="35" t="s">
         <v>150</v>
       </c>
-      <c r="Y14" s="86" t="s">
+      <c r="Y13" s="39" t="s">
         <v>151</v>
       </c>
-      <c r="Z14" s="83" t="s">
+      <c r="Z13" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="AA14" s="83" t="s">
+      <c r="AA13" s="35" t="s">
         <v>153</v>
       </c>
-      <c r="AB14" s="86" t="s">
+      <c r="AB13" s="39" t="s">
         <v>154</v>
       </c>
     </row>
-    <row r="15" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="E15" s="87"/>
-      <c r="F15" s="87"/>
-      <c r="G15" s="87"/>
-      <c r="H15" s="87"/>
-      <c r="I15" s="87"/>
-      <c r="J15" s="87"/>
-      <c r="K15" s="87"/>
-      <c r="L15" s="87"/>
-      <c r="M15" s="87"/>
-      <c r="N15" s="87"/>
-      <c r="O15" s="87"/>
-      <c r="P15" s="87"/>
-      <c r="Q15" s="87"/>
-      <c r="R15" s="87"/>
-      <c r="S15" s="87"/>
-      <c r="T15" s="87"/>
-      <c r="U15" s="87"/>
-      <c r="V15" s="87"/>
-      <c r="W15" s="87"/>
-      <c r="X15" s="87"/>
-      <c r="Y15" s="87"/>
-      <c r="Z15" s="87"/>
-      <c r="AA15" s="87"/>
-      <c r="AB15" s="87"/>
-    </row>
-    <row r="16" spans="2:28" ht="45" x14ac:dyDescent="0.25">
-      <c r="B16" s="34" t="s">
+    <row r="14" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B14" s="31"/>
+      <c r="C14" s="31"/>
+      <c r="D14" s="31"/>
+      <c r="E14" s="40"/>
+      <c r="F14" s="40"/>
+      <c r="G14" s="40"/>
+      <c r="H14" s="40"/>
+      <c r="I14" s="40"/>
+      <c r="J14" s="40"/>
+      <c r="K14" s="40"/>
+      <c r="L14" s="40"/>
+      <c r="M14" s="40"/>
+      <c r="N14" s="40"/>
+      <c r="O14" s="40"/>
+      <c r="P14" s="40"/>
+      <c r="Q14" s="40"/>
+      <c r="R14" s="40"/>
+      <c r="S14" s="40"/>
+      <c r="T14" s="40"/>
+      <c r="U14" s="40"/>
+      <c r="V14" s="40"/>
+      <c r="W14" s="40"/>
+      <c r="X14" s="40"/>
+      <c r="Y14" s="40"/>
+      <c r="Z14" s="40"/>
+      <c r="AA14" s="40"/>
+      <c r="AB14" s="40"/>
+    </row>
+    <row r="15" spans="2:31" ht="39" x14ac:dyDescent="0.25">
+      <c r="B15" s="95" t="s">
         <v>16</v>
       </c>
-      <c r="C16" s="34"/>
-      <c r="D16" s="34"/>
-      <c r="E16" s="22" t="s">
+      <c r="C15" s="95"/>
+      <c r="D15" s="95"/>
+      <c r="E15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="22" t="s">
+      <c r="F15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="G16" s="22" t="s">
+      <c r="G15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="H16" s="22" t="s">
+      <c r="H15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="22" t="s">
+      <c r="I15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="22" t="s">
+      <c r="J15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="K16" s="22" t="s">
+      <c r="K15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="L16" s="22" t="s">
+      <c r="L15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="M16" s="22" t="s">
+      <c r="M15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="N16" s="22" t="s">
+      <c r="N15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="O16" s="22" t="s">
+      <c r="O15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="P16" s="22" t="s">
+      <c r="P15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="Q16" s="22" t="s">
+      <c r="Q15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="R16" s="22" t="s">
+      <c r="R15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="S16" s="22" t="s">
+      <c r="S15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="T16" s="22" t="s">
+      <c r="T15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="U16" s="22" t="s">
+      <c r="U15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="V16" s="22" t="s">
+      <c r="V15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="W16" s="22" t="s">
+      <c r="W15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="X16" s="22" t="s">
+      <c r="X15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="Y16" s="22" t="s">
+      <c r="Y15" s="32" t="s">
         <v>7</v>
       </c>
-      <c r="Z16" s="22" t="s">
+      <c r="Z15" s="32" t="s">
         <v>5</v>
       </c>
-      <c r="AA16" s="22" t="s">
+      <c r="AA15" s="32" t="s">
         <v>6</v>
       </c>
-      <c r="AB16" s="22" t="s">
+      <c r="AB15" s="32" t="s">
         <v>7</v>
       </c>
+      <c r="AE15" s="21"/>
+    </row>
+    <row r="16" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B16" s="96" t="s">
+        <v>55</v>
+      </c>
+      <c r="C16" s="96"/>
+      <c r="D16" s="96"/>
+      <c r="E16" s="37" t="s">
+        <v>156</v>
+      </c>
+      <c r="F16" s="37" t="s">
+        <v>157</v>
+      </c>
+      <c r="G16" s="41" t="s">
+        <v>158</v>
+      </c>
+      <c r="H16" s="37" t="s">
+        <v>159</v>
+      </c>
+      <c r="I16" s="37" t="s">
+        <v>160</v>
+      </c>
+      <c r="J16" s="41" t="s">
+        <v>161</v>
+      </c>
+      <c r="K16" s="37" t="s">
+        <v>162</v>
+      </c>
+      <c r="L16" s="37" t="s">
+        <v>163</v>
+      </c>
+      <c r="M16" s="41" t="s">
+        <v>164</v>
+      </c>
+      <c r="N16" s="37" t="s">
+        <v>165</v>
+      </c>
+      <c r="O16" s="37" t="s">
+        <v>166</v>
+      </c>
+      <c r="P16" s="41" t="s">
+        <v>167</v>
+      </c>
+      <c r="Q16" s="37" t="s">
+        <v>168</v>
+      </c>
+      <c r="R16" s="37" t="s">
+        <v>169</v>
+      </c>
+      <c r="S16" s="41" t="s">
+        <v>170</v>
+      </c>
+      <c r="T16" s="37" t="s">
+        <v>171</v>
+      </c>
+      <c r="U16" s="37" t="s">
+        <v>172</v>
+      </c>
+      <c r="V16" s="41" t="s">
+        <v>173</v>
+      </c>
+      <c r="W16" s="37" t="s">
+        <v>174</v>
+      </c>
+      <c r="X16" s="37" t="s">
+        <v>175</v>
+      </c>
+      <c r="Y16" s="41" t="s">
+        <v>176</v>
+      </c>
+      <c r="Z16" s="37" t="s">
+        <v>177</v>
+      </c>
+      <c r="AA16" s="37" t="s">
+        <v>178</v>
+      </c>
+      <c r="AB16" s="41" t="s">
+        <v>179</v>
+      </c>
     </row>
     <row r="17" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B17" s="35" t="s">
+      <c r="B17" s="96" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="96"/>
+      <c r="D17" s="96"/>
+      <c r="E17" s="37" t="s">
+        <v>180</v>
+      </c>
+      <c r="F17" s="37" t="s">
+        <v>181</v>
+      </c>
+      <c r="G17" s="41" t="s">
+        <v>182</v>
+      </c>
+      <c r="H17" s="37" t="s">
+        <v>183</v>
+      </c>
+      <c r="I17" s="37" t="s">
+        <v>184</v>
+      </c>
+      <c r="J17" s="41" t="s">
+        <v>185</v>
+      </c>
+      <c r="K17" s="37" t="s">
+        <v>186</v>
+      </c>
+      <c r="L17" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="M17" s="41" t="s">
+        <v>188</v>
+      </c>
+      <c r="N17" s="37" t="s">
+        <v>189</v>
+      </c>
+      <c r="O17" s="37" t="s">
+        <v>190</v>
+      </c>
+      <c r="P17" s="41" t="s">
+        <v>191</v>
+      </c>
+      <c r="Q17" s="37" t="s">
+        <v>192</v>
+      </c>
+      <c r="R17" s="37" t="s">
+        <v>193</v>
+      </c>
+      <c r="S17" s="41" t="s">
+        <v>194</v>
+      </c>
+      <c r="T17" s="37" t="s">
+        <v>195</v>
+      </c>
+      <c r="U17" s="37" t="s">
+        <v>196</v>
+      </c>
+      <c r="V17" s="41" t="s">
+        <v>197</v>
+      </c>
+      <c r="W17" s="37" t="s">
+        <v>198</v>
+      </c>
+      <c r="X17" s="37" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y17" s="41" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z17" s="37" t="s">
+        <v>201</v>
+      </c>
+      <c r="AA17" s="37" t="s">
+        <v>202</v>
+      </c>
+      <c r="AB17" s="41" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B18" s="31"/>
+      <c r="C18" s="31"/>
+      <c r="D18" s="31"/>
+      <c r="E18" s="31"/>
+      <c r="F18" s="31"/>
+      <c r="G18" s="31"/>
+      <c r="H18" s="31"/>
+      <c r="I18" s="31"/>
+      <c r="J18" s="31"/>
+      <c r="K18" s="31"/>
+      <c r="L18" s="31"/>
+      <c r="M18" s="31"/>
+      <c r="N18" s="31"/>
+      <c r="O18" s="31"/>
+      <c r="P18" s="31"/>
+      <c r="Q18" s="31"/>
+      <c r="R18" s="31"/>
+      <c r="S18" s="31"/>
+      <c r="T18" s="31"/>
+      <c r="U18" s="31"/>
+      <c r="V18" s="31"/>
+      <c r="W18" s="31"/>
+      <c r="X18" s="31"/>
+      <c r="Y18" s="31"/>
+      <c r="Z18" s="31"/>
+      <c r="AA18" s="31"/>
+      <c r="AB18" s="31"/>
+    </row>
+    <row r="19" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B19" s="96" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="96"/>
+      <c r="D19" s="96"/>
+      <c r="E19" s="37" t="s">
+        <v>204</v>
+      </c>
+      <c r="F19" s="37" t="s">
+        <v>205</v>
+      </c>
+      <c r="G19" s="37" t="s">
+        <v>206</v>
+      </c>
+      <c r="H19" s="37" t="s">
+        <v>207</v>
+      </c>
+      <c r="I19" s="37" t="s">
+        <v>208</v>
+      </c>
+      <c r="J19" s="37" t="s">
+        <v>209</v>
+      </c>
+      <c r="K19" s="37" t="s">
+        <v>210</v>
+      </c>
+      <c r="L19" s="37" t="s">
+        <v>211</v>
+      </c>
+      <c r="M19" s="37" t="s">
+        <v>212</v>
+      </c>
+      <c r="N19" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="O19" s="37" t="s">
+        <v>214</v>
+      </c>
+      <c r="P19" s="37" t="s">
+        <v>215</v>
+      </c>
+      <c r="Q19" s="37" t="s">
+        <v>216</v>
+      </c>
+      <c r="R19" s="37" t="s">
+        <v>217</v>
+      </c>
+      <c r="S19" s="37" t="s">
+        <v>218</v>
+      </c>
+      <c r="T19" s="37" t="s">
+        <v>219</v>
+      </c>
+      <c r="U19" s="37" t="s">
+        <v>220</v>
+      </c>
+      <c r="V19" s="37" t="s">
+        <v>221</v>
+      </c>
+      <c r="W19" s="37" t="s">
+        <v>222</v>
+      </c>
+      <c r="X19" s="37" t="s">
+        <v>223</v>
+      </c>
+      <c r="Y19" s="37" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z19" s="37" t="s">
+        <v>225</v>
+      </c>
+      <c r="AA19" s="37" t="s">
+        <v>226</v>
+      </c>
+      <c r="AB19" s="37" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B20" s="96" t="s">
+        <v>228</v>
+      </c>
+      <c r="C20" s="96"/>
+      <c r="D20" s="96"/>
+      <c r="E20" s="37" t="s">
+        <v>229</v>
+      </c>
+      <c r="F20" s="37" t="s">
+        <v>230</v>
+      </c>
+      <c r="G20" s="37" t="s">
+        <v>231</v>
+      </c>
+      <c r="H20" s="37" t="s">
+        <v>232</v>
+      </c>
+      <c r="I20" s="37" t="s">
+        <v>233</v>
+      </c>
+      <c r="J20" s="37" t="s">
+        <v>234</v>
+      </c>
+      <c r="K20" s="37" t="s">
+        <v>235</v>
+      </c>
+      <c r="L20" s="37" t="s">
+        <v>236</v>
+      </c>
+      <c r="M20" s="37" t="s">
+        <v>237</v>
+      </c>
+      <c r="N20" s="37" t="s">
+        <v>238</v>
+      </c>
+      <c r="O20" s="37" t="s">
+        <v>239</v>
+      </c>
+      <c r="P20" s="37" t="s">
+        <v>240</v>
+      </c>
+      <c r="Q20" s="37" t="s">
+        <v>241</v>
+      </c>
+      <c r="R20" s="37" t="s">
+        <v>242</v>
+      </c>
+      <c r="S20" s="37" t="s">
+        <v>243</v>
+      </c>
+      <c r="T20" s="37" t="s">
+        <v>244</v>
+      </c>
+      <c r="U20" s="37" t="s">
+        <v>245</v>
+      </c>
+      <c r="V20" s="37" t="s">
+        <v>246</v>
+      </c>
+      <c r="W20" s="37" t="s">
+        <v>247</v>
+      </c>
+      <c r="X20" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y20" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z20" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="AA20" s="37" t="s">
+        <v>251</v>
+      </c>
+      <c r="AB20" s="37" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B21" s="31"/>
+      <c r="C21" s="31"/>
+      <c r="D21" s="31"/>
+      <c r="E21" s="31"/>
+      <c r="F21" s="31"/>
+      <c r="G21" s="31"/>
+      <c r="H21" s="31"/>
+      <c r="I21" s="31"/>
+      <c r="J21" s="31"/>
+      <c r="K21" s="31"/>
+      <c r="L21" s="31"/>
+      <c r="M21" s="31"/>
+      <c r="N21" s="31"/>
+      <c r="O21" s="31"/>
+      <c r="P21" s="31"/>
+      <c r="Q21" s="31"/>
+      <c r="R21" s="31"/>
+      <c r="S21" s="31"/>
+      <c r="T21" s="31"/>
+      <c r="U21" s="31"/>
+      <c r="V21" s="31"/>
+      <c r="W21" s="31"/>
+      <c r="X21" s="31"/>
+      <c r="Y21" s="31"/>
+      <c r="Z21" s="31"/>
+      <c r="AA21" s="31"/>
+      <c r="AB21" s="31"/>
+    </row>
+    <row r="22" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B22" s="72" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="72"/>
+      <c r="D22" s="72"/>
+      <c r="E22" s="72"/>
+      <c r="F22" s="72"/>
+      <c r="G22" s="72"/>
+      <c r="H22" s="72"/>
+      <c r="I22" s="72"/>
+      <c r="J22" s="72"/>
+      <c r="K22" s="72"/>
+      <c r="L22" s="72"/>
+      <c r="M22" s="72"/>
+      <c r="N22" s="72"/>
+      <c r="O22" s="72"/>
+      <c r="P22" s="72"/>
+      <c r="Q22" s="72"/>
+      <c r="R22" s="72"/>
+      <c r="S22" s="72"/>
+      <c r="T22" s="72"/>
+      <c r="U22" s="72"/>
+      <c r="V22" s="72"/>
+      <c r="W22" s="72"/>
+      <c r="X22" s="72"/>
+      <c r="Y22" s="72"/>
+      <c r="Z22" s="72"/>
+      <c r="AA22" s="72"/>
+      <c r="AB22" s="72"/>
+    </row>
+    <row r="23" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B23" s="31"/>
+      <c r="C23" s="31"/>
+      <c r="D23" s="31"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="31"/>
+      <c r="G23" s="31"/>
+      <c r="H23" s="31"/>
+      <c r="I23" s="31"/>
+      <c r="J23" s="31"/>
+      <c r="K23" s="31"/>
+      <c r="L23" s="31"/>
+      <c r="M23" s="31"/>
+      <c r="N23" s="31"/>
+      <c r="O23" s="31"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="31"/>
+      <c r="R23" s="31"/>
+      <c r="S23" s="31"/>
+      <c r="T23" s="31"/>
+      <c r="U23" s="31"/>
+      <c r="V23" s="31"/>
+      <c r="W23" s="31"/>
+      <c r="X23" s="31"/>
+      <c r="Y23" s="31"/>
+      <c r="Z23" s="31"/>
+      <c r="AA23" s="31"/>
+      <c r="AB23" s="31"/>
+    </row>
+    <row r="24" spans="2:28" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B24" s="61" t="s">
+        <v>17</v>
+      </c>
+      <c r="C24" s="61"/>
+      <c r="D24" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F24" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G24" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H24" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I24" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J24" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K24" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="L24" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="M24" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="N24" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="O24" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="P24" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q24" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="R24" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="S24" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="T24" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="U24" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="V24" s="42" t="s">
+        <v>24</v>
+      </c>
+      <c r="W24" s="42" t="s">
+        <v>25</v>
+      </c>
+      <c r="X24" s="31"/>
+      <c r="Y24" s="31"/>
+      <c r="Z24" s="31"/>
+      <c r="AA24" s="31"/>
+      <c r="AB24" s="31"/>
+    </row>
+    <row r="25" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B25" s="91" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="91"/>
+      <c r="D25" s="35" t="s">
+        <v>87</v>
+      </c>
+      <c r="E25" s="35" t="s">
+        <v>88</v>
+      </c>
+      <c r="F25" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="G25" s="35" t="s">
+        <v>90</v>
+      </c>
+      <c r="H25" s="35" t="s">
+        <v>91</v>
+      </c>
+      <c r="I25" s="35" t="s">
+        <v>92</v>
+      </c>
+      <c r="J25" s="35" t="s">
+        <v>93</v>
+      </c>
+      <c r="K25" s="35" t="s">
+        <v>94</v>
+      </c>
+      <c r="L25" s="35" t="s">
+        <v>95</v>
+      </c>
+      <c r="M25" s="35" t="s">
+        <v>96</v>
+      </c>
+      <c r="N25" s="35" t="s">
+        <v>97</v>
+      </c>
+      <c r="O25" s="35" t="s">
+        <v>98</v>
+      </c>
+      <c r="P25" s="35" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q25" s="35" t="s">
+        <v>100</v>
+      </c>
+      <c r="R25" s="35" t="s">
+        <v>101</v>
+      </c>
+      <c r="S25" s="35" t="s">
+        <v>102</v>
+      </c>
+      <c r="T25" s="35" t="s">
+        <v>103</v>
+      </c>
+      <c r="U25" s="35" t="s">
+        <v>104</v>
+      </c>
+      <c r="V25" s="35" t="s">
+        <v>105</v>
+      </c>
+      <c r="W25" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="X25" s="31"/>
+      <c r="Y25" s="31"/>
+      <c r="Z25" s="31"/>
+      <c r="AA25" s="31"/>
+      <c r="AB25" s="31"/>
+    </row>
+    <row r="26" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B26" s="91"/>
+      <c r="C26" s="91"/>
+      <c r="D26" s="37"/>
+      <c r="E26" s="37"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="37"/>
+      <c r="H26" s="37"/>
+      <c r="I26" s="37"/>
+      <c r="J26" s="37"/>
+      <c r="K26" s="37"/>
+      <c r="L26" s="37"/>
+      <c r="M26" s="37"/>
+      <c r="N26" s="37"/>
+      <c r="O26" s="37"/>
+      <c r="P26" s="37"/>
+      <c r="Q26" s="37"/>
+      <c r="R26" s="37"/>
+      <c r="S26" s="37"/>
+      <c r="T26" s="37"/>
+      <c r="U26" s="37"/>
+      <c r="V26" s="37"/>
+      <c r="W26" s="37"/>
+      <c r="X26" s="31"/>
+      <c r="Y26" s="31"/>
+      <c r="Z26" s="31"/>
+      <c r="AA26" s="31"/>
+      <c r="AB26" s="31"/>
+    </row>
+    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B27" s="31"/>
+      <c r="C27" s="31"/>
+      <c r="D27" s="31"/>
+      <c r="E27" s="31"/>
+      <c r="F27" s="31"/>
+      <c r="G27" s="31"/>
+      <c r="H27" s="31"/>
+      <c r="I27" s="31"/>
+      <c r="J27" s="31"/>
+      <c r="K27" s="31"/>
+      <c r="L27" s="31"/>
+      <c r="M27" s="31"/>
+      <c r="N27" s="31"/>
+      <c r="O27" s="31"/>
+      <c r="P27" s="31"/>
+      <c r="Q27" s="31"/>
+      <c r="R27" s="31"/>
+      <c r="S27" s="31"/>
+      <c r="T27" s="31"/>
+      <c r="U27" s="31"/>
+      <c r="V27" s="31"/>
+      <c r="W27" s="31"/>
+      <c r="X27" s="31"/>
+      <c r="Y27" s="31"/>
+      <c r="Z27" s="31"/>
+      <c r="AA27" s="31"/>
+      <c r="AB27" s="31"/>
+    </row>
+    <row r="28" spans="2:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B28" s="59"/>
+      <c r="C28" s="59"/>
+      <c r="D28" s="43" t="s">
+        <v>18</v>
+      </c>
+      <c r="E28" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F28" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="H28" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="I28" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="J28" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="K28" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="L28" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="M28" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="N28" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="O28" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="P28" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q28" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="R28" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="S28" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="T28" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="U28" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="V28" s="31"/>
+      <c r="W28" s="31"/>
+      <c r="X28" s="31"/>
+      <c r="Y28" s="31"/>
+      <c r="Z28" s="31"/>
+      <c r="AA28" s="31"/>
+      <c r="AB28" s="31"/>
+    </row>
+    <row r="29" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B29" s="60" t="s">
         <v>55</v>
       </c>
-      <c r="C17" s="35"/>
-      <c r="D17" s="35"/>
-      <c r="E17" s="85" t="s">
-        <v>156</v>
-      </c>
-      <c r="F17" s="85" t="s">
-        <v>157</v>
-      </c>
-      <c r="G17" s="88" t="s">
-        <v>158</v>
-      </c>
-      <c r="H17" s="85" t="s">
-        <v>159</v>
-      </c>
-      <c r="I17" s="85" t="s">
-        <v>160</v>
-      </c>
-      <c r="J17" s="88" t="s">
-        <v>161</v>
-      </c>
-      <c r="K17" s="85" t="s">
-        <v>162</v>
-      </c>
-      <c r="L17" s="85" t="s">
-        <v>163</v>
-      </c>
-      <c r="M17" s="88" t="s">
-        <v>164</v>
-      </c>
-      <c r="N17" s="85" t="s">
-        <v>165</v>
-      </c>
-      <c r="O17" s="85" t="s">
-        <v>166</v>
-      </c>
-      <c r="P17" s="88" t="s">
-        <v>167</v>
-      </c>
-      <c r="Q17" s="85" t="s">
-        <v>168</v>
-      </c>
-      <c r="R17" s="85" t="s">
-        <v>169</v>
-      </c>
-      <c r="S17" s="88" t="s">
-        <v>170</v>
-      </c>
-      <c r="T17" s="85" t="s">
-        <v>171</v>
-      </c>
-      <c r="U17" s="85" t="s">
-        <v>172</v>
-      </c>
-      <c r="V17" s="88" t="s">
-        <v>173</v>
-      </c>
-      <c r="W17" s="85" t="s">
-        <v>174</v>
-      </c>
-      <c r="X17" s="85" t="s">
-        <v>175</v>
-      </c>
-      <c r="Y17" s="88" t="s">
-        <v>176</v>
-      </c>
-      <c r="Z17" s="85" t="s">
-        <v>177</v>
-      </c>
-      <c r="AA17" s="85" t="s">
-        <v>178</v>
-      </c>
-      <c r="AB17" s="88" t="s">
-        <v>179</v>
-      </c>
-    </row>
-    <row r="18" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B18" s="35" t="s">
+      <c r="C29" s="60"/>
+      <c r="D29" s="44" t="s">
+        <v>253</v>
+      </c>
+      <c r="E29" s="45" t="s">
+        <v>254</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>255</v>
+      </c>
+      <c r="G29" s="44" t="s">
+        <v>256</v>
+      </c>
+      <c r="H29" s="45" t="s">
+        <v>257</v>
+      </c>
+      <c r="I29" s="44" t="s">
+        <v>258</v>
+      </c>
+      <c r="J29" s="44" t="s">
+        <v>259</v>
+      </c>
+      <c r="K29" s="45" t="s">
+        <v>260</v>
+      </c>
+      <c r="L29" s="44" t="s">
+        <v>261</v>
+      </c>
+      <c r="M29" s="44" t="s">
+        <v>262</v>
+      </c>
+      <c r="N29" s="45" t="s">
+        <v>263</v>
+      </c>
+      <c r="O29" s="44" t="s">
+        <v>264</v>
+      </c>
+      <c r="P29" s="44" t="s">
+        <v>265</v>
+      </c>
+      <c r="Q29" s="45" t="s">
+        <v>266</v>
+      </c>
+      <c r="R29" s="44" t="s">
+        <v>267</v>
+      </c>
+      <c r="S29" s="44" t="s">
+        <v>268</v>
+      </c>
+      <c r="T29" s="45" t="s">
+        <v>269</v>
+      </c>
+      <c r="U29" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="V29" s="31"/>
+      <c r="W29" s="31"/>
+      <c r="X29" s="31"/>
+      <c r="Y29" s="31"/>
+      <c r="Z29" s="31"/>
+      <c r="AA29" s="31"/>
+      <c r="AB29" s="31"/>
+    </row>
+    <row r="30" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B30" s="60" t="s">
         <v>56</v>
       </c>
-      <c r="C18" s="35"/>
-      <c r="D18" s="35"/>
-      <c r="E18" s="85" t="s">
-        <v>180</v>
-      </c>
-      <c r="F18" s="85" t="s">
-        <v>181</v>
-      </c>
-      <c r="G18" s="88" t="s">
-        <v>182</v>
-      </c>
-      <c r="H18" s="85" t="s">
-        <v>183</v>
-      </c>
-      <c r="I18" s="85" t="s">
-        <v>184</v>
-      </c>
-      <c r="J18" s="88" t="s">
-        <v>185</v>
-      </c>
-      <c r="K18" s="85" t="s">
-        <v>186</v>
-      </c>
-      <c r="L18" s="85" t="s">
-        <v>187</v>
-      </c>
-      <c r="M18" s="88" t="s">
-        <v>188</v>
-      </c>
-      <c r="N18" s="85" t="s">
-        <v>189</v>
-      </c>
-      <c r="O18" s="85" t="s">
-        <v>190</v>
-      </c>
-      <c r="P18" s="88" t="s">
-        <v>191</v>
-      </c>
-      <c r="Q18" s="85" t="s">
-        <v>192</v>
-      </c>
-      <c r="R18" s="85" t="s">
-        <v>193</v>
-      </c>
-      <c r="S18" s="88" t="s">
-        <v>194</v>
-      </c>
-      <c r="T18" s="85" t="s">
-        <v>195</v>
-      </c>
-      <c r="U18" s="85" t="s">
-        <v>196</v>
-      </c>
-      <c r="V18" s="88" t="s">
-        <v>197</v>
-      </c>
-      <c r="W18" s="85" t="s">
-        <v>198</v>
-      </c>
-      <c r="X18" s="85" t="s">
-        <v>199</v>
-      </c>
-      <c r="Y18" s="88" t="s">
-        <v>200</v>
-      </c>
-      <c r="Z18" s="85" t="s">
-        <v>201</v>
-      </c>
-      <c r="AA18" s="85" t="s">
-        <v>202</v>
-      </c>
-      <c r="AB18" s="88" t="s">
-        <v>203</v>
-      </c>
-    </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" s="35" t="s">
+      <c r="C30" s="60"/>
+      <c r="D30" s="44" t="s">
+        <v>271</v>
+      </c>
+      <c r="E30" s="45" t="s">
+        <v>272</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>273</v>
+      </c>
+      <c r="G30" s="44" t="s">
+        <v>274</v>
+      </c>
+      <c r="H30" s="45" t="s">
+        <v>275</v>
+      </c>
+      <c r="I30" s="44" t="s">
+        <v>276</v>
+      </c>
+      <c r="J30" s="44" t="s">
+        <v>277</v>
+      </c>
+      <c r="K30" s="45" t="s">
+        <v>278</v>
+      </c>
+      <c r="L30" s="44" t="s">
+        <v>279</v>
+      </c>
+      <c r="M30" s="44" t="s">
+        <v>280</v>
+      </c>
+      <c r="N30" s="45" t="s">
+        <v>281</v>
+      </c>
+      <c r="O30" s="44" t="s">
+        <v>282</v>
+      </c>
+      <c r="P30" s="44" t="s">
+        <v>283</v>
+      </c>
+      <c r="Q30" s="45" t="s">
+        <v>284</v>
+      </c>
+      <c r="R30" s="44" t="s">
+        <v>285</v>
+      </c>
+      <c r="S30" s="44" t="s">
+        <v>286</v>
+      </c>
+      <c r="T30" s="45" t="s">
+        <v>287</v>
+      </c>
+      <c r="U30" s="44" t="s">
+        <v>288</v>
+      </c>
+      <c r="V30" s="31"/>
+      <c r="W30" s="31"/>
+      <c r="X30" s="31"/>
+      <c r="Y30" s="31"/>
+      <c r="Z30" s="31"/>
+      <c r="AA30" s="31"/>
+      <c r="AB30" s="31"/>
+    </row>
+    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B31" s="62" t="s">
+        <v>27</v>
+      </c>
+      <c r="C31" s="62"/>
+      <c r="D31" s="46" t="s">
+        <v>289</v>
+      </c>
+      <c r="E31" s="45" t="s">
+        <v>290</v>
+      </c>
+      <c r="F31" s="46" t="s">
+        <v>291</v>
+      </c>
+      <c r="G31" s="46" t="s">
+        <v>292</v>
+      </c>
+      <c r="H31" s="46" t="s">
+        <v>293</v>
+      </c>
+      <c r="I31" s="46" t="s">
+        <v>294</v>
+      </c>
+      <c r="J31" s="46" t="s">
+        <v>295</v>
+      </c>
+      <c r="K31" s="46" t="s">
+        <v>296</v>
+      </c>
+      <c r="L31" s="46" t="s">
+        <v>297</v>
+      </c>
+      <c r="M31" s="46" t="s">
+        <v>298</v>
+      </c>
+      <c r="N31" s="45" t="s">
+        <v>299</v>
+      </c>
+      <c r="O31" s="46" t="s">
+        <v>300</v>
+      </c>
+      <c r="P31" s="46" t="s">
+        <v>301</v>
+      </c>
+      <c r="Q31" s="45" t="s">
+        <v>302</v>
+      </c>
+      <c r="R31" s="46" t="s">
+        <v>303</v>
+      </c>
+      <c r="S31" s="46" t="s">
+        <v>304</v>
+      </c>
+      <c r="T31" s="45" t="s">
+        <v>305</v>
+      </c>
+      <c r="U31" s="46" t="s">
+        <v>306</v>
+      </c>
+      <c r="V31" s="31"/>
+      <c r="W31" s="31"/>
+      <c r="X31" s="31"/>
+      <c r="Y31" s="31"/>
+      <c r="Z31" s="31"/>
+      <c r="AA31" s="31"/>
+      <c r="AB31" s="31"/>
+    </row>
+    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B32" s="31"/>
+      <c r="C32" s="31"/>
+      <c r="D32" s="31"/>
+      <c r="E32" s="31"/>
+      <c r="F32" s="31"/>
+      <c r="G32" s="31"/>
+      <c r="H32" s="31"/>
+      <c r="I32" s="31"/>
+      <c r="J32" s="31"/>
+      <c r="K32" s="47"/>
+      <c r="L32" s="31"/>
+      <c r="M32" s="31"/>
+      <c r="N32" s="31"/>
+      <c r="O32" s="31"/>
+      <c r="P32" s="31"/>
+      <c r="Q32" s="31"/>
+      <c r="R32" s="31"/>
+      <c r="S32" s="31"/>
+      <c r="T32" s="31"/>
+      <c r="U32" s="31"/>
+      <c r="V32" s="31"/>
+      <c r="W32" s="31"/>
+      <c r="X32" s="31"/>
+      <c r="Y32" s="31"/>
+      <c r="Z32" s="31"/>
+      <c r="AA32" s="31"/>
+      <c r="AB32" s="31"/>
+    </row>
+    <row r="33" spans="2:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B33" s="61"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="G33" s="32"/>
+      <c r="H33" s="32"/>
+      <c r="I33" s="32"/>
+      <c r="J33" s="32"/>
+      <c r="K33" s="32"/>
+      <c r="L33" s="32"/>
+      <c r="M33" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="N33" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="O33" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="P33" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="Q33" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="R33" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="S33" s="32" t="s">
+        <v>23</v>
+      </c>
+      <c r="T33" s="32" t="s">
+        <v>6</v>
+      </c>
+      <c r="U33" s="32" t="s">
+        <v>7</v>
+      </c>
+      <c r="V33" s="31"/>
+      <c r="W33" s="31"/>
+      <c r="X33" s="31"/>
+      <c r="Y33" s="31"/>
+      <c r="Z33" s="31"/>
+      <c r="AA33" s="31"/>
+      <c r="AB33" s="31"/>
+    </row>
+    <row r="34" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B34" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C34" s="60"/>
+      <c r="D34" s="44" t="s">
+        <v>307</v>
+      </c>
+      <c r="E34" s="45" t="s">
+        <v>308</v>
+      </c>
+      <c r="F34" s="44" t="s">
+        <v>309</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>310</v>
+      </c>
+      <c r="H34" s="45" t="s">
+        <v>311</v>
+      </c>
+      <c r="I34" s="44" t="s">
+        <v>312</v>
+      </c>
+      <c r="J34" s="44" t="s">
+        <v>313</v>
+      </c>
+      <c r="K34" s="45" t="s">
+        <v>314</v>
+      </c>
+      <c r="L34" s="44" t="s">
+        <v>315</v>
+      </c>
+      <c r="M34" s="44" t="s">
+        <v>316</v>
+      </c>
+      <c r="N34" s="45" t="s">
+        <v>317</v>
+      </c>
+      <c r="O34" s="44" t="s">
+        <v>318</v>
+      </c>
+      <c r="P34" s="44" t="s">
+        <v>319</v>
+      </c>
+      <c r="Q34" s="45" t="s">
+        <v>320</v>
+      </c>
+      <c r="R34" s="44" t="s">
+        <v>321</v>
+      </c>
+      <c r="S34" s="44" t="s">
+        <v>322</v>
+      </c>
+      <c r="T34" s="45" t="s">
+        <v>323</v>
+      </c>
+      <c r="U34" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="V34" s="31"/>
+      <c r="W34" s="31"/>
+      <c r="X34" s="31"/>
+      <c r="Y34" s="31"/>
+      <c r="Z34" s="31"/>
+      <c r="AA34" s="31"/>
+      <c r="AB34" s="31"/>
+    </row>
+    <row r="35" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B35" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="C35" s="64"/>
+      <c r="D35" s="44" t="s">
+        <v>325</v>
+      </c>
+      <c r="E35" s="45" t="s">
+        <v>326</v>
+      </c>
+      <c r="F35" s="44" t="s">
+        <v>327</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>328</v>
+      </c>
+      <c r="H35" s="44" t="s">
+        <v>329</v>
+      </c>
+      <c r="I35" s="44" t="s">
+        <v>330</v>
+      </c>
+      <c r="J35" s="44" t="s">
+        <v>331</v>
+      </c>
+      <c r="K35" s="44" t="s">
+        <v>332</v>
+      </c>
+      <c r="L35" s="44" t="s">
+        <v>333</v>
+      </c>
+      <c r="M35" s="44" t="s">
+        <v>334</v>
+      </c>
+      <c r="N35" s="45" t="s">
+        <v>335</v>
+      </c>
+      <c r="O35" s="44" t="s">
+        <v>336</v>
+      </c>
+      <c r="P35" s="44" t="s">
+        <v>337</v>
+      </c>
+      <c r="Q35" s="45" t="s">
+        <v>338</v>
+      </c>
+      <c r="R35" s="44" t="s">
+        <v>339</v>
+      </c>
+      <c r="S35" s="44" t="s">
+        <v>340</v>
+      </c>
+      <c r="T35" s="45" t="s">
+        <v>341</v>
+      </c>
+      <c r="U35" s="48" t="s">
+        <v>342</v>
+      </c>
+      <c r="V35" s="31"/>
+      <c r="W35" s="31"/>
+      <c r="X35" s="31"/>
+      <c r="Y35" s="31"/>
+      <c r="Z35" s="31"/>
+      <c r="AA35" s="31"/>
+      <c r="AB35" s="31"/>
+    </row>
+    <row r="36" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B36" s="65" t="s">
+        <v>27</v>
+      </c>
+      <c r="C36" s="66"/>
+      <c r="D36" s="46" t="s">
+        <v>343</v>
+      </c>
+      <c r="E36" s="45" t="s">
+        <v>344</v>
+      </c>
+      <c r="F36" s="46" t="s">
+        <v>345</v>
+      </c>
+      <c r="G36" s="46" t="s">
+        <v>346</v>
+      </c>
+      <c r="H36" s="46" t="s">
+        <v>347</v>
+      </c>
+      <c r="I36" s="46" t="s">
+        <v>348</v>
+      </c>
+      <c r="J36" s="46" t="s">
+        <v>349</v>
+      </c>
+      <c r="K36" s="46" t="s">
+        <v>350</v>
+      </c>
+      <c r="L36" s="46" t="s">
+        <v>351</v>
+      </c>
+      <c r="M36" s="46" t="s">
+        <v>352</v>
+      </c>
+      <c r="N36" s="45" t="s">
+        <v>353</v>
+      </c>
+      <c r="O36" s="46" t="s">
+        <v>354</v>
+      </c>
+      <c r="P36" s="46" t="s">
+        <v>355</v>
+      </c>
+      <c r="Q36" s="45" t="s">
+        <v>356</v>
+      </c>
+      <c r="R36" s="46" t="s">
+        <v>357</v>
+      </c>
+      <c r="S36" s="46" t="s">
+        <v>358</v>
+      </c>
+      <c r="T36" s="45" t="s">
+        <v>359</v>
+      </c>
+      <c r="U36" s="46" t="s">
+        <v>360</v>
+      </c>
+      <c r="V36" s="31"/>
+      <c r="W36" s="31"/>
+      <c r="X36" s="31"/>
+      <c r="Y36" s="31"/>
+      <c r="Z36" s="31"/>
+      <c r="AA36" s="31"/>
+      <c r="AB36" s="31"/>
+    </row>
+    <row r="37" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B37" s="31"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="31"/>
+      <c r="G37" s="31"/>
+      <c r="H37" s="31"/>
+      <c r="I37" s="31"/>
+      <c r="J37" s="31"/>
+      <c r="K37" s="31"/>
+      <c r="L37" s="31"/>
+      <c r="M37" s="31"/>
+      <c r="N37" s="31"/>
+      <c r="O37" s="31"/>
+      <c r="P37" s="31"/>
+      <c r="Q37" s="31"/>
+      <c r="R37" s="31"/>
+      <c r="S37" s="31"/>
+      <c r="T37" s="31"/>
+      <c r="U37" s="31"/>
+      <c r="V37" s="31"/>
+      <c r="W37" s="31"/>
+      <c r="X37" s="31"/>
+      <c r="Y37" s="31"/>
+      <c r="Z37" s="31"/>
+      <c r="AA37" s="31"/>
+      <c r="AB37" s="31"/>
+    </row>
+    <row r="38" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B38" s="57" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="35"/>
-      <c r="D20" s="35"/>
-      <c r="E20" s="85" t="s">
-        <v>204</v>
-      </c>
-      <c r="F20" s="85" t="s">
-        <v>205</v>
-      </c>
-      <c r="G20" s="85" t="s">
-        <v>206</v>
-      </c>
-      <c r="H20" s="85" t="s">
-        <v>207</v>
-      </c>
-      <c r="I20" s="85" t="s">
-        <v>208</v>
-      </c>
-      <c r="J20" s="85" t="s">
-        <v>209</v>
-      </c>
-      <c r="K20" s="85" t="s">
-        <v>210</v>
-      </c>
-      <c r="L20" s="85" t="s">
-        <v>211</v>
-      </c>
-      <c r="M20" s="85" t="s">
-        <v>212</v>
-      </c>
-      <c r="N20" s="85" t="s">
-        <v>213</v>
-      </c>
-      <c r="O20" s="85" t="s">
-        <v>214</v>
-      </c>
-      <c r="P20" s="85" t="s">
-        <v>215</v>
-      </c>
-      <c r="Q20" s="85" t="s">
-        <v>216</v>
-      </c>
-      <c r="R20" s="85" t="s">
-        <v>217</v>
-      </c>
-      <c r="S20" s="85" t="s">
-        <v>218</v>
-      </c>
-      <c r="T20" s="85" t="s">
-        <v>219</v>
-      </c>
-      <c r="U20" s="85" t="s">
-        <v>220</v>
-      </c>
-      <c r="V20" s="85" t="s">
-        <v>221</v>
-      </c>
-      <c r="W20" s="85" t="s">
-        <v>222</v>
-      </c>
-      <c r="X20" s="85" t="s">
-        <v>223</v>
-      </c>
-      <c r="Y20" s="85" t="s">
-        <v>224</v>
-      </c>
-      <c r="Z20" s="85" t="s">
-        <v>225</v>
-      </c>
-      <c r="AA20" s="85" t="s">
-        <v>226</v>
-      </c>
-      <c r="AB20" s="85" t="s">
-        <v>227</v>
-      </c>
-    </row>
-    <row r="21" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B21" s="35" t="s">
+      <c r="C38" s="58"/>
+      <c r="D38" s="49" t="s">
+        <v>361</v>
+      </c>
+      <c r="E38" s="49" t="s">
+        <v>362</v>
+      </c>
+      <c r="F38" s="49" t="s">
+        <v>363</v>
+      </c>
+      <c r="G38" s="49" t="s">
+        <v>364</v>
+      </c>
+      <c r="H38" s="49" t="s">
+        <v>365</v>
+      </c>
+      <c r="I38" s="49" t="s">
+        <v>366</v>
+      </c>
+      <c r="J38" s="49" t="s">
+        <v>367</v>
+      </c>
+      <c r="K38" s="49" t="s">
+        <v>368</v>
+      </c>
+      <c r="L38" s="49" t="s">
+        <v>369</v>
+      </c>
+      <c r="M38" s="49" t="s">
+        <v>370</v>
+      </c>
+      <c r="N38" s="49" t="s">
+        <v>371</v>
+      </c>
+      <c r="O38" s="49" t="s">
+        <v>372</v>
+      </c>
+      <c r="P38" s="49" t="s">
+        <v>373</v>
+      </c>
+      <c r="Q38" s="49" t="s">
+        <v>374</v>
+      </c>
+      <c r="R38" s="49" t="s">
+        <v>375</v>
+      </c>
+      <c r="S38" s="49" t="s">
+        <v>376</v>
+      </c>
+      <c r="T38" s="49" t="s">
+        <v>377</v>
+      </c>
+      <c r="U38" s="49" t="s">
+        <v>378</v>
+      </c>
+      <c r="V38" s="31"/>
+      <c r="W38" s="31"/>
+      <c r="X38" s="31"/>
+      <c r="Y38" s="31"/>
+      <c r="Z38" s="31"/>
+      <c r="AA38" s="31"/>
+      <c r="AB38" s="31"/>
+    </row>
+    <row r="39" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B39" s="57" t="s">
         <v>228</v>
       </c>
-      <c r="C21" s="35"/>
-      <c r="D21" s="35"/>
-      <c r="E21" s="85" t="s">
-        <v>229</v>
-      </c>
-      <c r="F21" s="85" t="s">
-        <v>230</v>
-      </c>
-      <c r="G21" s="85" t="s">
-        <v>231</v>
-      </c>
-      <c r="H21" s="85" t="s">
-        <v>232</v>
-      </c>
-      <c r="I21" s="85" t="s">
-        <v>233</v>
-      </c>
-      <c r="J21" s="85" t="s">
-        <v>234</v>
-      </c>
-      <c r="K21" s="85" t="s">
-        <v>235</v>
-      </c>
-      <c r="L21" s="85" t="s">
-        <v>236</v>
-      </c>
-      <c r="M21" s="85" t="s">
-        <v>237</v>
-      </c>
-      <c r="N21" s="85" t="s">
-        <v>238</v>
-      </c>
-      <c r="O21" s="85" t="s">
-        <v>239</v>
-      </c>
-      <c r="P21" s="85" t="s">
-        <v>240</v>
-      </c>
-      <c r="Q21" s="85" t="s">
-        <v>241</v>
-      </c>
-      <c r="R21" s="85" t="s">
-        <v>242</v>
-      </c>
-      <c r="S21" s="85" t="s">
-        <v>243</v>
-      </c>
-      <c r="T21" s="85" t="s">
-        <v>244</v>
-      </c>
-      <c r="U21" s="85" t="s">
-        <v>245</v>
-      </c>
-      <c r="V21" s="85" t="s">
-        <v>246</v>
-      </c>
-      <c r="W21" s="85" t="s">
-        <v>247</v>
-      </c>
-      <c r="X21" s="85" t="s">
-        <v>248</v>
-      </c>
-      <c r="Y21" s="85" t="s">
-        <v>249</v>
-      </c>
-      <c r="Z21" s="85" t="s">
-        <v>250</v>
-      </c>
-      <c r="AA21" s="85" t="s">
-        <v>251</v>
-      </c>
-      <c r="AB21" s="85" t="s">
-        <v>252</v>
-      </c>
-    </row>
-    <row r="24" spans="2:28" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B24" s="36" t="s">
-        <v>26</v>
-      </c>
-      <c r="C24" s="36"/>
-      <c r="D24" s="36"/>
-      <c r="E24" s="36"/>
-      <c r="F24" s="36"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
-      <c r="P24" s="36"/>
-      <c r="Q24" s="36"/>
-      <c r="R24" s="36"/>
-      <c r="S24" s="36"/>
-      <c r="T24" s="36"/>
-      <c r="U24" s="36"/>
-      <c r="V24" s="36"/>
-      <c r="W24" s="36"/>
-      <c r="X24" s="36"/>
-      <c r="Y24" s="36"/>
-      <c r="Z24" s="36"/>
-      <c r="AA24" s="36"/>
-      <c r="AB24" s="36"/>
-    </row>
-    <row r="26" spans="2:28" ht="75" x14ac:dyDescent="0.25">
-      <c r="B26" s="29" t="s">
-        <v>17</v>
-      </c>
-      <c r="C26" s="29"/>
-      <c r="D26" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E26" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F26" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G26" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H26" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="I26" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J26" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K26" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="L26" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="M26" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N26" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="O26" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="P26" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q26" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="R26" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="S26" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="T26" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="U26" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="V26" s="27" t="s">
-        <v>24</v>
-      </c>
-      <c r="W26" s="27" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B27" s="30" t="s">
-        <v>29</v>
-      </c>
-      <c r="C27" s="30"/>
-      <c r="D27" s="83" t="s">
-        <v>87</v>
-      </c>
-      <c r="E27" s="83" t="s">
-        <v>88</v>
-      </c>
-      <c r="F27" s="83" t="s">
-        <v>89</v>
-      </c>
-      <c r="G27" s="83" t="s">
-        <v>90</v>
-      </c>
-      <c r="H27" s="83" t="s">
-        <v>91</v>
-      </c>
-      <c r="I27" s="83" t="s">
-        <v>92</v>
-      </c>
-      <c r="J27" s="83" t="s">
-        <v>93</v>
-      </c>
-      <c r="K27" s="83" t="s">
-        <v>94</v>
-      </c>
-      <c r="L27" s="83" t="s">
-        <v>95</v>
-      </c>
-      <c r="M27" s="83" t="s">
-        <v>96</v>
-      </c>
-      <c r="N27" s="83" t="s">
-        <v>97</v>
-      </c>
-      <c r="O27" s="83" t="s">
-        <v>98</v>
-      </c>
-      <c r="P27" s="83" t="s">
-        <v>99</v>
-      </c>
-      <c r="Q27" s="83" t="s">
-        <v>100</v>
-      </c>
-      <c r="R27" s="83" t="s">
-        <v>101</v>
-      </c>
-      <c r="S27" s="83" t="s">
-        <v>102</v>
-      </c>
-      <c r="T27" s="83" t="s">
-        <v>103</v>
-      </c>
-      <c r="U27" s="83" t="s">
-        <v>104</v>
-      </c>
-      <c r="V27" s="83" t="s">
-        <v>105</v>
-      </c>
-      <c r="W27" s="83" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="28" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B28" s="30"/>
-      <c r="C28" s="30"/>
-      <c r="D28" s="85"/>
-      <c r="E28" s="85"/>
-      <c r="F28" s="85"/>
-      <c r="G28" s="85"/>
-      <c r="H28" s="85"/>
-      <c r="I28" s="85"/>
-      <c r="J28" s="85"/>
-      <c r="K28" s="85"/>
-      <c r="L28" s="85"/>
-      <c r="M28" s="85"/>
-      <c r="N28" s="85"/>
-      <c r="O28" s="85"/>
-      <c r="P28" s="85"/>
-      <c r="Q28" s="85"/>
-      <c r="R28" s="85"/>
-      <c r="S28" s="85"/>
-      <c r="T28" s="85"/>
-      <c r="U28" s="85"/>
-      <c r="V28" s="85"/>
-      <c r="W28" s="85"/>
-    </row>
-    <row r="30" spans="2:28" ht="68.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B30" s="62"/>
-      <c r="C30" s="62"/>
-      <c r="D30" s="28" t="s">
-        <v>18</v>
-      </c>
-      <c r="E30" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F30" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G30" s="22" t="s">
-        <v>19</v>
-      </c>
-      <c r="H30" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="I30" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="J30" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="K30" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="L30" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="M30" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N30" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="O30" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="P30" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q30" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="R30" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="S30" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="T30" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="U30" s="22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="31" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B31" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="C31" s="63"/>
-      <c r="D31" s="89" t="s">
-        <v>253</v>
-      </c>
-      <c r="E31" s="90" t="s">
-        <v>254</v>
-      </c>
-      <c r="F31" s="89" t="s">
-        <v>255</v>
-      </c>
-      <c r="G31" s="89" t="s">
-        <v>256</v>
-      </c>
-      <c r="H31" s="90" t="s">
-        <v>257</v>
-      </c>
-      <c r="I31" s="89" t="s">
-        <v>258</v>
-      </c>
-      <c r="J31" s="89" t="s">
-        <v>259</v>
-      </c>
-      <c r="K31" s="90" t="s">
-        <v>260</v>
-      </c>
-      <c r="L31" s="89" t="s">
-        <v>261</v>
-      </c>
-      <c r="M31" s="89" t="s">
-        <v>262</v>
-      </c>
-      <c r="N31" s="90" t="s">
-        <v>263</v>
-      </c>
-      <c r="O31" s="89" t="s">
-        <v>264</v>
-      </c>
-      <c r="P31" s="89" t="s">
-        <v>265</v>
-      </c>
-      <c r="Q31" s="90" t="s">
-        <v>266</v>
-      </c>
-      <c r="R31" s="89" t="s">
-        <v>267</v>
-      </c>
-      <c r="S31" s="89" t="s">
-        <v>268</v>
-      </c>
-      <c r="T31" s="90" t="s">
-        <v>269</v>
-      </c>
-      <c r="U31" s="89" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="32" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B32" s="63" t="s">
-        <v>56</v>
-      </c>
-      <c r="C32" s="63"/>
-      <c r="D32" s="89" t="s">
-        <v>271</v>
-      </c>
-      <c r="E32" s="90" t="s">
-        <v>272</v>
-      </c>
-      <c r="F32" s="89" t="s">
-        <v>273</v>
-      </c>
-      <c r="G32" s="89" t="s">
-        <v>274</v>
-      </c>
-      <c r="H32" s="90" t="s">
-        <v>275</v>
-      </c>
-      <c r="I32" s="89" t="s">
-        <v>276</v>
-      </c>
-      <c r="J32" s="89" t="s">
-        <v>277</v>
-      </c>
-      <c r="K32" s="90" t="s">
-        <v>278</v>
-      </c>
-      <c r="L32" s="89" t="s">
-        <v>279</v>
-      </c>
-      <c r="M32" s="89" t="s">
-        <v>280</v>
-      </c>
-      <c r="N32" s="90" t="s">
-        <v>281</v>
-      </c>
-      <c r="O32" s="89" t="s">
-        <v>282</v>
-      </c>
-      <c r="P32" s="89" t="s">
-        <v>283</v>
-      </c>
-      <c r="Q32" s="90" t="s">
-        <v>284</v>
-      </c>
-      <c r="R32" s="89" t="s">
-        <v>285</v>
-      </c>
-      <c r="S32" s="89" t="s">
-        <v>286</v>
-      </c>
-      <c r="T32" s="90" t="s">
-        <v>287</v>
-      </c>
-      <c r="U32" s="89" t="s">
-        <v>288</v>
-      </c>
-    </row>
-    <row r="33" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B33" s="64" t="s">
-        <v>27</v>
-      </c>
-      <c r="C33" s="64"/>
-      <c r="D33" s="91" t="s">
-        <v>289</v>
-      </c>
-      <c r="E33" s="90" t="s">
-        <v>290</v>
-      </c>
-      <c r="F33" s="91" t="s">
-        <v>291</v>
-      </c>
-      <c r="G33" s="91" t="s">
-        <v>292</v>
-      </c>
-      <c r="H33" s="91" t="s">
-        <v>293</v>
-      </c>
-      <c r="I33" s="91" t="s">
-        <v>294</v>
-      </c>
-      <c r="J33" s="91" t="s">
-        <v>295</v>
-      </c>
-      <c r="K33" s="91" t="s">
-        <v>296</v>
-      </c>
-      <c r="L33" s="91" t="s">
-        <v>297</v>
-      </c>
-      <c r="M33" s="91" t="s">
-        <v>298</v>
-      </c>
-      <c r="N33" s="90" t="s">
-        <v>299</v>
-      </c>
-      <c r="O33" s="91" t="s">
-        <v>300</v>
-      </c>
-      <c r="P33" s="91" t="s">
-        <v>301</v>
-      </c>
-      <c r="Q33" s="90" t="s">
-        <v>302</v>
-      </c>
-      <c r="R33" s="91" t="s">
-        <v>303</v>
-      </c>
-      <c r="S33" s="91" t="s">
-        <v>304</v>
-      </c>
-      <c r="T33" s="90" t="s">
-        <v>305</v>
-      </c>
-      <c r="U33" s="91" t="s">
-        <v>306</v>
-      </c>
-    </row>
-    <row r="34" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="K34" s="21"/>
-    </row>
-    <row r="35" spans="2:21" ht="66.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B35" s="29"/>
-      <c r="C35" s="29"/>
-      <c r="D35" s="22" t="s">
-        <v>18</v>
-      </c>
-      <c r="E35" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="F35" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="G35" s="22"/>
-      <c r="H35" s="22"/>
-      <c r="I35" s="22"/>
-      <c r="J35" s="22"/>
-      <c r="K35" s="22"/>
-      <c r="L35" s="22"/>
-      <c r="M35" s="22" t="s">
-        <v>21</v>
-      </c>
-      <c r="N35" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="O35" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="P35" s="22" t="s">
-        <v>22</v>
-      </c>
-      <c r="Q35" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="R35" s="22" t="s">
-        <v>7</v>
-      </c>
-      <c r="S35" s="22" t="s">
-        <v>23</v>
-      </c>
-      <c r="T35" s="22" t="s">
-        <v>6</v>
-      </c>
-      <c r="U35" s="22" t="s">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="36" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B36" s="63" t="s">
-        <v>55</v>
-      </c>
-      <c r="C36" s="63"/>
-      <c r="D36" s="89" t="s">
-        <v>307</v>
-      </c>
-      <c r="E36" s="90" t="s">
-        <v>308</v>
-      </c>
-      <c r="F36" s="89" t="s">
-        <v>309</v>
-      </c>
-      <c r="G36" s="89" t="s">
-        <v>310</v>
-      </c>
-      <c r="H36" s="90" t="s">
-        <v>311</v>
-      </c>
-      <c r="I36" s="89" t="s">
-        <v>312</v>
-      </c>
-      <c r="J36" s="89" t="s">
-        <v>313</v>
-      </c>
-      <c r="K36" s="90" t="s">
-        <v>314</v>
-      </c>
-      <c r="L36" s="89" t="s">
-        <v>315</v>
-      </c>
-      <c r="M36" s="89" t="s">
-        <v>316</v>
-      </c>
-      <c r="N36" s="90" t="s">
-        <v>317</v>
-      </c>
-      <c r="O36" s="89" t="s">
-        <v>318</v>
-      </c>
-      <c r="P36" s="89" t="s">
-        <v>319</v>
-      </c>
-      <c r="Q36" s="90" t="s">
-        <v>320</v>
-      </c>
-      <c r="R36" s="89" t="s">
-        <v>321</v>
-      </c>
-      <c r="S36" s="89" t="s">
-        <v>322</v>
-      </c>
-      <c r="T36" s="90" t="s">
-        <v>323</v>
-      </c>
-      <c r="U36" s="89" t="s">
-        <v>324</v>
-      </c>
-    </row>
-    <row r="37" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B37" s="65" t="s">
-        <v>56</v>
-      </c>
-      <c r="C37" s="66"/>
-      <c r="D37" s="89" t="s">
-        <v>325</v>
-      </c>
-      <c r="E37" s="90" t="s">
-        <v>326</v>
-      </c>
-      <c r="F37" s="89" t="s">
-        <v>327</v>
-      </c>
-      <c r="G37" s="89" t="s">
-        <v>328</v>
-      </c>
-      <c r="H37" s="89" t="s">
-        <v>329</v>
-      </c>
-      <c r="I37" s="89" t="s">
-        <v>330</v>
-      </c>
-      <c r="J37" s="89" t="s">
-        <v>331</v>
-      </c>
-      <c r="K37" s="89" t="s">
-        <v>332</v>
-      </c>
-      <c r="L37" s="89" t="s">
-        <v>333</v>
-      </c>
-      <c r="M37" s="89" t="s">
-        <v>334</v>
-      </c>
-      <c r="N37" s="90" t="s">
-        <v>335</v>
-      </c>
-      <c r="O37" s="89" t="s">
-        <v>336</v>
-      </c>
-      <c r="P37" s="89" t="s">
-        <v>337</v>
-      </c>
-      <c r="Q37" s="90" t="s">
-        <v>338</v>
-      </c>
-      <c r="R37" s="89" t="s">
-        <v>339</v>
-      </c>
-      <c r="S37" s="89" t="s">
-        <v>340</v>
-      </c>
-      <c r="T37" s="90" t="s">
-        <v>341</v>
-      </c>
-      <c r="U37" s="92" t="s">
-        <v>342</v>
-      </c>
-    </row>
-    <row r="38" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B38" s="67" t="s">
-        <v>27</v>
-      </c>
-      <c r="C38" s="68"/>
-      <c r="D38" s="91" t="s">
-        <v>343</v>
-      </c>
-      <c r="E38" s="90" t="s">
-        <v>344</v>
-      </c>
-      <c r="F38" s="91" t="s">
-        <v>345</v>
-      </c>
-      <c r="G38" s="91" t="s">
-        <v>346</v>
-      </c>
-      <c r="H38" s="91" t="s">
-        <v>347</v>
-      </c>
-      <c r="I38" s="91" t="s">
-        <v>348</v>
-      </c>
-      <c r="J38" s="91" t="s">
-        <v>349</v>
-      </c>
-      <c r="K38" s="91" t="s">
-        <v>350</v>
-      </c>
-      <c r="L38" s="91" t="s">
-        <v>351</v>
-      </c>
-      <c r="M38" s="91" t="s">
-        <v>352</v>
-      </c>
-      <c r="N38" s="90" t="s">
-        <v>353</v>
-      </c>
-      <c r="O38" s="91" t="s">
-        <v>354</v>
-      </c>
-      <c r="P38" s="91" t="s">
-        <v>355</v>
-      </c>
-      <c r="Q38" s="90" t="s">
-        <v>356</v>
-      </c>
-      <c r="R38" s="91" t="s">
-        <v>357</v>
-      </c>
-      <c r="S38" s="91" t="s">
-        <v>358</v>
-      </c>
-      <c r="T38" s="90" t="s">
-        <v>359</v>
-      </c>
-      <c r="U38" s="91" t="s">
-        <v>360</v>
-      </c>
-    </row>
-    <row r="40" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B40" s="60" t="s">
-        <v>28</v>
-      </c>
-      <c r="C40" s="61"/>
-      <c r="D40" s="93" t="s">
-        <v>361</v>
-      </c>
-      <c r="E40" s="93" t="s">
-        <v>362</v>
-      </c>
-      <c r="F40" s="93" t="s">
-        <v>363</v>
-      </c>
-      <c r="G40" s="93" t="s">
-        <v>364</v>
-      </c>
-      <c r="H40" s="93" t="s">
-        <v>365</v>
-      </c>
-      <c r="I40" s="93" t="s">
-        <v>366</v>
-      </c>
-      <c r="J40" s="93" t="s">
-        <v>367</v>
-      </c>
-      <c r="K40" s="93" t="s">
-        <v>368</v>
-      </c>
-      <c r="L40" s="93" t="s">
-        <v>369</v>
-      </c>
-      <c r="M40" s="93" t="s">
-        <v>370</v>
-      </c>
-      <c r="N40" s="93" t="s">
-        <v>371</v>
-      </c>
-      <c r="O40" s="93" t="s">
-        <v>372</v>
-      </c>
-      <c r="P40" s="93" t="s">
-        <v>373</v>
-      </c>
-      <c r="Q40" s="93" t="s">
-        <v>374</v>
-      </c>
-      <c r="R40" s="93" t="s">
-        <v>375</v>
-      </c>
-      <c r="S40" s="93" t="s">
-        <v>376</v>
-      </c>
-      <c r="T40" s="93" t="s">
-        <v>377</v>
-      </c>
-      <c r="U40" s="93" t="s">
-        <v>378</v>
-      </c>
-    </row>
-    <row r="41" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="B41" s="60" t="s">
-        <v>228</v>
-      </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="93" t="s">
+      <c r="C39" s="58"/>
+      <c r="D39" s="49" t="s">
         <v>379</v>
       </c>
-      <c r="E41" s="93" t="s">
+      <c r="E39" s="49" t="s">
         <v>380</v>
       </c>
-      <c r="F41" s="93" t="s">
+      <c r="F39" s="49" t="s">
         <v>381</v>
       </c>
-      <c r="G41" s="93" t="s">
+      <c r="G39" s="49" t="s">
         <v>382</v>
       </c>
-      <c r="H41" s="93" t="s">
+      <c r="H39" s="49" t="s">
         <v>383</v>
       </c>
-      <c r="I41" s="93" t="s">
+      <c r="I39" s="49" t="s">
         <v>384</v>
       </c>
-      <c r="J41" s="93" t="s">
+      <c r="J39" s="49" t="s">
         <v>385</v>
       </c>
-      <c r="K41" s="93" t="s">
+      <c r="K39" s="49" t="s">
         <v>386</v>
       </c>
-      <c r="L41" s="93" t="s">
+      <c r="L39" s="49" t="s">
         <v>387</v>
       </c>
-      <c r="M41" s="93" t="s">
+      <c r="M39" s="49" t="s">
         <v>388</v>
       </c>
-      <c r="N41" s="93" t="s">
+      <c r="N39" s="49" t="s">
         <v>389</v>
       </c>
-      <c r="O41" s="93" t="s">
+      <c r="O39" s="49" t="s">
         <v>390</v>
       </c>
-      <c r="P41" s="93" t="s">
+      <c r="P39" s="49" t="s">
         <v>391</v>
       </c>
-      <c r="Q41" s="93" t="s">
+      <c r="Q39" s="49" t="s">
         <v>392</v>
       </c>
-      <c r="R41" s="93" t="s">
+      <c r="R39" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="S41" s="93" t="s">
+      <c r="S39" s="49" t="s">
         <v>394</v>
       </c>
-      <c r="T41" s="93" t="s">
+      <c r="T39" s="49" t="s">
         <v>395</v>
       </c>
-      <c r="U41" s="93" t="s">
+      <c r="U39" s="49" t="s">
         <v>396</v>
       </c>
-    </row>
-    <row r="42" spans="2:21" x14ac:dyDescent="0.25">
-      <c r="E42" s="21"/>
+      <c r="V39" s="31"/>
+      <c r="W39" s="31"/>
+      <c r="X39" s="31"/>
+      <c r="Y39" s="31"/>
+      <c r="Z39" s="31"/>
+      <c r="AA39" s="31"/>
+      <c r="AB39" s="31"/>
+    </row>
+    <row r="40" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="E40" s="21"/>
     </row>
   </sheetData>
   <mergeCells count="35">
-    <mergeCell ref="B41:C41"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B40:C40"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B32:C32"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B36:C36"/>
-    <mergeCell ref="B37:C37"/>
-    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B24:C24"/>
+    <mergeCell ref="B25:C25"/>
+    <mergeCell ref="B26:C26"/>
+    <mergeCell ref="B8:D8"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B22:AB22"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B12:D12"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="E6:G6"/>
     <mergeCell ref="Z6:AB6"/>
@@ -4333,20 +4862,16 @@
     <mergeCell ref="T6:V6"/>
     <mergeCell ref="K6:M6"/>
     <mergeCell ref="N6:P6"/>
-    <mergeCell ref="B26:C26"/>
-    <mergeCell ref="B27:C27"/>
+    <mergeCell ref="B39:C39"/>
     <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B8:D8"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B24:AB24"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4377,10 +4902,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="B2" s="77" t="s">
+      <c r="B2" s="105" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="77"/>
+      <c r="C2" s="105"/>
       <c r="D2" s="4" t="s">
         <v>1</v>
       </c>
@@ -4392,43 +4917,43 @@
       </c>
     </row>
     <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="B4" s="36" t="s">
+      <c r="B4" s="106" t="s">
         <v>76</v>
       </c>
-      <c r="C4" s="36"/>
-      <c r="D4" s="36"/>
-      <c r="E4" s="36"/>
-      <c r="F4" s="36"/>
-      <c r="G4" s="36"/>
-      <c r="H4" s="36"/>
-      <c r="I4" s="36"/>
-      <c r="J4" s="36"/>
-      <c r="K4" s="36"/>
-      <c r="L4" s="36"/>
+      <c r="C4" s="106"/>
+      <c r="D4" s="106"/>
+      <c r="E4" s="106"/>
+      <c r="F4" s="106"/>
+      <c r="G4" s="106"/>
+      <c r="H4" s="106"/>
+      <c r="I4" s="106"/>
+      <c r="J4" s="106"/>
+      <c r="K4" s="106"/>
+      <c r="L4" s="106"/>
     </row>
     <row r="6" spans="2:12" ht="36.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="42" t="s">
+      <c r="B6" s="107" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="79" t="s">
+      <c r="C6" s="110" t="s">
         <v>75</v>
       </c>
-      <c r="D6" s="80"/>
-      <c r="E6" s="80"/>
-      <c r="F6" s="81"/>
-      <c r="G6" s="78" t="s">
+      <c r="D6" s="111"/>
+      <c r="E6" s="111"/>
+      <c r="F6" s="112"/>
+      <c r="G6" s="109" t="s">
         <v>74</v>
       </c>
-      <c r="H6" s="78"/>
-      <c r="I6" s="78"/>
-      <c r="J6" s="56" t="s">
+      <c r="H6" s="109"/>
+      <c r="I6" s="109"/>
+      <c r="J6" s="113" t="s">
         <v>73</v>
       </c>
-      <c r="K6" s="57"/>
-      <c r="L6" s="57"/>
+      <c r="K6" s="114"/>
+      <c r="L6" s="114"/>
     </row>
     <row r="7" spans="2:12" s="3" customFormat="1" ht="45" x14ac:dyDescent="0.25">
-      <c r="B7" s="45"/>
+      <c r="B7" s="108"/>
       <c r="C7" s="22" t="s">
         <v>71</v>
       </c>
@@ -4464,49 +4989,49 @@
       <c r="B8" s="6" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="94" t="s">
+      <c r="C8" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="85" t="s">
+      <c r="D8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="85" t="s">
+      <c r="E8" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="85" t="s">
+      <c r="F8" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="85" t="s">
+      <c r="G8" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="85" t="s">
+      <c r="H8" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="85" t="s">
+      <c r="I8" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="85" t="s">
+      <c r="J8" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="85" t="s">
+      <c r="K8" s="24" t="s">
         <v>85</v>
       </c>
-      <c r="L8" s="85" t="s">
+      <c r="L8" s="24" t="s">
         <v>86</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B9" s="6"/>
-      <c r="C9" s="94"/>
-      <c r="D9" s="85"/>
-      <c r="E9" s="85"/>
-      <c r="F9" s="85"/>
-      <c r="G9" s="85"/>
-      <c r="H9" s="85"/>
-      <c r="I9" s="85"/>
-      <c r="J9" s="85"/>
-      <c r="K9" s="85"/>
-      <c r="L9" s="85"/>
+      <c r="C9" s="25"/>
+      <c r="D9" s="24"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
+      <c r="H9" s="24"/>
+      <c r="I9" s="24"/>
+      <c r="J9" s="24"/>
+      <c r="K9" s="24"/>
+      <c r="L9" s="24"/>
     </row>
     <row r="11" spans="2:12" ht="45" x14ac:dyDescent="0.25">
       <c r="B11" s="2" t="s">
@@ -4547,34 +5072,34 @@
       <c r="B12" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="85" t="s">
+      <c r="C12" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="85" t="s">
+      <c r="D12" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="E12" s="85" t="s">
+      <c r="E12" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="F12" s="85" t="s">
+      <c r="F12" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="G12" s="85" t="s">
+      <c r="G12" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="H12" s="85" t="s">
+      <c r="H12" s="24" t="s">
         <v>402</v>
       </c>
-      <c r="I12" s="85" t="s">
+      <c r="I12" s="24" t="s">
         <v>403</v>
       </c>
-      <c r="J12" s="85" t="s">
+      <c r="J12" s="24" t="s">
         <v>404</v>
       </c>
-      <c r="K12" s="85" t="s">
+      <c r="K12" s="24" t="s">
         <v>405</v>
       </c>
-      <c r="L12" s="85" t="s">
+      <c r="L12" s="24" t="s">
         <v>406</v>
       </c>
     </row>
@@ -4582,34 +5107,34 @@
       <c r="B13" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C13" s="85" t="s">
+      <c r="C13" s="24" t="s">
         <v>407</v>
       </c>
-      <c r="D13" s="85" t="s">
+      <c r="D13" s="24" t="s">
         <v>408</v>
       </c>
-      <c r="E13" s="85" t="s">
+      <c r="E13" s="24" t="s">
         <v>409</v>
       </c>
-      <c r="F13" s="85" t="s">
+      <c r="F13" s="24" t="s">
         <v>410</v>
       </c>
-      <c r="G13" s="85" t="s">
+      <c r="G13" s="24" t="s">
         <v>411</v>
       </c>
-      <c r="H13" s="85" t="s">
+      <c r="H13" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="I13" s="85" t="s">
+      <c r="I13" s="24" t="s">
         <v>413</v>
       </c>
-      <c r="J13" s="85" t="s">
+      <c r="J13" s="24" t="s">
         <v>414</v>
       </c>
-      <c r="K13" s="85" t="s">
+      <c r="K13" s="24" t="s">
         <v>415</v>
       </c>
-      <c r="L13" s="85" t="s">
+      <c r="L13" s="24" t="s">
         <v>416</v>
       </c>
     </row>
@@ -4652,34 +5177,34 @@
       <c r="B16" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="85" t="s">
+      <c r="C16" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="D16" s="85" t="s">
+      <c r="D16" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="E16" s="85" t="s">
+      <c r="E16" s="24" t="s">
         <v>419</v>
       </c>
-      <c r="F16" s="85" t="s">
+      <c r="F16" s="24" t="s">
         <v>420</v>
       </c>
-      <c r="G16" s="85" t="s">
+      <c r="G16" s="24" t="s">
         <v>421</v>
       </c>
-      <c r="H16" s="85" t="s">
+      <c r="H16" s="24" t="s">
         <v>422</v>
       </c>
-      <c r="I16" s="85" t="s">
+      <c r="I16" s="24" t="s">
         <v>423</v>
       </c>
-      <c r="J16" s="85" t="s">
+      <c r="J16" s="24" t="s">
         <v>424</v>
       </c>
-      <c r="K16" s="85" t="s">
+      <c r="K16" s="24" t="s">
         <v>425</v>
       </c>
-      <c r="L16" s="85" t="s">
+      <c r="L16" s="24" t="s">
         <v>426</v>
       </c>
     </row>
@@ -4687,34 +5212,34 @@
       <c r="B17" s="1" t="s">
         <v>56</v>
       </c>
-      <c r="C17" s="85" t="s">
+      <c r="C17" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="D17" s="85" t="s">
+      <c r="D17" s="24" t="s">
         <v>428</v>
       </c>
-      <c r="E17" s="85" t="s">
+      <c r="E17" s="24" t="s">
         <v>429</v>
       </c>
-      <c r="F17" s="85" t="s">
+      <c r="F17" s="24" t="s">
         <v>430</v>
       </c>
-      <c r="G17" s="85" t="s">
+      <c r="G17" s="24" t="s">
         <v>431</v>
       </c>
-      <c r="H17" s="85" t="s">
+      <c r="H17" s="24" t="s">
         <v>432</v>
       </c>
-      <c r="I17" s="85" t="s">
+      <c r="I17" s="24" t="s">
         <v>433</v>
       </c>
-      <c r="J17" s="85" t="s">
+      <c r="J17" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="K17" s="85" t="s">
+      <c r="K17" s="24" t="s">
         <v>435</v>
       </c>
-      <c r="L17" s="85" t="s">
+      <c r="L17" s="24" t="s">
         <v>436</v>
       </c>
     </row>
@@ -4722,34 +5247,34 @@
       <c r="B19" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="85" t="s">
+      <c r="C19" s="24" t="s">
         <v>437</v>
       </c>
-      <c r="D19" s="85" t="s">
+      <c r="D19" s="24" t="s">
         <v>438</v>
       </c>
-      <c r="E19" s="85" t="s">
+      <c r="E19" s="24" t="s">
         <v>439</v>
       </c>
-      <c r="F19" s="85" t="s">
+      <c r="F19" s="24" t="s">
         <v>440</v>
       </c>
-      <c r="G19" s="85" t="s">
+      <c r="G19" s="24" t="s">
         <v>441</v>
       </c>
-      <c r="H19" s="85" t="s">
+      <c r="H19" s="24" t="s">
         <v>442</v>
       </c>
-      <c r="I19" s="85" t="s">
+      <c r="I19" s="24" t="s">
         <v>443</v>
       </c>
-      <c r="J19" s="85" t="s">
+      <c r="J19" s="24" t="s">
         <v>444</v>
       </c>
-      <c r="K19" s="85" t="s">
+      <c r="K19" s="24" t="s">
         <v>445</v>
       </c>
-      <c r="L19" s="85" t="s">
+      <c r="L19" s="24" t="s">
         <v>446</v>
       </c>
     </row>
@@ -4757,57 +5282,57 @@
       <c r="B20" s="1" t="s">
         <v>228</v>
       </c>
-      <c r="C20" s="85" t="s">
+      <c r="C20" s="24" t="s">
         <v>447</v>
       </c>
-      <c r="D20" s="85" t="s">
+      <c r="D20" s="24" t="s">
         <v>448</v>
       </c>
-      <c r="E20" s="85" t="s">
+      <c r="E20" s="24" t="s">
         <v>449</v>
       </c>
-      <c r="F20" s="85" t="s">
+      <c r="F20" s="24" t="s">
         <v>450</v>
       </c>
-      <c r="G20" s="85" t="s">
+      <c r="G20" s="24" t="s">
         <v>451</v>
       </c>
-      <c r="H20" s="85" t="s">
+      <c r="H20" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="I20" s="85" t="s">
+      <c r="I20" s="24" t="s">
         <v>453</v>
       </c>
-      <c r="J20" s="85" t="s">
+      <c r="J20" s="24" t="s">
         <v>454</v>
       </c>
-      <c r="K20" s="85" t="s">
+      <c r="K20" s="24" t="s">
         <v>455</v>
       </c>
-      <c r="L20" s="85" t="s">
+      <c r="L20" s="24" t="s">
         <v>456</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
       <c r="D22" s="21"/>
-      <c r="F22" s="69" t="s">
+      <c r="F22" s="97" t="s">
         <v>59</v>
       </c>
-      <c r="G22" s="70"/>
-      <c r="H22" s="71"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="99"/>
       <c r="I22" s="8"/>
-      <c r="J22" s="69" t="s">
+      <c r="J22" s="97" t="s">
         <v>58</v>
       </c>
-      <c r="K22" s="74"/>
-      <c r="L22" s="75"/>
+      <c r="K22" s="102"/>
+      <c r="L22" s="103"/>
     </row>
     <row r="23" spans="2:12" x14ac:dyDescent="0.25">
       <c r="F23" s="17" t="s">
         <v>68</v>
       </c>
       <c r="G23" s="20"/>
-      <c r="H23" s="95" t="s">
+      <c r="H23" s="26" t="s">
         <v>457</v>
       </c>
       <c r="I23" s="8"/>
@@ -4815,7 +5340,7 @@
         <v>68</v>
       </c>
       <c r="K23" s="16"/>
-      <c r="L23" s="95" t="s">
+      <c r="L23" s="26" t="s">
         <v>462</v>
       </c>
     </row>
@@ -4824,7 +5349,7 @@
         <v>67</v>
       </c>
       <c r="G24" s="20"/>
-      <c r="H24" s="95" t="s">
+      <c r="H24" s="26" t="s">
         <v>458</v>
       </c>
       <c r="I24" s="8"/>
@@ -4832,7 +5357,7 @@
         <v>67</v>
       </c>
       <c r="K24" s="16"/>
-      <c r="L24" s="95" t="s">
+      <c r="L24" s="26" t="s">
         <v>463</v>
       </c>
     </row>
@@ -4841,7 +5366,7 @@
         <v>66</v>
       </c>
       <c r="G25" s="20"/>
-      <c r="H25" s="95" t="s">
+      <c r="H25" s="26" t="s">
         <v>459</v>
       </c>
       <c r="I25" s="8"/>
@@ -4849,7 +5374,7 @@
         <v>66</v>
       </c>
       <c r="K25" s="16"/>
-      <c r="L25" s="95" t="s">
+      <c r="L25" s="26" t="s">
         <v>464</v>
       </c>
     </row>
@@ -4858,7 +5383,7 @@
         <v>65</v>
       </c>
       <c r="G26" s="18"/>
-      <c r="H26" s="95" t="s">
+      <c r="H26" s="26" t="s">
         <v>460</v>
       </c>
       <c r="I26" s="8"/>
@@ -4866,24 +5391,24 @@
         <v>65</v>
       </c>
       <c r="K26" s="16"/>
-      <c r="L26" s="95" t="s">
+      <c r="L26" s="26" t="s">
         <v>465</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
-      <c r="F27" s="72" t="s">
+      <c r="F27" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="G27" s="73"/>
-      <c r="H27" s="95" t="s">
+      <c r="G27" s="101"/>
+      <c r="H27" s="26" t="s">
         <v>461</v>
       </c>
       <c r="I27" s="8"/>
-      <c r="J27" s="72" t="s">
+      <c r="J27" s="100" t="s">
         <v>64</v>
       </c>
-      <c r="K27" s="76"/>
-      <c r="L27" s="95" t="s">
+      <c r="K27" s="104"/>
+      <c r="L27" s="26" t="s">
         <v>466</v>
       </c>
     </row>
@@ -4942,20 +5467,20 @@
       <c r="F31" s="9" t="s">
         <v>59</v>
       </c>
-      <c r="G31" s="96" t="s">
+      <c r="G31" s="27" t="s">
         <v>467</v>
       </c>
-      <c r="H31" s="96" t="s">
+      <c r="H31" s="27" t="s">
         <v>468</v>
       </c>
       <c r="I31" s="8"/>
       <c r="J31" s="7" t="s">
         <v>58</v>
       </c>
-      <c r="K31" s="96" t="s">
+      <c r="K31" s="27" t="s">
         <v>469</v>
       </c>
-      <c r="L31" s="96" t="s">
+      <c r="L31" s="27" t="s">
         <v>470</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actulización de reportes Mensuales
</commit_message>
<xml_diff>
--- a/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ResumenBalanceEnergLIV.xlsx
+++ b/Unna.OperationalReport.WebSite/wwwroot/plantillas/reporte/quincenal/ResumenBalanceEnergLIV.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\SPP_UNNA_MAIN\UnnaReportesOperativos\Unna.OperationalReport.WebSite\wwwroot\plantillas\reporte\quincenal\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B6F9FE8-4890-4F62-825F-78882D6BEA4D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E227DCB2-AB18-4EC5-8AFA-1C6D0BB28420}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -312,9 +312,6 @@
     <t>GAS LICUADO DE PETRÓLEO - GLP</t>
   </si>
   <si>
-    <t>MEDICIÓN DE GAS NATURAL DEL LOTE IV - BALANCE ENERGETICO DE PLANTA DE UNNA ENERGIA LGN (GLP y CGN)</t>
-  </si>
-  <si>
     <t>{{item.MedGasGlpVolumen}}</t>
   </si>
   <si>
@@ -1507,6 +1504,9 @@
   </si>
   <si>
     <t>{{GNSEnergia2Q}}</t>
+  </si>
+  <si>
+    <t>MEDICIÓN DE GAS NATURAL DEL LOTE IV - BALANCE ENERGETICO DE PLANTA DE GMP LGN (GLP y CGN)</t>
   </si>
 </sst>
 </file>
@@ -2248,6 +2248,99 @@
     <xf numFmtId="0" fontId="25" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2260,9 +2353,6 @@
     <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="17" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="17" fillId="19" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2277,96 +2367,6 @@
     </xf>
     <xf numFmtId="0" fontId="17" fillId="19" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="10" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="17" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="11" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="16" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="14" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="15" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="13" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="8" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -2714,9 +2714,7 @@
   </sheetPr>
   <dimension ref="B1:AE40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="AE11" sqref="AE11"/>
-    </sheetView>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2730,12 +2728,12 @@
   <sheetData>
     <row r="1" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:31" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="67" t="s">
+      <c r="B2" s="65" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="67"/>
-      <c r="D2" s="67"/>
-      <c r="E2" s="67"/>
+      <c r="C2" s="65"/>
+      <c r="D2" s="65"/>
+      <c r="E2" s="65"/>
       <c r="F2" s="28" t="s">
         <v>1</v>
       </c>
@@ -2796,35 +2794,35 @@
       <c r="AB3" s="31"/>
     </row>
     <row r="4" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B4" s="72" t="s">
+      <c r="B4" s="64" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="72"/>
-      <c r="D4" s="72"/>
-      <c r="E4" s="72"/>
-      <c r="F4" s="72"/>
-      <c r="G4" s="72"/>
-      <c r="H4" s="72"/>
-      <c r="I4" s="72"/>
-      <c r="J4" s="72"/>
-      <c r="K4" s="72"/>
-      <c r="L4" s="72"/>
-      <c r="M4" s="72"/>
-      <c r="N4" s="72"/>
-      <c r="O4" s="72"/>
-      <c r="P4" s="72"/>
-      <c r="Q4" s="72"/>
-      <c r="R4" s="72"/>
-      <c r="S4" s="72"/>
-      <c r="T4" s="72"/>
-      <c r="U4" s="72"/>
-      <c r="V4" s="72"/>
-      <c r="W4" s="72"/>
-      <c r="X4" s="72"/>
-      <c r="Y4" s="72"/>
-      <c r="Z4" s="72"/>
-      <c r="AA4" s="72"/>
-      <c r="AB4" s="72"/>
+      <c r="C4" s="64"/>
+      <c r="D4" s="64"/>
+      <c r="E4" s="64"/>
+      <c r="F4" s="64"/>
+      <c r="G4" s="64"/>
+      <c r="H4" s="64"/>
+      <c r="I4" s="64"/>
+      <c r="J4" s="64"/>
+      <c r="K4" s="64"/>
+      <c r="L4" s="64"/>
+      <c r="M4" s="64"/>
+      <c r="N4" s="64"/>
+      <c r="O4" s="64"/>
+      <c r="P4" s="64"/>
+      <c r="Q4" s="64"/>
+      <c r="R4" s="64"/>
+      <c r="S4" s="64"/>
+      <c r="T4" s="64"/>
+      <c r="U4" s="64"/>
+      <c r="V4" s="64"/>
+      <c r="W4" s="64"/>
+      <c r="X4" s="64"/>
+      <c r="Y4" s="64"/>
+      <c r="Z4" s="64"/>
+      <c r="AA4" s="64"/>
+      <c r="AB4" s="64"/>
     </row>
     <row r="5" spans="2:31" x14ac:dyDescent="0.25">
       <c r="B5" s="31"/>
@@ -2856,60 +2854,60 @@
       <c r="AB5" s="31"/>
     </row>
     <row r="6" spans="2:31" ht="24" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="73" t="s">
+      <c r="B6" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="74"/>
-      <c r="D6" s="75"/>
-      <c r="E6" s="68" t="s">
+      <c r="C6" s="71"/>
+      <c r="D6" s="72"/>
+      <c r="E6" s="66" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="68"/>
-      <c r="G6" s="68"/>
-      <c r="H6" s="79" t="s">
+      <c r="F6" s="66"/>
+      <c r="G6" s="66"/>
+      <c r="H6" s="76" t="s">
         <v>8</v>
       </c>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="87" t="s">
+      <c r="I6" s="76"/>
+      <c r="J6" s="76"/>
+      <c r="K6" s="84" t="s">
         <v>9</v>
       </c>
-      <c r="L6" s="88"/>
-      <c r="M6" s="88"/>
-      <c r="N6" s="89" t="s">
+      <c r="L6" s="85"/>
+      <c r="M6" s="85"/>
+      <c r="N6" s="86" t="s">
         <v>10</v>
       </c>
-      <c r="O6" s="90"/>
-      <c r="P6" s="90"/>
-      <c r="Q6" s="83" t="s">
+      <c r="O6" s="87"/>
+      <c r="P6" s="87"/>
+      <c r="Q6" s="80" t="s">
         <v>11</v>
       </c>
-      <c r="R6" s="84"/>
-      <c r="S6" s="84"/>
-      <c r="T6" s="85" t="s">
+      <c r="R6" s="81"/>
+      <c r="S6" s="81"/>
+      <c r="T6" s="82" t="s">
         <v>12</v>
       </c>
-      <c r="U6" s="86"/>
-      <c r="V6" s="86"/>
-      <c r="W6" s="80" t="s">
+      <c r="U6" s="83"/>
+      <c r="V6" s="83"/>
+      <c r="W6" s="77" t="s">
         <v>13</v>
       </c>
-      <c r="X6" s="81"/>
-      <c r="Y6" s="82"/>
-      <c r="Z6" s="69" t="s">
+      <c r="X6" s="78"/>
+      <c r="Y6" s="79"/>
+      <c r="Z6" s="67" t="s">
         <v>14</v>
       </c>
-      <c r="AA6" s="70"/>
-      <c r="AB6" s="71"/>
+      <c r="AA6" s="68"/>
+      <c r="AB6" s="69"/>
       <c r="AD6" s="50"/>
       <c r="AE6" s="50" t="s">
-        <v>471</v>
+        <v>470</v>
       </c>
     </row>
     <row r="7" spans="2:31" s="3" customFormat="1" ht="39" x14ac:dyDescent="0.25">
-      <c r="B7" s="76"/>
-      <c r="C7" s="77"/>
-      <c r="D7" s="78"/>
+      <c r="B7" s="73"/>
+      <c r="C7" s="74"/>
+      <c r="D7" s="75"/>
       <c r="E7" s="32" t="s">
         <v>5</v>
       </c>
@@ -2988,11 +2986,11 @@
       </c>
     </row>
     <row r="8" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B8" s="92" t="s">
+      <c r="B8" s="59" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="93"/>
-      <c r="D8" s="94"/>
+      <c r="C8" s="60"/>
+      <c r="D8" s="61"/>
       <c r="E8" s="34" t="s">
         <v>30</v>
       </c>
@@ -3071,9 +3069,9 @@
       </c>
     </row>
     <row r="9" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B9" s="92"/>
-      <c r="C9" s="93"/>
-      <c r="D9" s="94"/>
+      <c r="B9" s="59"/>
+      <c r="C9" s="60"/>
+      <c r="D9" s="61"/>
       <c r="E9" s="36"/>
       <c r="F9" s="37"/>
       <c r="G9" s="37"/>
@@ -3102,7 +3100,7 @@
         <v>59</v>
       </c>
       <c r="AE9" s="52" t="s">
-        <v>473</v>
+        <v>472</v>
       </c>
     </row>
     <row r="10" spans="2:31" x14ac:dyDescent="0.25">
@@ -3134,18 +3132,18 @@
       <c r="AA10" s="31"/>
       <c r="AB10" s="31"/>
       <c r="AD10" s="53" t="s">
-        <v>472</v>
+        <v>471</v>
       </c>
       <c r="AE10" s="54" t="s">
-        <v>474</v>
+        <v>473</v>
       </c>
     </row>
     <row r="11" spans="2:31" ht="39" x14ac:dyDescent="0.25">
-      <c r="B11" s="95" t="s">
-        <v>155</v>
-      </c>
-      <c r="C11" s="95"/>
-      <c r="D11" s="95"/>
+      <c r="B11" s="62" t="s">
+        <v>154</v>
+      </c>
+      <c r="C11" s="62"/>
+      <c r="D11" s="62"/>
       <c r="E11" s="32" t="s">
         <v>5</v>
       </c>
@@ -3220,161 +3218,161 @@
       </c>
     </row>
     <row r="12" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B12" s="96" t="s">
+      <c r="B12" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="C12" s="96"/>
-      <c r="D12" s="96"/>
+      <c r="C12" s="63"/>
+      <c r="D12" s="63"/>
       <c r="E12" s="35" t="s">
+        <v>106</v>
+      </c>
+      <c r="F12" s="35" t="s">
         <v>107</v>
       </c>
-      <c r="F12" s="35" t="s">
+      <c r="G12" s="39" t="s">
         <v>108</v>
       </c>
-      <c r="G12" s="39" t="s">
+      <c r="H12" s="35" t="s">
         <v>109</v>
       </c>
-      <c r="H12" s="35" t="s">
+      <c r="I12" s="35" t="s">
         <v>110</v>
       </c>
-      <c r="I12" s="35" t="s">
+      <c r="J12" s="39" t="s">
         <v>111</v>
       </c>
-      <c r="J12" s="39" t="s">
+      <c r="K12" s="35" t="s">
         <v>112</v>
       </c>
-      <c r="K12" s="35" t="s">
+      <c r="L12" s="35" t="s">
         <v>113</v>
       </c>
-      <c r="L12" s="35" t="s">
+      <c r="M12" s="39" t="s">
         <v>114</v>
       </c>
-      <c r="M12" s="39" t="s">
+      <c r="N12" s="35" t="s">
         <v>115</v>
       </c>
-      <c r="N12" s="35" t="s">
+      <c r="O12" s="35" t="s">
         <v>116</v>
       </c>
-      <c r="O12" s="35" t="s">
+      <c r="P12" s="39" t="s">
         <v>117</v>
       </c>
-      <c r="P12" s="39" t="s">
+      <c r="Q12" s="35" t="s">
         <v>118</v>
       </c>
-      <c r="Q12" s="35" t="s">
+      <c r="R12" s="35" t="s">
         <v>119</v>
       </c>
-      <c r="R12" s="35" t="s">
+      <c r="S12" s="39" t="s">
         <v>120</v>
       </c>
-      <c r="S12" s="39" t="s">
+      <c r="T12" s="35" t="s">
         <v>121</v>
       </c>
-      <c r="T12" s="35" t="s">
+      <c r="U12" s="35" t="s">
         <v>122</v>
       </c>
-      <c r="U12" s="35" t="s">
+      <c r="V12" s="39" t="s">
         <v>123</v>
       </c>
-      <c r="V12" s="39" t="s">
+      <c r="W12" s="35" t="s">
         <v>124</v>
       </c>
-      <c r="W12" s="35" t="s">
+      <c r="X12" s="35" t="s">
         <v>125</v>
       </c>
-      <c r="X12" s="35" t="s">
+      <c r="Y12" s="39" t="s">
         <v>126</v>
       </c>
-      <c r="Y12" s="39" t="s">
+      <c r="Z12" s="35" t="s">
         <v>127</v>
       </c>
-      <c r="Z12" s="35" t="s">
+      <c r="AA12" s="35" t="s">
         <v>128</v>
       </c>
-      <c r="AA12" s="35" t="s">
+      <c r="AB12" s="39" t="s">
         <v>129</v>
       </c>
-      <c r="AB12" s="39" t="s">
+    </row>
+    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
+      <c r="B13" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="C13" s="63"/>
+      <c r="D13" s="63"/>
+      <c r="E13" s="35" t="s">
         <v>130</v>
       </c>
-    </row>
-    <row r="13" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B13" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="C13" s="96"/>
-      <c r="D13" s="96"/>
-      <c r="E13" s="35" t="s">
+      <c r="F13" s="35" t="s">
         <v>131</v>
       </c>
-      <c r="F13" s="35" t="s">
+      <c r="G13" s="39" t="s">
         <v>132</v>
       </c>
-      <c r="G13" s="39" t="s">
+      <c r="H13" s="35" t="s">
         <v>133</v>
       </c>
-      <c r="H13" s="35" t="s">
+      <c r="I13" s="35" t="s">
         <v>134</v>
       </c>
-      <c r="I13" s="35" t="s">
+      <c r="J13" s="39" t="s">
         <v>135</v>
       </c>
-      <c r="J13" s="39" t="s">
+      <c r="K13" s="35" t="s">
         <v>136</v>
       </c>
-      <c r="K13" s="35" t="s">
+      <c r="L13" s="35" t="s">
         <v>137</v>
       </c>
-      <c r="L13" s="35" t="s">
+      <c r="M13" s="39" t="s">
         <v>138</v>
       </c>
-      <c r="M13" s="39" t="s">
+      <c r="N13" s="35" t="s">
         <v>139</v>
       </c>
-      <c r="N13" s="35" t="s">
+      <c r="O13" s="35" t="s">
         <v>140</v>
       </c>
-      <c r="O13" s="35" t="s">
+      <c r="P13" s="39" t="s">
         <v>141</v>
       </c>
-      <c r="P13" s="39" t="s">
+      <c r="Q13" s="35" t="s">
         <v>142</v>
       </c>
-      <c r="Q13" s="35" t="s">
+      <c r="R13" s="35" t="s">
         <v>143</v>
       </c>
-      <c r="R13" s="35" t="s">
+      <c r="S13" s="39" t="s">
         <v>144</v>
       </c>
-      <c r="S13" s="39" t="s">
+      <c r="T13" s="35" t="s">
         <v>145</v>
       </c>
-      <c r="T13" s="35" t="s">
+      <c r="U13" s="35" t="s">
         <v>146</v>
       </c>
-      <c r="U13" s="35" t="s">
+      <c r="V13" s="39" t="s">
         <v>147</v>
       </c>
-      <c r="V13" s="39" t="s">
+      <c r="W13" s="35" t="s">
         <v>148</v>
       </c>
-      <c r="W13" s="35" t="s">
+      <c r="X13" s="35" t="s">
         <v>149</v>
       </c>
-      <c r="X13" s="35" t="s">
+      <c r="Y13" s="39" t="s">
         <v>150</v>
       </c>
-      <c r="Y13" s="39" t="s">
+      <c r="Z13" s="35" t="s">
         <v>151</v>
       </c>
-      <c r="Z13" s="35" t="s">
+      <c r="AA13" s="35" t="s">
         <v>152</v>
       </c>
-      <c r="AA13" s="35" t="s">
+      <c r="AB13" s="39" t="s">
         <v>153</v>
-      </c>
-      <c r="AB13" s="39" t="s">
-        <v>154</v>
       </c>
     </row>
     <row r="14" spans="2:31" x14ac:dyDescent="0.25">
@@ -3407,11 +3405,11 @@
       <c r="AB14" s="40"/>
     </row>
     <row r="15" spans="2:31" ht="39" x14ac:dyDescent="0.25">
-      <c r="B15" s="95" t="s">
+      <c r="B15" s="62" t="s">
         <v>16</v>
       </c>
-      <c r="C15" s="95"/>
-      <c r="D15" s="95"/>
+      <c r="C15" s="62"/>
+      <c r="D15" s="62"/>
       <c r="E15" s="32" t="s">
         <v>5</v>
       </c>
@@ -3487,161 +3485,161 @@
       <c r="AE15" s="21"/>
     </row>
     <row r="16" spans="2:31" x14ac:dyDescent="0.25">
-      <c r="B16" s="96" t="s">
+      <c r="B16" s="63" t="s">
         <v>55</v>
       </c>
-      <c r="C16" s="96"/>
-      <c r="D16" s="96"/>
+      <c r="C16" s="63"/>
+      <c r="D16" s="63"/>
       <c r="E16" s="37" t="s">
+        <v>155</v>
+      </c>
+      <c r="F16" s="37" t="s">
         <v>156</v>
       </c>
-      <c r="F16" s="37" t="s">
+      <c r="G16" s="41" t="s">
         <v>157</v>
       </c>
-      <c r="G16" s="41" t="s">
+      <c r="H16" s="37" t="s">
         <v>158</v>
       </c>
-      <c r="H16" s="37" t="s">
+      <c r="I16" s="37" t="s">
         <v>159</v>
       </c>
-      <c r="I16" s="37" t="s">
+      <c r="J16" s="41" t="s">
         <v>160</v>
       </c>
-      <c r="J16" s="41" t="s">
+      <c r="K16" s="37" t="s">
         <v>161</v>
       </c>
-      <c r="K16" s="37" t="s">
+      <c r="L16" s="37" t="s">
         <v>162</v>
       </c>
-      <c r="L16" s="37" t="s">
+      <c r="M16" s="41" t="s">
         <v>163</v>
       </c>
-      <c r="M16" s="41" t="s">
+      <c r="N16" s="37" t="s">
         <v>164</v>
       </c>
-      <c r="N16" s="37" t="s">
+      <c r="O16" s="37" t="s">
         <v>165</v>
       </c>
-      <c r="O16" s="37" t="s">
+      <c r="P16" s="41" t="s">
         <v>166</v>
       </c>
-      <c r="P16" s="41" t="s">
+      <c r="Q16" s="37" t="s">
         <v>167</v>
       </c>
-      <c r="Q16" s="37" t="s">
+      <c r="R16" s="37" t="s">
         <v>168</v>
       </c>
-      <c r="R16" s="37" t="s">
+      <c r="S16" s="41" t="s">
         <v>169</v>
       </c>
-      <c r="S16" s="41" t="s">
+      <c r="T16" s="37" t="s">
         <v>170</v>
       </c>
-      <c r="T16" s="37" t="s">
+      <c r="U16" s="37" t="s">
         <v>171</v>
       </c>
-      <c r="U16" s="37" t="s">
+      <c r="V16" s="41" t="s">
         <v>172</v>
       </c>
-      <c r="V16" s="41" t="s">
+      <c r="W16" s="37" t="s">
         <v>173</v>
       </c>
-      <c r="W16" s="37" t="s">
+      <c r="X16" s="37" t="s">
         <v>174</v>
       </c>
-      <c r="X16" s="37" t="s">
+      <c r="Y16" s="41" t="s">
         <v>175</v>
       </c>
-      <c r="Y16" s="41" t="s">
+      <c r="Z16" s="37" t="s">
         <v>176</v>
       </c>
-      <c r="Z16" s="37" t="s">
+      <c r="AA16" s="37" t="s">
         <v>177</v>
       </c>
-      <c r="AA16" s="37" t="s">
+      <c r="AB16" s="41" t="s">
         <v>178</v>
       </c>
-      <c r="AB16" s="41" t="s">
+    </row>
+    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B17" s="63" t="s">
+        <v>56</v>
+      </c>
+      <c r="C17" s="63"/>
+      <c r="D17" s="63"/>
+      <c r="E17" s="37" t="s">
         <v>179</v>
       </c>
-    </row>
-    <row r="17" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B17" s="96" t="s">
-        <v>56</v>
-      </c>
-      <c r="C17" s="96"/>
-      <c r="D17" s="96"/>
-      <c r="E17" s="37" t="s">
+      <c r="F17" s="37" t="s">
         <v>180</v>
       </c>
-      <c r="F17" s="37" t="s">
+      <c r="G17" s="41" t="s">
         <v>181</v>
       </c>
-      <c r="G17" s="41" t="s">
+      <c r="H17" s="37" t="s">
         <v>182</v>
       </c>
-      <c r="H17" s="37" t="s">
+      <c r="I17" s="37" t="s">
         <v>183</v>
       </c>
-      <c r="I17" s="37" t="s">
+      <c r="J17" s="41" t="s">
         <v>184</v>
       </c>
-      <c r="J17" s="41" t="s">
+      <c r="K17" s="37" t="s">
         <v>185</v>
       </c>
-      <c r="K17" s="37" t="s">
+      <c r="L17" s="37" t="s">
         <v>186</v>
       </c>
-      <c r="L17" s="37" t="s">
+      <c r="M17" s="41" t="s">
         <v>187</v>
       </c>
-      <c r="M17" s="41" t="s">
+      <c r="N17" s="37" t="s">
         <v>188</v>
       </c>
-      <c r="N17" s="37" t="s">
+      <c r="O17" s="37" t="s">
         <v>189</v>
       </c>
-      <c r="O17" s="37" t="s">
+      <c r="P17" s="41" t="s">
         <v>190</v>
       </c>
-      <c r="P17" s="41" t="s">
+      <c r="Q17" s="37" t="s">
         <v>191</v>
       </c>
-      <c r="Q17" s="37" t="s">
+      <c r="R17" s="37" t="s">
         <v>192</v>
       </c>
-      <c r="R17" s="37" t="s">
+      <c r="S17" s="41" t="s">
         <v>193</v>
       </c>
-      <c r="S17" s="41" t="s">
+      <c r="T17" s="37" t="s">
         <v>194</v>
       </c>
-      <c r="T17" s="37" t="s">
+      <c r="U17" s="37" t="s">
         <v>195</v>
       </c>
-      <c r="U17" s="37" t="s">
+      <c r="V17" s="41" t="s">
         <v>196</v>
       </c>
-      <c r="V17" s="41" t="s">
+      <c r="W17" s="37" t="s">
         <v>197</v>
       </c>
-      <c r="W17" s="37" t="s">
+      <c r="X17" s="37" t="s">
         <v>198</v>
       </c>
-      <c r="X17" s="37" t="s">
+      <c r="Y17" s="41" t="s">
         <v>199</v>
       </c>
-      <c r="Y17" s="41" t="s">
+      <c r="Z17" s="37" t="s">
         <v>200</v>
       </c>
-      <c r="Z17" s="37" t="s">
+      <c r="AA17" s="37" t="s">
         <v>201</v>
       </c>
-      <c r="AA17" s="37" t="s">
+      <c r="AB17" s="41" t="s">
         <v>202</v>
-      </c>
-      <c r="AB17" s="41" t="s">
-        <v>203</v>
       </c>
     </row>
     <row r="18" spans="2:28" x14ac:dyDescent="0.25">
@@ -3674,161 +3672,161 @@
       <c r="AB18" s="31"/>
     </row>
     <row r="19" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B19" s="96" t="s">
+      <c r="B19" s="63" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="96"/>
-      <c r="D19" s="96"/>
+      <c r="C19" s="63"/>
+      <c r="D19" s="63"/>
       <c r="E19" s="37" t="s">
+        <v>203</v>
+      </c>
+      <c r="F19" s="37" t="s">
         <v>204</v>
       </c>
-      <c r="F19" s="37" t="s">
+      <c r="G19" s="37" t="s">
         <v>205</v>
       </c>
-      <c r="G19" s="37" t="s">
+      <c r="H19" s="37" t="s">
         <v>206</v>
       </c>
-      <c r="H19" s="37" t="s">
+      <c r="I19" s="37" t="s">
         <v>207</v>
       </c>
-      <c r="I19" s="37" t="s">
+      <c r="J19" s="37" t="s">
         <v>208</v>
       </c>
-      <c r="J19" s="37" t="s">
+      <c r="K19" s="37" t="s">
         <v>209</v>
       </c>
-      <c r="K19" s="37" t="s">
+      <c r="L19" s="37" t="s">
         <v>210</v>
       </c>
-      <c r="L19" s="37" t="s">
+      <c r="M19" s="37" t="s">
         <v>211</v>
       </c>
-      <c r="M19" s="37" t="s">
+      <c r="N19" s="37" t="s">
         <v>212</v>
       </c>
-      <c r="N19" s="37" t="s">
+      <c r="O19" s="37" t="s">
         <v>213</v>
       </c>
-      <c r="O19" s="37" t="s">
+      <c r="P19" s="37" t="s">
         <v>214</v>
       </c>
-      <c r="P19" s="37" t="s">
+      <c r="Q19" s="37" t="s">
         <v>215</v>
       </c>
-      <c r="Q19" s="37" t="s">
+      <c r="R19" s="37" t="s">
         <v>216</v>
       </c>
-      <c r="R19" s="37" t="s">
+      <c r="S19" s="37" t="s">
         <v>217</v>
       </c>
-      <c r="S19" s="37" t="s">
+      <c r="T19" s="37" t="s">
         <v>218</v>
       </c>
-      <c r="T19" s="37" t="s">
+      <c r="U19" s="37" t="s">
         <v>219</v>
       </c>
-      <c r="U19" s="37" t="s">
+      <c r="V19" s="37" t="s">
         <v>220</v>
       </c>
-      <c r="V19" s="37" t="s">
+      <c r="W19" s="37" t="s">
         <v>221</v>
       </c>
-      <c r="W19" s="37" t="s">
+      <c r="X19" s="37" t="s">
         <v>222</v>
       </c>
-      <c r="X19" s="37" t="s">
+      <c r="Y19" s="37" t="s">
         <v>223</v>
       </c>
-      <c r="Y19" s="37" t="s">
+      <c r="Z19" s="37" t="s">
         <v>224</v>
       </c>
-      <c r="Z19" s="37" t="s">
+      <c r="AA19" s="37" t="s">
         <v>225</v>
       </c>
-      <c r="AA19" s="37" t="s">
+      <c r="AB19" s="37" t="s">
         <v>226</v>
       </c>
-      <c r="AB19" s="37" t="s">
+    </row>
+    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
+      <c r="B20" s="63" t="s">
         <v>227</v>
       </c>
-    </row>
-    <row r="20" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B20" s="96" t="s">
+      <c r="C20" s="63"/>
+      <c r="D20" s="63"/>
+      <c r="E20" s="37" t="s">
         <v>228</v>
       </c>
-      <c r="C20" s="96"/>
-      <c r="D20" s="96"/>
-      <c r="E20" s="37" t="s">
+      <c r="F20" s="37" t="s">
         <v>229</v>
       </c>
-      <c r="F20" s="37" t="s">
+      <c r="G20" s="37" t="s">
         <v>230</v>
       </c>
-      <c r="G20" s="37" t="s">
+      <c r="H20" s="37" t="s">
         <v>231</v>
       </c>
-      <c r="H20" s="37" t="s">
+      <c r="I20" s="37" t="s">
         <v>232</v>
       </c>
-      <c r="I20" s="37" t="s">
+      <c r="J20" s="37" t="s">
         <v>233</v>
       </c>
-      <c r="J20" s="37" t="s">
+      <c r="K20" s="37" t="s">
         <v>234</v>
       </c>
-      <c r="K20" s="37" t="s">
+      <c r="L20" s="37" t="s">
         <v>235</v>
       </c>
-      <c r="L20" s="37" t="s">
+      <c r="M20" s="37" t="s">
         <v>236</v>
       </c>
-      <c r="M20" s="37" t="s">
+      <c r="N20" s="37" t="s">
         <v>237</v>
       </c>
-      <c r="N20" s="37" t="s">
+      <c r="O20" s="37" t="s">
         <v>238</v>
       </c>
-      <c r="O20" s="37" t="s">
+      <c r="P20" s="37" t="s">
         <v>239</v>
       </c>
-      <c r="P20" s="37" t="s">
+      <c r="Q20" s="37" t="s">
         <v>240</v>
       </c>
-      <c r="Q20" s="37" t="s">
+      <c r="R20" s="37" t="s">
         <v>241</v>
       </c>
-      <c r="R20" s="37" t="s">
+      <c r="S20" s="37" t="s">
         <v>242</v>
       </c>
-      <c r="S20" s="37" t="s">
+      <c r="T20" s="37" t="s">
         <v>243</v>
       </c>
-      <c r="T20" s="37" t="s">
+      <c r="U20" s="37" t="s">
         <v>244</v>
       </c>
-      <c r="U20" s="37" t="s">
+      <c r="V20" s="37" t="s">
         <v>245</v>
       </c>
-      <c r="V20" s="37" t="s">
+      <c r="W20" s="37" t="s">
         <v>246</v>
       </c>
-      <c r="W20" s="37" t="s">
+      <c r="X20" s="37" t="s">
         <v>247</v>
       </c>
-      <c r="X20" s="37" t="s">
+      <c r="Y20" s="37" t="s">
         <v>248</v>
       </c>
-      <c r="Y20" s="37" t="s">
+      <c r="Z20" s="37" t="s">
         <v>249</v>
       </c>
-      <c r="Z20" s="37" t="s">
+      <c r="AA20" s="37" t="s">
         <v>250</v>
       </c>
-      <c r="AA20" s="37" t="s">
+      <c r="AB20" s="37" t="s">
         <v>251</v>
-      </c>
-      <c r="AB20" s="37" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="21" spans="2:28" x14ac:dyDescent="0.25">
@@ -3861,35 +3859,35 @@
       <c r="AB21" s="31"/>
     </row>
     <row r="22" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B22" s="72" t="s">
+      <c r="B22" s="64" t="s">
         <v>26</v>
       </c>
-      <c r="C22" s="72"/>
-      <c r="D22" s="72"/>
-      <c r="E22" s="72"/>
-      <c r="F22" s="72"/>
-      <c r="G22" s="72"/>
-      <c r="H22" s="72"/>
-      <c r="I22" s="72"/>
-      <c r="J22" s="72"/>
-      <c r="K22" s="72"/>
-      <c r="L22" s="72"/>
-      <c r="M22" s="72"/>
-      <c r="N22" s="72"/>
-      <c r="O22" s="72"/>
-      <c r="P22" s="72"/>
-      <c r="Q22" s="72"/>
-      <c r="R22" s="72"/>
-      <c r="S22" s="72"/>
-      <c r="T22" s="72"/>
-      <c r="U22" s="72"/>
-      <c r="V22" s="72"/>
-      <c r="W22" s="72"/>
-      <c r="X22" s="72"/>
-      <c r="Y22" s="72"/>
-      <c r="Z22" s="72"/>
-      <c r="AA22" s="72"/>
-      <c r="AB22" s="72"/>
+      <c r="C22" s="64"/>
+      <c r="D22" s="64"/>
+      <c r="E22" s="64"/>
+      <c r="F22" s="64"/>
+      <c r="G22" s="64"/>
+      <c r="H22" s="64"/>
+      <c r="I22" s="64"/>
+      <c r="J22" s="64"/>
+      <c r="K22" s="64"/>
+      <c r="L22" s="64"/>
+      <c r="M22" s="64"/>
+      <c r="N22" s="64"/>
+      <c r="O22" s="64"/>
+      <c r="P22" s="64"/>
+      <c r="Q22" s="64"/>
+      <c r="R22" s="64"/>
+      <c r="S22" s="64"/>
+      <c r="T22" s="64"/>
+      <c r="U22" s="64"/>
+      <c r="V22" s="64"/>
+      <c r="W22" s="64"/>
+      <c r="X22" s="64"/>
+      <c r="Y22" s="64"/>
+      <c r="Z22" s="64"/>
+      <c r="AA22" s="64"/>
+      <c r="AB22" s="64"/>
     </row>
     <row r="23" spans="2:28" x14ac:dyDescent="0.25">
       <c r="B23" s="31"/>
@@ -3921,10 +3919,10 @@
       <c r="AB23" s="31"/>
     </row>
     <row r="24" spans="2:28" ht="59.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B24" s="61" t="s">
+      <c r="B24" s="57" t="s">
         <v>17</v>
       </c>
-      <c r="C24" s="61"/>
+      <c r="C24" s="57"/>
       <c r="D24" s="32" t="s">
         <v>18</v>
       </c>
@@ -3992,69 +3990,69 @@
       <c r="AB24" s="31"/>
     </row>
     <row r="25" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B25" s="91" t="s">
+      <c r="B25" s="58" t="s">
         <v>29</v>
       </c>
-      <c r="C25" s="91"/>
+      <c r="C25" s="58"/>
       <c r="D25" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="E25" s="35" t="s">
         <v>87</v>
       </c>
-      <c r="E25" s="35" t="s">
+      <c r="F25" s="35" t="s">
         <v>88</v>
       </c>
-      <c r="F25" s="35" t="s">
+      <c r="G25" s="35" t="s">
         <v>89</v>
       </c>
-      <c r="G25" s="35" t="s">
+      <c r="H25" s="35" t="s">
         <v>90</v>
       </c>
-      <c r="H25" s="35" t="s">
+      <c r="I25" s="35" t="s">
         <v>91</v>
       </c>
-      <c r="I25" s="35" t="s">
+      <c r="J25" s="35" t="s">
         <v>92</v>
       </c>
-      <c r="J25" s="35" t="s">
+      <c r="K25" s="35" t="s">
         <v>93</v>
       </c>
-      <c r="K25" s="35" t="s">
+      <c r="L25" s="35" t="s">
         <v>94</v>
       </c>
-      <c r="L25" s="35" t="s">
+      <c r="M25" s="35" t="s">
         <v>95</v>
       </c>
-      <c r="M25" s="35" t="s">
+      <c r="N25" s="35" t="s">
         <v>96</v>
       </c>
-      <c r="N25" s="35" t="s">
+      <c r="O25" s="35" t="s">
         <v>97</v>
       </c>
-      <c r="O25" s="35" t="s">
+      <c r="P25" s="35" t="s">
         <v>98</v>
       </c>
-      <c r="P25" s="35" t="s">
+      <c r="Q25" s="35" t="s">
         <v>99</v>
       </c>
-      <c r="Q25" s="35" t="s">
+      <c r="R25" s="35" t="s">
         <v>100</v>
       </c>
-      <c r="R25" s="35" t="s">
+      <c r="S25" s="35" t="s">
         <v>101</v>
       </c>
-      <c r="S25" s="35" t="s">
+      <c r="T25" s="35" t="s">
         <v>102</v>
       </c>
-      <c r="T25" s="35" t="s">
+      <c r="U25" s="35" t="s">
         <v>103</v>
       </c>
-      <c r="U25" s="35" t="s">
+      <c r="V25" s="35" t="s">
         <v>104</v>
       </c>
-      <c r="V25" s="35" t="s">
+      <c r="W25" s="35" t="s">
         <v>105</v>
-      </c>
-      <c r="W25" s="35" t="s">
-        <v>106</v>
       </c>
       <c r="X25" s="31"/>
       <c r="Y25" s="31"/>
@@ -4063,8 +4061,8 @@
       <c r="AB25" s="31"/>
     </row>
     <row r="26" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B26" s="91"/>
-      <c r="C26" s="91"/>
+      <c r="B26" s="58"/>
+      <c r="C26" s="58"/>
       <c r="D26" s="37"/>
       <c r="E26" s="37"/>
       <c r="F26" s="37"/>
@@ -4121,8 +4119,8 @@
       <c r="AB27" s="31"/>
     </row>
     <row r="28" spans="2:28" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B28" s="59"/>
-      <c r="C28" s="59"/>
+      <c r="B28" s="90"/>
+      <c r="C28" s="90"/>
       <c r="D28" s="43" t="s">
         <v>18</v>
       </c>
@@ -4186,63 +4184,63 @@
       <c r="AB28" s="31"/>
     </row>
     <row r="29" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B29" s="60" t="s">
+      <c r="B29" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="C29" s="60"/>
+      <c r="C29" s="91"/>
       <c r="D29" s="44" t="s">
+        <v>252</v>
+      </c>
+      <c r="E29" s="45" t="s">
         <v>253</v>
       </c>
-      <c r="E29" s="45" t="s">
+      <c r="F29" s="44" t="s">
         <v>254</v>
       </c>
-      <c r="F29" s="44" t="s">
+      <c r="G29" s="44" t="s">
         <v>255</v>
       </c>
-      <c r="G29" s="44" t="s">
+      <c r="H29" s="45" t="s">
         <v>256</v>
       </c>
-      <c r="H29" s="45" t="s">
+      <c r="I29" s="44" t="s">
         <v>257</v>
       </c>
-      <c r="I29" s="44" t="s">
+      <c r="J29" s="44" t="s">
         <v>258</v>
       </c>
-      <c r="J29" s="44" t="s">
+      <c r="K29" s="45" t="s">
         <v>259</v>
       </c>
-      <c r="K29" s="45" t="s">
+      <c r="L29" s="44" t="s">
         <v>260</v>
       </c>
-      <c r="L29" s="44" t="s">
+      <c r="M29" s="44" t="s">
         <v>261</v>
       </c>
-      <c r="M29" s="44" t="s">
+      <c r="N29" s="45" t="s">
         <v>262</v>
       </c>
-      <c r="N29" s="45" t="s">
+      <c r="O29" s="44" t="s">
         <v>263</v>
       </c>
-      <c r="O29" s="44" t="s">
+      <c r="P29" s="44" t="s">
         <v>264</v>
       </c>
-      <c r="P29" s="44" t="s">
+      <c r="Q29" s="45" t="s">
         <v>265</v>
       </c>
-      <c r="Q29" s="45" t="s">
+      <c r="R29" s="44" t="s">
         <v>266</v>
       </c>
-      <c r="R29" s="44" t="s">
+      <c r="S29" s="44" t="s">
         <v>267</v>
       </c>
-      <c r="S29" s="44" t="s">
+      <c r="T29" s="45" t="s">
         <v>268</v>
       </c>
-      <c r="T29" s="45" t="s">
+      <c r="U29" s="44" t="s">
         <v>269</v>
-      </c>
-      <c r="U29" s="44" t="s">
-        <v>270</v>
       </c>
       <c r="V29" s="31"/>
       <c r="W29" s="31"/>
@@ -4253,63 +4251,63 @@
       <c r="AB29" s="31"/>
     </row>
     <row r="30" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="91" t="s">
         <v>56</v>
       </c>
-      <c r="C30" s="60"/>
+      <c r="C30" s="91"/>
       <c r="D30" s="44" t="s">
+        <v>270</v>
+      </c>
+      <c r="E30" s="45" t="s">
         <v>271</v>
       </c>
-      <c r="E30" s="45" t="s">
+      <c r="F30" s="44" t="s">
         <v>272</v>
       </c>
-      <c r="F30" s="44" t="s">
+      <c r="G30" s="44" t="s">
         <v>273</v>
       </c>
-      <c r="G30" s="44" t="s">
+      <c r="H30" s="45" t="s">
         <v>274</v>
       </c>
-      <c r="H30" s="45" t="s">
+      <c r="I30" s="44" t="s">
         <v>275</v>
       </c>
-      <c r="I30" s="44" t="s">
+      <c r="J30" s="44" t="s">
         <v>276</v>
       </c>
-      <c r="J30" s="44" t="s">
+      <c r="K30" s="45" t="s">
         <v>277</v>
       </c>
-      <c r="K30" s="45" t="s">
+      <c r="L30" s="44" t="s">
         <v>278</v>
       </c>
-      <c r="L30" s="44" t="s">
+      <c r="M30" s="44" t="s">
         <v>279</v>
       </c>
-      <c r="M30" s="44" t="s">
+      <c r="N30" s="45" t="s">
         <v>280</v>
       </c>
-      <c r="N30" s="45" t="s">
+      <c r="O30" s="44" t="s">
         <v>281</v>
       </c>
-      <c r="O30" s="44" t="s">
+      <c r="P30" s="44" t="s">
         <v>282</v>
       </c>
-      <c r="P30" s="44" t="s">
+      <c r="Q30" s="45" t="s">
         <v>283</v>
       </c>
-      <c r="Q30" s="45" t="s">
+      <c r="R30" s="44" t="s">
         <v>284</v>
       </c>
-      <c r="R30" s="44" t="s">
+      <c r="S30" s="44" t="s">
         <v>285</v>
       </c>
-      <c r="S30" s="44" t="s">
+      <c r="T30" s="45" t="s">
         <v>286</v>
       </c>
-      <c r="T30" s="45" t="s">
+      <c r="U30" s="44" t="s">
         <v>287</v>
-      </c>
-      <c r="U30" s="44" t="s">
-        <v>288</v>
       </c>
       <c r="V30" s="31"/>
       <c r="W30" s="31"/>
@@ -4320,63 +4318,63 @@
       <c r="AB30" s="31"/>
     </row>
     <row r="31" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B31" s="62" t="s">
+      <c r="B31" s="92" t="s">
         <v>27</v>
       </c>
-      <c r="C31" s="62"/>
+      <c r="C31" s="92"/>
       <c r="D31" s="46" t="s">
+        <v>288</v>
+      </c>
+      <c r="E31" s="45" t="s">
         <v>289</v>
       </c>
-      <c r="E31" s="45" t="s">
+      <c r="F31" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="F31" s="46" t="s">
+      <c r="G31" s="46" t="s">
         <v>291</v>
       </c>
-      <c r="G31" s="46" t="s">
+      <c r="H31" s="46" t="s">
         <v>292</v>
       </c>
-      <c r="H31" s="46" t="s">
+      <c r="I31" s="46" t="s">
         <v>293</v>
       </c>
-      <c r="I31" s="46" t="s">
+      <c r="J31" s="46" t="s">
         <v>294</v>
       </c>
-      <c r="J31" s="46" t="s">
+      <c r="K31" s="46" t="s">
         <v>295</v>
       </c>
-      <c r="K31" s="46" t="s">
+      <c r="L31" s="46" t="s">
         <v>296</v>
       </c>
-      <c r="L31" s="46" t="s">
+      <c r="M31" s="46" t="s">
         <v>297</v>
       </c>
-      <c r="M31" s="46" t="s">
+      <c r="N31" s="45" t="s">
         <v>298</v>
       </c>
-      <c r="N31" s="45" t="s">
+      <c r="O31" s="46" t="s">
         <v>299</v>
       </c>
-      <c r="O31" s="46" t="s">
+      <c r="P31" s="46" t="s">
         <v>300</v>
       </c>
-      <c r="P31" s="46" t="s">
+      <c r="Q31" s="45" t="s">
         <v>301</v>
       </c>
-      <c r="Q31" s="45" t="s">
+      <c r="R31" s="46" t="s">
         <v>302</v>
       </c>
-      <c r="R31" s="46" t="s">
+      <c r="S31" s="46" t="s">
         <v>303</v>
       </c>
-      <c r="S31" s="46" t="s">
+      <c r="T31" s="45" t="s">
         <v>304</v>
       </c>
-      <c r="T31" s="45" t="s">
+      <c r="U31" s="46" t="s">
         <v>305</v>
-      </c>
-      <c r="U31" s="46" t="s">
-        <v>306</v>
       </c>
       <c r="V31" s="31"/>
       <c r="W31" s="31"/>
@@ -4416,8 +4414,8 @@
       <c r="AB32" s="31"/>
     </row>
     <row r="33" spans="2:28" ht="42.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B33" s="61"/>
-      <c r="C33" s="61"/>
+      <c r="B33" s="57"/>
+      <c r="C33" s="57"/>
       <c r="D33" s="32" t="s">
         <v>18</v>
       </c>
@@ -4469,63 +4467,63 @@
       <c r="AB33" s="31"/>
     </row>
     <row r="34" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B34" s="60" t="s">
+      <c r="B34" s="91" t="s">
         <v>55</v>
       </c>
-      <c r="C34" s="60"/>
+      <c r="C34" s="91"/>
       <c r="D34" s="44" t="s">
+        <v>306</v>
+      </c>
+      <c r="E34" s="45" t="s">
         <v>307</v>
       </c>
-      <c r="E34" s="45" t="s">
+      <c r="F34" s="44" t="s">
         <v>308</v>
       </c>
-      <c r="F34" s="44" t="s">
+      <c r="G34" s="44" t="s">
         <v>309</v>
       </c>
-      <c r="G34" s="44" t="s">
+      <c r="H34" s="45" t="s">
         <v>310</v>
       </c>
-      <c r="H34" s="45" t="s">
+      <c r="I34" s="44" t="s">
         <v>311</v>
       </c>
-      <c r="I34" s="44" t="s">
+      <c r="J34" s="44" t="s">
         <v>312</v>
       </c>
-      <c r="J34" s="44" t="s">
+      <c r="K34" s="45" t="s">
         <v>313</v>
       </c>
-      <c r="K34" s="45" t="s">
+      <c r="L34" s="44" t="s">
         <v>314</v>
       </c>
-      <c r="L34" s="44" t="s">
+      <c r="M34" s="44" t="s">
         <v>315</v>
       </c>
-      <c r="M34" s="44" t="s">
+      <c r="N34" s="45" t="s">
         <v>316</v>
       </c>
-      <c r="N34" s="45" t="s">
+      <c r="O34" s="44" t="s">
         <v>317</v>
       </c>
-      <c r="O34" s="44" t="s">
+      <c r="P34" s="44" t="s">
         <v>318</v>
       </c>
-      <c r="P34" s="44" t="s">
+      <c r="Q34" s="45" t="s">
         <v>319</v>
       </c>
-      <c r="Q34" s="45" t="s">
+      <c r="R34" s="44" t="s">
         <v>320</v>
       </c>
-      <c r="R34" s="44" t="s">
+      <c r="S34" s="44" t="s">
         <v>321</v>
       </c>
-      <c r="S34" s="44" t="s">
+      <c r="T34" s="45" t="s">
         <v>322</v>
       </c>
-      <c r="T34" s="45" t="s">
+      <c r="U34" s="44" t="s">
         <v>323</v>
-      </c>
-      <c r="U34" s="44" t="s">
-        <v>324</v>
       </c>
       <c r="V34" s="31"/>
       <c r="W34" s="31"/>
@@ -4536,63 +4534,63 @@
       <c r="AB34" s="31"/>
     </row>
     <row r="35" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B35" s="63" t="s">
+      <c r="B35" s="93" t="s">
         <v>56</v>
       </c>
-      <c r="C35" s="64"/>
+      <c r="C35" s="94"/>
       <c r="D35" s="44" t="s">
+        <v>324</v>
+      </c>
+      <c r="E35" s="45" t="s">
         <v>325</v>
       </c>
-      <c r="E35" s="45" t="s">
+      <c r="F35" s="44" t="s">
         <v>326</v>
       </c>
-      <c r="F35" s="44" t="s">
+      <c r="G35" s="44" t="s">
         <v>327</v>
       </c>
-      <c r="G35" s="44" t="s">
+      <c r="H35" s="44" t="s">
         <v>328</v>
       </c>
-      <c r="H35" s="44" t="s">
+      <c r="I35" s="44" t="s">
         <v>329</v>
       </c>
-      <c r="I35" s="44" t="s">
+      <c r="J35" s="44" t="s">
         <v>330</v>
       </c>
-      <c r="J35" s="44" t="s">
+      <c r="K35" s="44" t="s">
         <v>331</v>
       </c>
-      <c r="K35" s="44" t="s">
+      <c r="L35" s="44" t="s">
         <v>332</v>
       </c>
-      <c r="L35" s="44" t="s">
+      <c r="M35" s="44" t="s">
         <v>333</v>
       </c>
-      <c r="M35" s="44" t="s">
+      <c r="N35" s="45" t="s">
         <v>334</v>
       </c>
-      <c r="N35" s="45" t="s">
+      <c r="O35" s="44" t="s">
         <v>335</v>
       </c>
-      <c r="O35" s="44" t="s">
+      <c r="P35" s="44" t="s">
         <v>336</v>
       </c>
-      <c r="P35" s="44" t="s">
+      <c r="Q35" s="45" t="s">
         <v>337</v>
       </c>
-      <c r="Q35" s="45" t="s">
+      <c r="R35" s="44" t="s">
         <v>338</v>
       </c>
-      <c r="R35" s="44" t="s">
+      <c r="S35" s="44" t="s">
         <v>339</v>
       </c>
-      <c r="S35" s="44" t="s">
+      <c r="T35" s="45" t="s">
         <v>340</v>
       </c>
-      <c r="T35" s="45" t="s">
+      <c r="U35" s="48" t="s">
         <v>341</v>
-      </c>
-      <c r="U35" s="48" t="s">
-        <v>342</v>
       </c>
       <c r="V35" s="31"/>
       <c r="W35" s="31"/>
@@ -4603,63 +4601,63 @@
       <c r="AB35" s="31"/>
     </row>
     <row r="36" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B36" s="65" t="s">
+      <c r="B36" s="95" t="s">
         <v>27</v>
       </c>
-      <c r="C36" s="66"/>
+      <c r="C36" s="96"/>
       <c r="D36" s="46" t="s">
+        <v>342</v>
+      </c>
+      <c r="E36" s="45" t="s">
         <v>343</v>
       </c>
-      <c r="E36" s="45" t="s">
+      <c r="F36" s="46" t="s">
         <v>344</v>
       </c>
-      <c r="F36" s="46" t="s">
+      <c r="G36" s="46" t="s">
         <v>345</v>
       </c>
-      <c r="G36" s="46" t="s">
+      <c r="H36" s="46" t="s">
         <v>346</v>
       </c>
-      <c r="H36" s="46" t="s">
+      <c r="I36" s="46" t="s">
         <v>347</v>
       </c>
-      <c r="I36" s="46" t="s">
+      <c r="J36" s="46" t="s">
         <v>348</v>
       </c>
-      <c r="J36" s="46" t="s">
+      <c r="K36" s="46" t="s">
         <v>349</v>
       </c>
-      <c r="K36" s="46" t="s">
+      <c r="L36" s="46" t="s">
         <v>350</v>
       </c>
-      <c r="L36" s="46" t="s">
+      <c r="M36" s="46" t="s">
         <v>351</v>
       </c>
-      <c r="M36" s="46" t="s">
+      <c r="N36" s="45" t="s">
         <v>352</v>
       </c>
-      <c r="N36" s="45" t="s">
+      <c r="O36" s="46" t="s">
         <v>353</v>
       </c>
-      <c r="O36" s="46" t="s">
+      <c r="P36" s="46" t="s">
         <v>354</v>
       </c>
-      <c r="P36" s="46" t="s">
+      <c r="Q36" s="45" t="s">
         <v>355</v>
       </c>
-      <c r="Q36" s="45" t="s">
+      <c r="R36" s="46" t="s">
         <v>356</v>
       </c>
-      <c r="R36" s="46" t="s">
+      <c r="S36" s="46" t="s">
         <v>357</v>
       </c>
-      <c r="S36" s="46" t="s">
+      <c r="T36" s="45" t="s">
         <v>358</v>
       </c>
-      <c r="T36" s="45" t="s">
+      <c r="U36" s="46" t="s">
         <v>359</v>
-      </c>
-      <c r="U36" s="46" t="s">
-        <v>360</v>
       </c>
       <c r="V36" s="31"/>
       <c r="W36" s="31"/>
@@ -4699,63 +4697,63 @@
       <c r="AB37" s="31"/>
     </row>
     <row r="38" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B38" s="57" t="s">
+      <c r="B38" s="88" t="s">
         <v>28</v>
       </c>
-      <c r="C38" s="58"/>
+      <c r="C38" s="89"/>
       <c r="D38" s="49" t="s">
+        <v>360</v>
+      </c>
+      <c r="E38" s="49" t="s">
         <v>361</v>
       </c>
-      <c r="E38" s="49" t="s">
+      <c r="F38" s="49" t="s">
         <v>362</v>
       </c>
-      <c r="F38" s="49" t="s">
+      <c r="G38" s="49" t="s">
         <v>363</v>
       </c>
-      <c r="G38" s="49" t="s">
+      <c r="H38" s="49" t="s">
         <v>364</v>
       </c>
-      <c r="H38" s="49" t="s">
+      <c r="I38" s="49" t="s">
         <v>365</v>
       </c>
-      <c r="I38" s="49" t="s">
+      <c r="J38" s="49" t="s">
         <v>366</v>
       </c>
-      <c r="J38" s="49" t="s">
+      <c r="K38" s="49" t="s">
         <v>367</v>
       </c>
-      <c r="K38" s="49" t="s">
+      <c r="L38" s="49" t="s">
         <v>368</v>
       </c>
-      <c r="L38" s="49" t="s">
+      <c r="M38" s="49" t="s">
         <v>369</v>
       </c>
-      <c r="M38" s="49" t="s">
+      <c r="N38" s="49" t="s">
         <v>370</v>
       </c>
-      <c r="N38" s="49" t="s">
+      <c r="O38" s="49" t="s">
         <v>371</v>
       </c>
-      <c r="O38" s="49" t="s">
+      <c r="P38" s="49" t="s">
         <v>372</v>
       </c>
-      <c r="P38" s="49" t="s">
+      <c r="Q38" s="49" t="s">
         <v>373</v>
       </c>
-      <c r="Q38" s="49" t="s">
+      <c r="R38" s="49" t="s">
         <v>374</v>
       </c>
-      <c r="R38" s="49" t="s">
+      <c r="S38" s="49" t="s">
         <v>375</v>
       </c>
-      <c r="S38" s="49" t="s">
+      <c r="T38" s="49" t="s">
         <v>376</v>
       </c>
-      <c r="T38" s="49" t="s">
+      <c r="U38" s="49" t="s">
         <v>377</v>
-      </c>
-      <c r="U38" s="49" t="s">
-        <v>378</v>
       </c>
       <c r="V38" s="31"/>
       <c r="W38" s="31"/>
@@ -4766,63 +4764,63 @@
       <c r="AB38" s="31"/>
     </row>
     <row r="39" spans="2:28" x14ac:dyDescent="0.25">
-      <c r="B39" s="57" t="s">
-        <v>228</v>
-      </c>
-      <c r="C39" s="58"/>
+      <c r="B39" s="88" t="s">
+        <v>227</v>
+      </c>
+      <c r="C39" s="89"/>
       <c r="D39" s="49" t="s">
+        <v>378</v>
+      </c>
+      <c r="E39" s="49" t="s">
         <v>379</v>
       </c>
-      <c r="E39" s="49" t="s">
+      <c r="F39" s="49" t="s">
         <v>380</v>
       </c>
-      <c r="F39" s="49" t="s">
+      <c r="G39" s="49" t="s">
         <v>381</v>
       </c>
-      <c r="G39" s="49" t="s">
+      <c r="H39" s="49" t="s">
         <v>382</v>
       </c>
-      <c r="H39" s="49" t="s">
+      <c r="I39" s="49" t="s">
         <v>383</v>
       </c>
-      <c r="I39" s="49" t="s">
+      <c r="J39" s="49" t="s">
         <v>384</v>
       </c>
-      <c r="J39" s="49" t="s">
+      <c r="K39" s="49" t="s">
         <v>385</v>
       </c>
-      <c r="K39" s="49" t="s">
+      <c r="L39" s="49" t="s">
         <v>386</v>
       </c>
-      <c r="L39" s="49" t="s">
+      <c r="M39" s="49" t="s">
         <v>387</v>
       </c>
-      <c r="M39" s="49" t="s">
+      <c r="N39" s="49" t="s">
         <v>388</v>
       </c>
-      <c r="N39" s="49" t="s">
+      <c r="O39" s="49" t="s">
         <v>389</v>
       </c>
-      <c r="O39" s="49" t="s">
+      <c r="P39" s="49" t="s">
         <v>390</v>
       </c>
-      <c r="P39" s="49" t="s">
+      <c r="Q39" s="49" t="s">
         <v>391</v>
       </c>
-      <c r="Q39" s="49" t="s">
+      <c r="R39" s="49" t="s">
         <v>392</v>
       </c>
-      <c r="R39" s="49" t="s">
+      <c r="S39" s="49" t="s">
         <v>393</v>
       </c>
-      <c r="S39" s="49" t="s">
+      <c r="T39" s="49" t="s">
         <v>394</v>
       </c>
-      <c r="T39" s="49" t="s">
+      <c r="U39" s="49" t="s">
         <v>395</v>
-      </c>
-      <c r="U39" s="49" t="s">
-        <v>396</v>
       </c>
       <c r="V39" s="31"/>
       <c r="W39" s="31"/>
@@ -4837,6 +4835,27 @@
     </row>
   </sheetData>
   <mergeCells count="35">
+    <mergeCell ref="B39:C39"/>
+    <mergeCell ref="B28:C28"/>
+    <mergeCell ref="B29:C29"/>
+    <mergeCell ref="B38:C38"/>
+    <mergeCell ref="B33:C33"/>
+    <mergeCell ref="B30:C30"/>
+    <mergeCell ref="B31:C31"/>
+    <mergeCell ref="B34:C34"/>
+    <mergeCell ref="B35:C35"/>
+    <mergeCell ref="B36:C36"/>
+    <mergeCell ref="B2:E2"/>
+    <mergeCell ref="E6:G6"/>
+    <mergeCell ref="Z6:AB6"/>
+    <mergeCell ref="B4:AB4"/>
+    <mergeCell ref="B6:D7"/>
+    <mergeCell ref="H6:J6"/>
+    <mergeCell ref="W6:Y6"/>
+    <mergeCell ref="Q6:S6"/>
+    <mergeCell ref="T6:V6"/>
+    <mergeCell ref="K6:M6"/>
+    <mergeCell ref="N6:P6"/>
     <mergeCell ref="B24:C24"/>
     <mergeCell ref="B25:C25"/>
     <mergeCell ref="B26:C26"/>
@@ -4851,27 +4870,6 @@
     <mergeCell ref="B22:AB22"/>
     <mergeCell ref="B19:D19"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B2:E2"/>
-    <mergeCell ref="E6:G6"/>
-    <mergeCell ref="Z6:AB6"/>
-    <mergeCell ref="B4:AB4"/>
-    <mergeCell ref="B6:D7"/>
-    <mergeCell ref="H6:J6"/>
-    <mergeCell ref="W6:Y6"/>
-    <mergeCell ref="Q6:S6"/>
-    <mergeCell ref="T6:V6"/>
-    <mergeCell ref="K6:M6"/>
-    <mergeCell ref="N6:P6"/>
-    <mergeCell ref="B39:C39"/>
-    <mergeCell ref="B28:C28"/>
-    <mergeCell ref="B29:C29"/>
-    <mergeCell ref="B38:C38"/>
-    <mergeCell ref="B33:C33"/>
-    <mergeCell ref="B30:C30"/>
-    <mergeCell ref="B31:C31"/>
-    <mergeCell ref="B34:C34"/>
-    <mergeCell ref="B35:C35"/>
-    <mergeCell ref="B36:C36"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -4886,7 +4884,7 @@
   <dimension ref="B2:L31"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:C2"/>
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4918,7 +4916,7 @@
     </row>
     <row r="4" spans="2:12" ht="15.75" x14ac:dyDescent="0.25">
       <c r="B4" s="106" t="s">
-        <v>76</v>
+        <v>474</v>
       </c>
       <c r="C4" s="106"/>
       <c r="D4" s="106"/>
@@ -4990,34 +4988,34 @@
         <v>29</v>
       </c>
       <c r="C8" s="25" t="s">
+        <v>76</v>
+      </c>
+      <c r="D8" s="24" t="s">
         <v>77</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="E8" s="24" t="s">
         <v>78</v>
       </c>
-      <c r="E8" s="24" t="s">
+      <c r="F8" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="F8" s="24" t="s">
+      <c r="G8" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="G8" s="24" t="s">
+      <c r="H8" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="H8" s="24" t="s">
+      <c r="I8" s="24" t="s">
         <v>82</v>
       </c>
-      <c r="I8" s="24" t="s">
+      <c r="J8" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="J8" s="24" t="s">
+      <c r="K8" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="K8" s="24" t="s">
+      <c r="L8" s="24" t="s">
         <v>85</v>
-      </c>
-      <c r="L8" s="24" t="s">
-        <v>86</v>
       </c>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.25">
@@ -5073,34 +5071,34 @@
         <v>55</v>
       </c>
       <c r="C12" s="24" t="s">
+        <v>396</v>
+      </c>
+      <c r="D12" s="24" t="s">
         <v>397</v>
       </c>
-      <c r="D12" s="24" t="s">
+      <c r="E12" s="24" t="s">
         <v>398</v>
       </c>
-      <c r="E12" s="24" t="s">
+      <c r="F12" s="24" t="s">
         <v>399</v>
       </c>
-      <c r="F12" s="24" t="s">
+      <c r="G12" s="24" t="s">
         <v>400</v>
       </c>
-      <c r="G12" s="24" t="s">
+      <c r="H12" s="24" t="s">
         <v>401</v>
       </c>
-      <c r="H12" s="24" t="s">
+      <c r="I12" s="24" t="s">
         <v>402</v>
       </c>
-      <c r="I12" s="24" t="s">
+      <c r="J12" s="24" t="s">
         <v>403</v>
       </c>
-      <c r="J12" s="24" t="s">
+      <c r="K12" s="24" t="s">
         <v>404</v>
       </c>
-      <c r="K12" s="24" t="s">
+      <c r="L12" s="24" t="s">
         <v>405</v>
-      </c>
-      <c r="L12" s="24" t="s">
-        <v>406</v>
       </c>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.25">
@@ -5108,34 +5106,34 @@
         <v>56</v>
       </c>
       <c r="C13" s="24" t="s">
+        <v>406</v>
+      </c>
+      <c r="D13" s="24" t="s">
         <v>407</v>
       </c>
-      <c r="D13" s="24" t="s">
+      <c r="E13" s="24" t="s">
         <v>408</v>
       </c>
-      <c r="E13" s="24" t="s">
+      <c r="F13" s="24" t="s">
         <v>409</v>
       </c>
-      <c r="F13" s="24" t="s">
+      <c r="G13" s="24" t="s">
         <v>410</v>
       </c>
-      <c r="G13" s="24" t="s">
+      <c r="H13" s="24" t="s">
         <v>411</v>
       </c>
-      <c r="H13" s="24" t="s">
+      <c r="I13" s="24" t="s">
         <v>412</v>
       </c>
-      <c r="I13" s="24" t="s">
+      <c r="J13" s="24" t="s">
         <v>413</v>
       </c>
-      <c r="J13" s="24" t="s">
+      <c r="K13" s="24" t="s">
         <v>414</v>
       </c>
-      <c r="K13" s="24" t="s">
+      <c r="L13" s="24" t="s">
         <v>415</v>
-      </c>
-      <c r="L13" s="24" t="s">
-        <v>416</v>
       </c>
     </row>
     <row r="15" spans="2:12" ht="45" x14ac:dyDescent="0.25">
@@ -5178,34 +5176,34 @@
         <v>55</v>
       </c>
       <c r="C16" s="24" t="s">
+        <v>416</v>
+      </c>
+      <c r="D16" s="24" t="s">
         <v>417</v>
       </c>
-      <c r="D16" s="24" t="s">
+      <c r="E16" s="24" t="s">
         <v>418</v>
       </c>
-      <c r="E16" s="24" t="s">
+      <c r="F16" s="24" t="s">
         <v>419</v>
       </c>
-      <c r="F16" s="24" t="s">
+      <c r="G16" s="24" t="s">
         <v>420</v>
       </c>
-      <c r="G16" s="24" t="s">
+      <c r="H16" s="24" t="s">
         <v>421</v>
       </c>
-      <c r="H16" s="24" t="s">
+      <c r="I16" s="24" t="s">
         <v>422</v>
       </c>
-      <c r="I16" s="24" t="s">
+      <c r="J16" s="24" t="s">
         <v>423</v>
       </c>
-      <c r="J16" s="24" t="s">
+      <c r="K16" s="24" t="s">
         <v>424</v>
       </c>
-      <c r="K16" s="24" t="s">
+      <c r="L16" s="24" t="s">
         <v>425</v>
-      </c>
-      <c r="L16" s="24" t="s">
-        <v>426</v>
       </c>
     </row>
     <row r="17" spans="2:12" x14ac:dyDescent="0.25">
@@ -5213,34 +5211,34 @@
         <v>56</v>
       </c>
       <c r="C17" s="24" t="s">
+        <v>426</v>
+      </c>
+      <c r="D17" s="24" t="s">
         <v>427</v>
       </c>
-      <c r="D17" s="24" t="s">
+      <c r="E17" s="24" t="s">
         <v>428</v>
       </c>
-      <c r="E17" s="24" t="s">
+      <c r="F17" s="24" t="s">
         <v>429</v>
       </c>
-      <c r="F17" s="24" t="s">
+      <c r="G17" s="24" t="s">
         <v>430</v>
       </c>
-      <c r="G17" s="24" t="s">
+      <c r="H17" s="24" t="s">
         <v>431</v>
       </c>
-      <c r="H17" s="24" t="s">
+      <c r="I17" s="24" t="s">
         <v>432</v>
       </c>
-      <c r="I17" s="24" t="s">
+      <c r="J17" s="24" t="s">
         <v>433</v>
       </c>
-      <c r="J17" s="24" t="s">
+      <c r="K17" s="24" t="s">
         <v>434</v>
       </c>
-      <c r="K17" s="24" t="s">
+      <c r="L17" s="24" t="s">
         <v>435</v>
-      </c>
-      <c r="L17" s="24" t="s">
-        <v>436</v>
       </c>
     </row>
     <row r="19" spans="2:12" x14ac:dyDescent="0.25">
@@ -5248,69 +5246,69 @@
         <v>28</v>
       </c>
       <c r="C19" s="24" t="s">
+        <v>436</v>
+      </c>
+      <c r="D19" s="24" t="s">
         <v>437</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="E19" s="24" t="s">
         <v>438</v>
       </c>
-      <c r="E19" s="24" t="s">
+      <c r="F19" s="24" t="s">
         <v>439</v>
       </c>
-      <c r="F19" s="24" t="s">
+      <c r="G19" s="24" t="s">
         <v>440</v>
       </c>
-      <c r="G19" s="24" t="s">
+      <c r="H19" s="24" t="s">
         <v>441</v>
       </c>
-      <c r="H19" s="24" t="s">
+      <c r="I19" s="24" t="s">
         <v>442</v>
       </c>
-      <c r="I19" s="24" t="s">
+      <c r="J19" s="24" t="s">
         <v>443</v>
       </c>
-      <c r="J19" s="24" t="s">
+      <c r="K19" s="24" t="s">
         <v>444</v>
       </c>
-      <c r="K19" s="24" t="s">
+      <c r="L19" s="24" t="s">
         <v>445</v>
-      </c>
-      <c r="L19" s="24" t="s">
-        <v>446</v>
       </c>
     </row>
     <row r="20" spans="2:12" x14ac:dyDescent="0.25">
       <c r="B20" s="1" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C20" s="24" t="s">
+        <v>446</v>
+      </c>
+      <c r="D20" s="24" t="s">
         <v>447</v>
       </c>
-      <c r="D20" s="24" t="s">
+      <c r="E20" s="24" t="s">
         <v>448</v>
       </c>
-      <c r="E20" s="24" t="s">
+      <c r="F20" s="24" t="s">
         <v>449</v>
       </c>
-      <c r="F20" s="24" t="s">
+      <c r="G20" s="24" t="s">
         <v>450</v>
       </c>
-      <c r="G20" s="24" t="s">
+      <c r="H20" s="24" t="s">
         <v>451</v>
       </c>
-      <c r="H20" s="24" t="s">
+      <c r="I20" s="24" t="s">
         <v>452</v>
       </c>
-      <c r="I20" s="24" t="s">
+      <c r="J20" s="24" t="s">
         <v>453</v>
       </c>
-      <c r="J20" s="24" t="s">
+      <c r="K20" s="24" t="s">
         <v>454</v>
       </c>
-      <c r="K20" s="24" t="s">
+      <c r="L20" s="24" t="s">
         <v>455</v>
-      </c>
-      <c r="L20" s="24" t="s">
-        <v>456</v>
       </c>
     </row>
     <row r="22" spans="2:12" x14ac:dyDescent="0.25">
@@ -5333,7 +5331,7 @@
       </c>
       <c r="G23" s="20"/>
       <c r="H23" s="26" t="s">
-        <v>457</v>
+        <v>456</v>
       </c>
       <c r="I23" s="8"/>
       <c r="J23" s="17" t="s">
@@ -5341,7 +5339,7 @@
       </c>
       <c r="K23" s="16"/>
       <c r="L23" s="26" t="s">
-        <v>462</v>
+        <v>461</v>
       </c>
     </row>
     <row r="24" spans="2:12" x14ac:dyDescent="0.25">
@@ -5350,7 +5348,7 @@
       </c>
       <c r="G24" s="20"/>
       <c r="H24" s="26" t="s">
-        <v>458</v>
+        <v>457</v>
       </c>
       <c r="I24" s="8"/>
       <c r="J24" s="17" t="s">
@@ -5358,7 +5356,7 @@
       </c>
       <c r="K24" s="16"/>
       <c r="L24" s="26" t="s">
-        <v>463</v>
+        <v>462</v>
       </c>
     </row>
     <row r="25" spans="2:12" x14ac:dyDescent="0.25">
@@ -5367,7 +5365,7 @@
       </c>
       <c r="G25" s="20"/>
       <c r="H25" s="26" t="s">
-        <v>459</v>
+        <v>458</v>
       </c>
       <c r="I25" s="8"/>
       <c r="J25" s="17" t="s">
@@ -5375,7 +5373,7 @@
       </c>
       <c r="K25" s="16"/>
       <c r="L25" s="26" t="s">
-        <v>464</v>
+        <v>463</v>
       </c>
     </row>
     <row r="26" spans="2:12" x14ac:dyDescent="0.25">
@@ -5384,7 +5382,7 @@
       </c>
       <c r="G26" s="18"/>
       <c r="H26" s="26" t="s">
-        <v>460</v>
+        <v>459</v>
       </c>
       <c r="I26" s="8"/>
       <c r="J26" s="17" t="s">
@@ -5392,7 +5390,7 @@
       </c>
       <c r="K26" s="16"/>
       <c r="L26" s="26" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
     </row>
     <row r="27" spans="2:12" x14ac:dyDescent="0.25">
@@ -5401,7 +5399,7 @@
       </c>
       <c r="G27" s="101"/>
       <c r="H27" s="26" t="s">
-        <v>461</v>
+        <v>460</v>
       </c>
       <c r="I27" s="8"/>
       <c r="J27" s="100" t="s">
@@ -5409,7 +5407,7 @@
       </c>
       <c r="K27" s="104"/>
       <c r="L27" s="26" t="s">
-        <v>466</v>
+        <v>465</v>
       </c>
     </row>
     <row r="28" spans="2:12" x14ac:dyDescent="0.25">
@@ -5468,20 +5466,20 @@
         <v>59</v>
       </c>
       <c r="G31" s="27" t="s">
+        <v>466</v>
+      </c>
+      <c r="H31" s="27" t="s">
         <v>467</v>
-      </c>
-      <c r="H31" s="27" t="s">
-        <v>468</v>
       </c>
       <c r="I31" s="8"/>
       <c r="J31" s="7" t="s">
         <v>58</v>
       </c>
       <c r="K31" s="27" t="s">
+        <v>468</v>
+      </c>
+      <c r="L31" s="27" t="s">
         <v>469</v>
-      </c>
-      <c r="L31" s="27" t="s">
-        <v>470</v>
       </c>
     </row>
   </sheetData>

</xml_diff>